<commit_message>
start refacroting: fonts, button
</commit_message>
<xml_diff>
--- a/feed_tab.xlsx
+++ b/feed_tab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13550" windowHeight="7890" tabRatio="286" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13550" windowHeight="7890" tabRatio="286"/>
   </bookViews>
   <sheets>
     <sheet name="feed" sheetId="1" r:id="rId1"/>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y161"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -960,6 +960,10 @@
       <c r="A3" s="1"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
+      <c r="K3">
+        <f>$A$6*2/($B$6/$C$6*A9)</f>
+        <v>4.5</v>
+      </c>
       <c r="P3" s="6" t="s">
         <v>5</v>
       </c>
@@ -982,6 +986,14 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="6"/>
+      <c r="J4">
+        <f>A6*2*C6/A9/B6*B1</f>
+        <v>75497472</v>
+      </c>
+      <c r="K4">
+        <f>ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0)</f>
+        <v>75497472</v>
+      </c>
       <c r="P4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1041,6 +1053,10 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="6"/>
+      <c r="J6" s="13" t="str">
+        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0),9)),"0x000000000")</f>
+        <v>0x004800000</v>
+      </c>
       <c r="P6" s="6" t="s">
         <v>11</v>
       </c>
@@ -1117,10 +1133,6 @@
       <c r="A9" s="14">
         <v>2</v>
       </c>
-      <c r="B9" s="13" t="str">
-        <f t="shared" ref="B9" si="0">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0),9)),"0x000000000")</f>
-        <v>0x004800000</v>
-      </c>
       <c r="C9" s="14">
         <v>0</v>
       </c>
@@ -1140,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="12" t="str">
-        <f>$A$2&amp;B9&amp;$C$2&amp;C9&amp;$D$2&amp;SUBSTITUTE(TEXT(A9,"0,00"),",",".")&amp;$G$2&amp;D9&amp;$E$2&amp;E9&amp;$D$2&amp;F9&amp;$G$2&amp;G9&amp;$E$2&amp;H9&amp;$B$2</f>
+        <f>$A$2&amp;J6&amp;$C$2&amp;C9&amp;$D$2&amp;SUBSTITUTE(TEXT(A9,"0,00"),",",".")&amp;$G$2&amp;D9&amp;$E$2&amp;E9&amp;$D$2&amp;F9&amp;$G$2&amp;G9&amp;$E$2&amp;H9&amp;$B$2</f>
         <v>{ 0x004800000, 0, "2.00", "mm", 0, "1.26", ".050", 0 },</v>
       </c>
       <c r="J9" s="4"/>
@@ -1163,7 +1175,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="13" t="str">
-        <f t="shared" ref="B10:B11" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A10)*$B$1,0),9)),"0x000000000")</f>
+        <f t="shared" ref="B10:B11" si="0">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A10)*$B$1,0),9)),"0x000000000")</f>
         <v>0x004800000</v>
       </c>
       <c r="C10" s="14">
@@ -1196,7 +1208,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0x004800000</v>
       </c>
       <c r="C11" s="14">
@@ -1229,7 +1241,7 @@
         <v>1.5</v>
       </c>
       <c r="B12" s="13" t="str">
-        <f t="shared" ref="B12:B41" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A12)*$B$1,0),9)),"0x000000000")</f>
+        <f t="shared" ref="B12:B41" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A12)*$B$1,0),9)),"0x000000000")</f>
         <v>0x006000000</v>
       </c>
       <c r="C12" s="14">
@@ -1251,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="12" t="str">
-        <f t="shared" ref="I12:I41" si="3">$A$2&amp;B12&amp;$C$2&amp;C12&amp;$D$2&amp;SUBSTITUTE(TEXT(A12,"0,00"),",",".")&amp;$G$2&amp;D12&amp;$E$2&amp;E12&amp;$D$2&amp;F12&amp;$G$2&amp;G12&amp;$E$2&amp;H12&amp;$B$2</f>
+        <f t="shared" ref="I12:I41" si="2">$A$2&amp;B12&amp;$C$2&amp;C12&amp;$D$2&amp;SUBSTITUTE(TEXT(A12,"0,00"),",",".")&amp;$G$2&amp;D12&amp;$E$2&amp;E12&amp;$D$2&amp;F12&amp;$G$2&amp;G12&amp;$E$2&amp;H12&amp;$B$2</f>
         <v>{ 0x006000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
       </c>
       <c r="P12" s="6" t="s">
@@ -1266,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x009000000</v>
       </c>
       <c r="C13" s="14">
@@ -1304,7 +1316,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000000000</v>
       </c>
       <c r="C14" s="14">
@@ -1322,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000000000, 20, "F", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J14" s="4"/>
@@ -1333,7 +1345,7 @@
         <v>0.2</v>
       </c>
       <c r="B15" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x02D000000</v>
       </c>
       <c r="C15" s="14">
@@ -1351,7 +1363,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x02D000000, 0, "0.20", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J15" s="4"/>
@@ -1362,7 +1374,7 @@
         <v>0.18</v>
       </c>
       <c r="B16" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x032000000</v>
       </c>
       <c r="C16" s="14">
@@ -1380,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x032000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J16" s="4"/>
@@ -1391,7 +1403,7 @@
         <v>0.15</v>
       </c>
       <c r="B17" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x03C000000</v>
       </c>
       <c r="C17" s="14">
@@ -1409,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x03C000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J17" s="4"/>
@@ -1420,7 +1432,7 @@
         <v>0.12</v>
       </c>
       <c r="B18" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x04B000000</v>
       </c>
       <c r="C18" s="14">
@@ -1438,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x04B000000, 0, "0.12", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J18" s="4"/>
@@ -1449,7 +1461,7 @@
         <v>0.09</v>
       </c>
       <c r="B19" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x064000000</v>
       </c>
       <c r="C19" s="14">
@@ -1467,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x064000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J19" s="4"/>
@@ -1478,7 +1490,7 @@
         <v>0.06</v>
       </c>
       <c r="B20" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x096000000</v>
       </c>
       <c r="C20" s="14">
@@ -1496,7 +1508,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x096000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J20" s="4"/>
@@ -1507,7 +1519,7 @@
         <v>0.04</v>
       </c>
       <c r="B21" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x0E1000000</v>
       </c>
       <c r="C21" s="14">
@@ -1525,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x0E1000000, 0, "0.04", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J21" s="4"/>
@@ -1536,7 +1548,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000000000</v>
       </c>
       <c r="C22" s="14">
@@ -1554,7 +1566,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000000000, 0, "..", "up", 20, "", "", 0 },</v>
       </c>
       <c r="J22" s="4"/>
@@ -1565,7 +1577,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000000000</v>
       </c>
       <c r="C23" s="14">
@@ -1583,7 +1595,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000000000, 10, "T", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J23" s="4"/>
@@ -1594,7 +1606,7 @@
         <v>1.25</v>
       </c>
       <c r="B24" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x007333333</v>
       </c>
       <c r="C24" s="14">
@@ -1616,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x007333333, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
       </c>
       <c r="J24" s="4"/>
@@ -1627,7 +1639,7 @@
         <v>1.75</v>
       </c>
       <c r="B25" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x005249249</v>
       </c>
       <c r="C25" s="14">
@@ -1649,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x005249249, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
       </c>
       <c r="J25" s="4"/>
@@ -1660,7 +1672,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x004800000</v>
       </c>
       <c r="C26" s="14">
@@ -1682,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x004800000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
       </c>
       <c r="J26" s="4"/>
@@ -1693,7 +1705,7 @@
         <v>0.5</v>
       </c>
       <c r="B27" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x012000000</v>
       </c>
       <c r="C27" s="14">
@@ -1715,7 +1727,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x012000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
       </c>
       <c r="J27" s="4"/>
@@ -1726,7 +1738,7 @@
         <v>0.75</v>
       </c>
       <c r="B28" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x00C000000</v>
       </c>
       <c r="C28" s="14">
@@ -1748,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x00C000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
       </c>
       <c r="J28" s="4"/>
@@ -1759,7 +1771,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000000000</v>
       </c>
       <c r="C29" s="14">
@@ -1777,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000000000, 0, "..", "up", 10, "", "", 0 },</v>
       </c>
       <c r="J29" s="4"/>
@@ -1788,7 +1800,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000000000</v>
       </c>
       <c r="C30" s="14">
@@ -1806,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000000000, 30, "T", "tpi", 0, "", "", 0 },</v>
       </c>
       <c r="J30" s="4"/>
@@ -1817,7 +1829,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000555555</v>
       </c>
       <c r="C31" s="14">
@@ -1835,7 +1847,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000555555, 0, "27.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J31" s="4"/>
@@ -1846,7 +1858,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000589D89</v>
       </c>
       <c r="C32" s="14">
@@ -1864,7 +1876,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000589D89, 0, "26.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J32" s="4"/>
@@ -1875,7 +1887,7 @@
         <v>24</v>
       </c>
       <c r="B33" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000600000</v>
       </c>
       <c r="C33" s="14">
@@ -1893,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000600000, 0, "24.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J33" s="4"/>
@@ -1904,7 +1916,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x00068BA2E</v>
       </c>
       <c r="C34" s="14">
@@ -1922,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x00068BA2E, 0, "22.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J34" s="4"/>
@@ -1933,7 +1945,7 @@
         <v>20</v>
       </c>
       <c r="B35" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000733333</v>
       </c>
       <c r="C35" s="14">
@@ -1951,7 +1963,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000733333, 0, "20.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J35" s="4"/>
@@ -1962,7 +1974,7 @@
         <v>19</v>
       </c>
       <c r="B36" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x00079435E</v>
       </c>
       <c r="C36" s="14">
@@ -1980,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x00079435E, 0, "19.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J36" s="4"/>
@@ -1991,7 +2003,7 @@
         <v>18</v>
       </c>
       <c r="B37" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000800000</v>
       </c>
       <c r="C37" s="14">
@@ -2009,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000800000, 0, "18.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J37" s="4"/>
@@ -2020,7 +2032,7 @@
         <v>16</v>
       </c>
       <c r="B38" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000900000</v>
       </c>
       <c r="C38" s="14">
@@ -2038,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000900000, 0, "16.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J38" s="4"/>
@@ -2049,7 +2061,7 @@
         <v>14</v>
       </c>
       <c r="B39" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000A49249</v>
       </c>
       <c r="C39" s="14">
@@ -2067,7 +2079,7 @@
         <v>0</v>
       </c>
       <c r="I39" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000A49249, 0, "14.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J39" s="4"/>
@@ -2078,7 +2090,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000C00000</v>
       </c>
       <c r="C40" s="14">
@@ -2096,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="I40" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000C00000, 0, "12.00", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J40" s="4"/>
@@ -2107,7 +2119,7 @@
         <v>24</v>
       </c>
       <c r="B41" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0x000000000</v>
       </c>
       <c r="C41" s="14">
@@ -2125,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>{ 0x000000000, 0, "..", "up", 30, "", "", 0 },</v>
       </c>
       <c r="J41" s="4"/>
@@ -2560,10 +2572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2576,9 +2588,10 @@
     <col min="6" max="6" width="9.90625" customWidth="1"/>
     <col min="7" max="7" width="12.6328125" customWidth="1"/>
     <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>107</v>
       </c>
@@ -2589,8 +2602,15 @@
       <c r="C1" s="6"/>
       <c r="F1" s="18"/>
       <c r="G1" s="19"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L1" s="4">
+        <v>24</v>
+      </c>
+      <c r="M1" s="8">
+        <f>_xlfn.BITLSHIFT(1,L1)</f>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>108</v>
       </c>
@@ -2602,8 +2622,10 @@
       <c r="E2" s="21"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>109</v>
       </c>
@@ -2615,8 +2637,10 @@
       <c r="E3" s="21"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>102</v>
       </c>
@@ -2630,24 +2654,28 @@
       <c r="D4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>103</v>
       </c>
       <c r="B5" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5" s="22">
         <f>TAN(RADIANS(B4/2-B5))</f>
-        <v>0.57735026918962573</v>
+        <v>0.46630765815499858</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+    </row>
+    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>104</v>
       </c>
@@ -2660,8 +2688,10 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>45</v>
       </c>
@@ -2669,11 +2699,15 @@
         <v>1800</v>
       </c>
       <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" ht="5.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>105</v>
       </c>
@@ -2695,8 +2729,10 @@
       <c r="I9" s="16" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L9" s="14"/>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -2727,8 +2763,10 @@
         <f>H10*C10/2</f>
         <v>3.2524065164348914E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L10" s="14"/>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -2745,11 +2783,11 @@
       </c>
       <c r="E11" s="19">
         <f t="shared" ref="E11:E17" si="2">$B$6-($B$1-C11)*$C$5</f>
-        <v>0.11315308470820817</v>
+        <v>0.20939001427155168</v>
       </c>
       <c r="F11" s="20">
         <f t="shared" si="1"/>
-        <v>101.83777623738736</v>
+        <v>188.4510128443965</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="22">
@@ -2757,11 +2795,13 @@
         <v>0.50037023329767572</v>
       </c>
       <c r="I11" s="22">
-        <f>0.5*(H11*H11-H10*H10)*TAN(RADIANS(60))</f>
+        <f t="shared" ref="I11:I27" si="3">0.5*(H11*H11-H10*H10)*TAN(RADIANS(60))</f>
         <v>0.15177897076696162</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L11" s="14"/>
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>3</v>
       </c>
@@ -2773,28 +2813,30 @@
         <v>0.61282587702834124</v>
       </c>
       <c r="D12" s="19">
-        <f t="shared" ref="D12:D27" si="3">C12/25.4</f>
+        <f t="shared" ref="D12:D27" si="4">C12/25.4</f>
         <v>2.4127003032611862E-2</v>
       </c>
       <c r="E12" s="19">
         <f t="shared" si="2"/>
-        <v>0.21678315312805158</v>
+        <v>0.29308876197825456</v>
       </c>
       <c r="F12" s="20">
         <f t="shared" si="1"/>
-        <v>195.10483781524641</v>
+        <v>263.77988578042908</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="22">
-        <f t="shared" ref="H12:H27" si="4">C12/SIN(RADIANS(60))</f>
+        <f t="shared" ref="H12:H27" si="5">C12/SIN(RADIANS(60))</f>
         <v>0.70763037013736263</v>
       </c>
       <c r="I12" s="22">
-        <f>0.5*(H12*H12-H11*H11)*TAN(RADIANS(60))</f>
+        <f t="shared" si="3"/>
         <v>0.21682710109565942</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L12" s="14"/>
+      <c r="M12" s="13"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>4</v>
       </c>
@@ -2806,28 +2848,28 @@
         <v>0.75055534994651341</v>
       </c>
       <c r="D13" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.9549423226240688E-2</v>
       </c>
       <c r="E13" s="19">
         <f t="shared" si="2"/>
-        <v>0.29630130139270355</v>
+        <v>0.3573130699536497</v>
       </c>
       <c r="F13" s="20">
         <f t="shared" si="1"/>
-        <v>266.67117125343322</v>
+        <v>321.58176295828474</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.86666666666666659</v>
       </c>
       <c r="I13" s="22">
-        <f>0.5*(H13*H13-H12*H12)*TAN(RADIANS(60))</f>
+        <f t="shared" si="3"/>
         <v>0.21682710109565917</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>5</v>
       </c>
@@ -2839,28 +2881,28 @@
         <v>0.8666666666666667</v>
       </c>
       <c r="D14" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4120734908136489E-2</v>
       </c>
       <c r="E14" s="19">
         <f t="shared" si="2"/>
-        <v>0.36333820135704598</v>
+        <v>0.41145666613871773</v>
       </c>
       <c r="F14" s="20">
         <f t="shared" si="1"/>
-        <v>327.00438122134136</v>
+        <v>370.31099952484595</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0007404665953514</v>
       </c>
       <c r="I14" s="22">
-        <f>0.5*(H14*H14-H13*H13)*TAN(RADIANS(60))</f>
+        <f t="shared" si="3"/>
         <v>0.21682710109565967</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>6</v>
       </c>
@@ -2872,28 +2914,28 @@
         <v>0.96896279024990895</v>
       </c>
       <c r="D15" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.8148141348421614E-2</v>
       </c>
       <c r="E15" s="19">
         <f t="shared" si="2"/>
-        <v>0.4223988958448861</v>
+        <v>0.45915813196515376</v>
       </c>
       <c r="F15" s="20">
         <f t="shared" si="1"/>
-        <v>380.15900626039752</v>
+        <v>413.24231876863837</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1188618555710317</v>
       </c>
       <c r="I15" s="22">
-        <f>0.5*(H15*H15-H14*H14)*TAN(RADIANS(60))</f>
+        <f t="shared" si="3"/>
         <v>0.21682710109565956</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>7</v>
       </c>
@@ -2905,24 +2947,24 @@
         <v>1.0614455552060438</v>
       </c>
       <c r="D16" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.1789195086852117E-2</v>
       </c>
       <c r="E16" s="19">
         <f t="shared" si="2"/>
-        <v>0.47579384508771139</v>
+        <v>0.50228355351154819</v>
       </c>
       <c r="F16" s="20">
         <f t="shared" si="1"/>
-        <v>428.21446057894025</v>
+        <v>452.05519816039339</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2256517540566825</v>
       </c>
       <c r="I16" s="22">
-        <f>0.5*(H16*H16-H15*H15)*TAN(RADIANS(60))</f>
+        <f t="shared" si="3"/>
         <v>0.21682710109565936</v>
       </c>
     </row>
@@ -2938,23 +2980,23 @@
         <v>1.146492234794656</v>
       </c>
       <c r="D17" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.513748955884473E-2</v>
       </c>
       <c r="E17" s="19">
         <f t="shared" si="2"/>
-        <v>0.52489556844188057</v>
+        <v>0.54194147150437244</v>
       </c>
       <c r="F17" s="20">
         <f t="shared" si="1"/>
-        <v>472.4060115976925</v>
+        <v>487.7473243539352</v>
       </c>
       <c r="H17" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3238552007650206</v>
       </c>
       <c r="I17" s="22">
-        <f>0.5*(H17*H17-H16*H16)*TAN(RADIANS(60))</f>
+        <f t="shared" si="3"/>
         <v>0.21682710109565936</v>
       </c>
     </row>
@@ -2966,27 +3008,27 @@
         <v>8</v>
       </c>
       <c r="C18" s="18">
-        <f t="shared" ref="C18:C27" si="5">$B$1*SQRT(B18)/SQRT($B$2-1)</f>
+        <f t="shared" ref="C18:C27" si="6">$B$1*SQRT(B18)/SQRT($B$2-1)</f>
         <v>1.2256517540566825</v>
       </c>
       <c r="D18" s="19">
+        <f t="shared" si="4"/>
+        <v>4.8254006065223724E-2</v>
+      </c>
+      <c r="E18" s="19">
+        <f t="shared" ref="E18:E20" si="7">$B$6-($B$1-C18)*$C$5</f>
+        <v>0.57885416155212344</v>
+      </c>
+      <c r="F18" s="20">
+        <f t="shared" ref="F18:F27" si="8">$B$7/$B$3*E18</f>
+        <v>520.96874539691112</v>
+      </c>
+      <c r="H18" s="22">
+        <f t="shared" si="5"/>
+        <v>1.4152607402747253</v>
+      </c>
+      <c r="I18" s="22">
         <f t="shared" si="3"/>
-        <v>4.8254006065223724E-2</v>
-      </c>
-      <c r="E18" s="19">
-        <f t="shared" ref="E18:E20" si="6">$B$6-($B$1-C18)*$C$5</f>
-        <v>0.57059833819673289</v>
-      </c>
-      <c r="F18" s="20">
-        <f t="shared" ref="F18:F27" si="7">$B$7/$B$3*E18</f>
-        <v>513.53850437705955</v>
-      </c>
-      <c r="H18" s="22">
-        <f t="shared" si="4"/>
-        <v>1.4152607402747253</v>
-      </c>
-      <c r="I18" s="22">
-        <f>0.5*(H18*H18-H17*H17)*TAN(RADIANS(60))</f>
         <v>0.21682710109565936</v>
       </c>
     </row>
@@ -2998,27 +3040,27 @@
         <v>9</v>
       </c>
       <c r="C19" s="18">
+        <f t="shared" si="6"/>
+        <v>1.3</v>
+      </c>
+      <c r="D19" s="19">
+        <f t="shared" si="4"/>
+        <v>5.1181102362204731E-2</v>
+      </c>
+      <c r="E19" s="19">
+        <f t="shared" si="7"/>
+        <v>0.61352331800588378</v>
+      </c>
+      <c r="F19" s="20">
+        <f t="shared" si="8"/>
+        <v>552.17098620529543</v>
+      </c>
+      <c r="H19" s="22">
         <f t="shared" si="5"/>
-        <v>1.3</v>
-      </c>
-      <c r="D19" s="19">
+        <v>1.501110699893027</v>
+      </c>
+      <c r="I19" s="22">
         <f t="shared" si="3"/>
-        <v>5.1181102362204731E-2</v>
-      </c>
-      <c r="E19" s="19">
-        <f t="shared" si="6"/>
-        <v>0.61352331800588378</v>
-      </c>
-      <c r="F19" s="20">
-        <f t="shared" si="7"/>
-        <v>552.17098620529543</v>
-      </c>
-      <c r="H19" s="22">
-        <f t="shared" si="4"/>
-        <v>1.501110699893027</v>
-      </c>
-      <c r="I19" s="22">
-        <f>0.5*(H19*H19-H18*H18)*TAN(RADIANS(60))</f>
         <v>0.21682710109565917</v>
       </c>
     </row>
@@ -3030,27 +3072,27 @@
         <v>10</v>
       </c>
       <c r="C20" s="18">
+        <f t="shared" si="6"/>
+        <v>1.3703203194062981</v>
+      </c>
+      <c r="D20" s="19">
+        <f t="shared" si="4"/>
+        <v>5.3949618874263708E-2</v>
+      </c>
+      <c r="E20" s="19">
+        <f t="shared" si="7"/>
+        <v>0.64631422146894613</v>
+      </c>
+      <c r="F20" s="20">
+        <f t="shared" si="8"/>
+        <v>581.68279932205155</v>
+      </c>
+      <c r="H20" s="22">
         <f t="shared" si="5"/>
-        <v>1.3703203194062981</v>
-      </c>
-      <c r="D20" s="19">
+        <v>1.5823096105704804</v>
+      </c>
+      <c r="I20" s="22">
         <f t="shared" si="3"/>
-        <v>5.3949618874263708E-2</v>
-      </c>
-      <c r="E20" s="19">
-        <f t="shared" si="6"/>
-        <v>0.65412277334461044</v>
-      </c>
-      <c r="F20" s="20">
-        <f t="shared" si="7"/>
-        <v>588.71049601014943</v>
-      </c>
-      <c r="H20" s="22">
-        <f t="shared" si="4"/>
-        <v>1.5823096105704804</v>
-      </c>
-      <c r="I20" s="22">
-        <f>0.5*(H20*H20-H19*H19)*TAN(RADIANS(60))</f>
         <v>0.21682710109566072</v>
       </c>
     </row>
@@ -3062,27 +3104,27 @@
         <v>11</v>
       </c>
       <c r="C21" s="18">
+        <f t="shared" si="6"/>
+        <v>1.4372040758206734</v>
+      </c>
+      <c r="D21" s="19">
+        <f t="shared" si="4"/>
+        <v>5.6582837630735176E-2</v>
+      </c>
+      <c r="E21" s="19">
+        <f t="shared" ref="E21:E23" si="9">$B$6-($B$1-C21)*$C$5</f>
+        <v>0.6775026292911428</v>
+      </c>
+      <c r="F21" s="20">
+        <f t="shared" si="8"/>
+        <v>609.75236636202851</v>
+      </c>
+      <c r="H21" s="22">
         <f t="shared" si="5"/>
-        <v>1.4372040758206734</v>
-      </c>
-      <c r="D21" s="19">
+        <v>1.6595403201109864</v>
+      </c>
+      <c r="I21" s="22">
         <f t="shared" si="3"/>
-        <v>5.6582837630735176E-2</v>
-      </c>
-      <c r="E21" s="19">
-        <f t="shared" ref="E21:E23" si="8">$B$6-($B$1-C21)*$C$5</f>
-        <v>0.69273812811486335</v>
-      </c>
-      <c r="F21" s="20">
-        <f t="shared" si="7"/>
-        <v>623.46431530337702</v>
-      </c>
-      <c r="H21" s="22">
-        <f t="shared" si="4"/>
-        <v>1.6595403201109864</v>
-      </c>
-      <c r="I21" s="22">
-        <f>0.5*(H21*H21-H20*H20)*TAN(RADIANS(60))</f>
         <v>0.21682710109565881</v>
       </c>
     </row>
@@ -3094,27 +3136,27 @@
         <v>12</v>
       </c>
       <c r="C22" s="18">
+        <f t="shared" si="6"/>
+        <v>1.5011106998930268</v>
+      </c>
+      <c r="D22" s="19">
+        <f t="shared" si="4"/>
+        <v>5.9098846452481375E-2</v>
+      </c>
+      <c r="E22" s="19">
+        <f t="shared" si="9"/>
+        <v>0.70730277750291382</v>
+      </c>
+      <c r="F22" s="20">
+        <f t="shared" si="8"/>
+        <v>636.57249975262243</v>
+      </c>
+      <c r="H22" s="22">
         <f t="shared" si="5"/>
-        <v>1.5011106998930268</v>
-      </c>
-      <c r="D22" s="19">
+        <v>1.7333333333333332</v>
+      </c>
+      <c r="I22" s="22">
         <f t="shared" si="3"/>
-        <v>5.9098846452481375E-2</v>
-      </c>
-      <c r="E22" s="19">
-        <f t="shared" si="8"/>
-        <v>0.72963463472603685</v>
-      </c>
-      <c r="F22" s="20">
-        <f t="shared" si="7"/>
-        <v>656.67117125343316</v>
-      </c>
-      <c r="H22" s="22">
-        <f t="shared" si="4"/>
-        <v>1.7333333333333332</v>
-      </c>
-      <c r="I22" s="22">
-        <f>0.5*(H22*H22-H21*H21)*TAN(RADIANS(60))</f>
         <v>0.21682710109565803</v>
       </c>
     </row>
@@ -3126,27 +3168,27 @@
         <v>13</v>
       </c>
       <c r="C23" s="18">
+        <f t="shared" si="6"/>
+        <v>1.5624055527010621</v>
+      </c>
+      <c r="D23" s="19">
+        <f t="shared" si="4"/>
+        <v>6.1512029633900088E-2</v>
+      </c>
+      <c r="E23" s="19">
+        <f t="shared" si="9"/>
+        <v>0.73588503677278405</v>
+      </c>
+      <c r="F23" s="20">
+        <f t="shared" si="8"/>
+        <v>662.29653309550565</v>
+      </c>
+      <c r="H23" s="22">
         <f t="shared" si="5"/>
-        <v>1.5624055527010621</v>
-      </c>
-      <c r="D23" s="19">
+        <v>1.8041105328706486</v>
+      </c>
+      <c r="I23" s="22">
         <f t="shared" si="3"/>
-        <v>6.1512029633900088E-2</v>
-      </c>
-      <c r="E23" s="19">
-        <f t="shared" si="8"/>
-        <v>0.76502323449469445</v>
-      </c>
-      <c r="F23" s="20">
-        <f t="shared" si="7"/>
-        <v>688.52091104522503</v>
-      </c>
-      <c r="H23" s="22">
-        <f t="shared" si="4"/>
-        <v>1.8041105328706486</v>
-      </c>
-      <c r="I23" s="22">
-        <f>0.5*(H23*H23-H22*H22)*TAN(RADIANS(60))</f>
         <v>0.21682710109566072</v>
       </c>
     </row>
@@ -3158,27 +3200,27 @@
         <v>14</v>
       </c>
       <c r="C24" s="18">
+        <f t="shared" si="6"/>
+        <v>1.6213848676020415</v>
+      </c>
+      <c r="D24" s="19">
+        <f t="shared" si="4"/>
+        <v>6.3834049905592188E-2</v>
+      </c>
+      <c r="E24" s="19">
+        <f t="shared" ref="E24:E27" si="10">$B$6-($B$1-C24)*$C$5</f>
+        <v>0.76338754298384603</v>
+      </c>
+      <c r="F24" s="20">
+        <f t="shared" si="8"/>
+        <v>687.04878868546143</v>
+      </c>
+      <c r="H24" s="22">
         <f t="shared" si="5"/>
-        <v>1.6213848676020415</v>
-      </c>
-      <c r="D24" s="19">
+        <v>1.8722139795400488</v>
+      </c>
+      <c r="I24" s="22">
         <f t="shared" si="3"/>
-        <v>6.3834049905592188E-2</v>
-      </c>
-      <c r="E24" s="19">
-        <f t="shared" ref="E24:E27" si="9">$B$6-($B$1-C24)*$C$5</f>
-        <v>0.79907495782939464</v>
-      </c>
-      <c r="F24" s="20">
-        <f t="shared" si="7"/>
-        <v>719.16746204645517</v>
-      </c>
-      <c r="H24" s="22">
-        <f t="shared" si="4"/>
-        <v>1.8722139795400488</v>
-      </c>
-      <c r="I24" s="22">
-        <f>0.5*(H24*H24-H23*H23)*TAN(RADIANS(60))</f>
         <v>0.21682710109565956</v>
       </c>
     </row>
@@ -3190,27 +3232,27 @@
         <v>15</v>
       </c>
       <c r="C25" s="18">
+        <f t="shared" si="6"/>
+        <v>1.6782927833565475</v>
+      </c>
+      <c r="D25" s="19">
+        <f t="shared" si="4"/>
+        <v>6.6074519029785339E-2</v>
+      </c>
+      <c r="E25" s="19">
+        <f t="shared" si="10"/>
+        <v>0.7899241399098117</v>
+      </c>
+      <c r="F25" s="20">
+        <f t="shared" si="8"/>
+        <v>710.93172591883058</v>
+      </c>
+      <c r="H25" s="22">
         <f t="shared" si="5"/>
-        <v>1.6782927833565475</v>
-      </c>
-      <c r="D25" s="19">
+        <v>1.9379255804998181</v>
+      </c>
+      <c r="I25" s="22">
         <f t="shared" si="3"/>
-        <v>6.6074519029785339E-2</v>
-      </c>
-      <c r="E25" s="19">
-        <f t="shared" si="9"/>
-        <v>0.83193075830927921</v>
-      </c>
-      <c r="F25" s="20">
-        <f t="shared" si="7"/>
-        <v>748.7376824783513</v>
-      </c>
-      <c r="H25" s="22">
-        <f t="shared" si="4"/>
-        <v>1.9379255804998181</v>
-      </c>
-      <c r="I25" s="22">
-        <f>0.5*(H25*H25-H24*H24)*TAN(RADIANS(60))</f>
         <v>0.21682710109565956</v>
       </c>
     </row>
@@ -3222,27 +3264,27 @@
         <v>16</v>
       </c>
       <c r="C26" s="18">
+        <f t="shared" si="6"/>
+        <v>1.7333333333333334</v>
+      </c>
+      <c r="D26" s="19">
+        <f t="shared" si="4"/>
+        <v>6.8241469816272979E-2</v>
+      </c>
+      <c r="E26" s="19">
+        <f t="shared" si="10"/>
+        <v>0.81558996987304977</v>
+      </c>
+      <c r="F26" s="20">
+        <f t="shared" si="8"/>
+        <v>734.03097288574475</v>
+      </c>
+      <c r="H26" s="22">
         <f t="shared" si="5"/>
-        <v>1.7333333333333334</v>
-      </c>
-      <c r="D26" s="19">
+        <v>2.0014809331907029</v>
+      </c>
+      <c r="I26" s="22">
         <f t="shared" si="3"/>
-        <v>6.8241469816272979E-2</v>
-      </c>
-      <c r="E26" s="19">
-        <f t="shared" si="9"/>
-        <v>0.86370843465472158</v>
-      </c>
-      <c r="F26" s="20">
-        <f t="shared" si="7"/>
-        <v>777.33759118924945</v>
-      </c>
-      <c r="H26" s="22">
-        <f t="shared" si="4"/>
-        <v>2.0014809331907029</v>
-      </c>
-      <c r="I26" s="22">
-        <f>0.5*(H26*H26-H25*H25)*TAN(RADIANS(60))</f>
         <v>0.21682710109565881</v>
       </c>
     </row>
@@ -3254,27 +3296,27 @@
         <v>17</v>
       </c>
       <c r="C27" s="18">
+        <f t="shared" si="6"/>
+        <v>1.7866791044343195</v>
+      </c>
+      <c r="D27" s="19">
+        <f t="shared" si="4"/>
+        <v>7.0341697024973213E-2</v>
+      </c>
+      <c r="E27" s="19">
+        <f t="shared" si="10"/>
+        <v>0.84046551146762327</v>
+      </c>
+      <c r="F27" s="20">
+        <f t="shared" si="8"/>
+        <v>756.41896032086095</v>
+      </c>
+      <c r="H27" s="22">
         <f t="shared" si="5"/>
-        <v>1.7866791044343195</v>
-      </c>
-      <c r="D27" s="19">
+        <v>2.0630793238012677</v>
+      </c>
+      <c r="I27" s="22">
         <f t="shared" si="3"/>
-        <v>7.0341697024973213E-2</v>
-      </c>
-      <c r="E27" s="19">
-        <f t="shared" si="9"/>
-        <v>0.8945076299600041</v>
-      </c>
-      <c r="F27" s="20">
-        <f t="shared" si="7"/>
-        <v>805.05686696400369</v>
-      </c>
-      <c r="H27" s="22">
-        <f t="shared" si="4"/>
-        <v>2.0630793238012677</v>
-      </c>
-      <c r="I27" s="22">
-        <f>0.5*(H27*H27-H26*H26)*TAN(RADIANS(60))</f>
         <v>0.21682710109565842</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clean step by step threading routine, there was few errors when thread shift slightly, now it seems to fit well
</commit_message>
<xml_diff>
--- a/feed_tab.xlsx
+++ b/feed_tab.xlsx
@@ -373,7 +373,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -406,6 +406,13 @@
       <name val="Microsoft Sans Serif"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -468,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -500,9 +507,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -523,6 +527,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,7 +909,7 @@
   <dimension ref="A1:Y161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -905,7 +922,7 @@
     <col min="6" max="6" width="7.7265625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="9.54296875" customWidth="1"/>
-    <col min="9" max="9" width="35" customWidth="1"/>
+    <col min="9" max="9" width="42.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -972,17 +989,17 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="6"/>
@@ -1002,19 +1019,19 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="25" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>50</v>
       </c>
       <c r="F5" s="11"/>
@@ -1035,19 +1052,19 @@
       <c r="Y5" s="6"/>
     </row>
     <row r="6" spans="1:25" ht="13" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>1800</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>400</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>1</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>400</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>1</v>
       </c>
       <c r="F6" s="11"/>
@@ -1095,24 +1112,24 @@
       <c r="Y7" s="6"/>
     </row>
     <row r="8" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="16" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="28"/>
+      <c r="E8" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="29" t="s">
         <v>101</v>
       </c>
       <c r="P8" s="6" t="s">
@@ -1130,30 +1147,34 @@
       <c r="Y8" s="6"/>
     </row>
     <row r="9" spans="1:25" ht="13" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
+      <c r="A9" s="26">
         <v>2</v>
       </c>
-      <c r="C9" s="14">
-        <v>0</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="B9" s="26" t="str">
+        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D9,"tpi"),25.4/A9,A9))*$B$1,0),8)),"0x00000000")</f>
+        <v>0x04800000</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="14">
-        <v>0</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="26">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="12" t="str">
-        <f>$A$2&amp;J6&amp;$C$2&amp;C9&amp;$D$2&amp;SUBSTITUTE(TEXT(A9,"0,00"),",",".")&amp;$G$2&amp;D9&amp;$E$2&amp;E9&amp;$D$2&amp;F9&amp;$G$2&amp;G9&amp;$E$2&amp;H9&amp;$B$2</f>
-        <v>{ 0x004800000, 0, "2.00", "mm", 0, "1.26", ".050", 0 },</v>
+      <c r="H9" s="25">
+        <v>0</v>
+      </c>
+      <c r="I9" s="25" t="str">
+        <f t="shared" ref="I9:I35" si="0">$A$2&amp;B9&amp;$C$2&amp;C9&amp;$D$2&amp;SUBSTITUTE(TEXT(A9,IF(EXACT(D9,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D9&amp;$E$2&amp;E9&amp;$D$2&amp;F9&amp;$G$2&amp;G9&amp;$E$2&amp;H9&amp;$B$2</f>
+        <v>{ 0x04800000, 0, "2.00", "mm", 0, "1.26", ".050", 0 },</v>
       </c>
       <c r="J9" s="4"/>
       <c r="P9" s="6" t="s">
@@ -1171,100 +1192,100 @@
       <c r="Y9" s="6"/>
     </row>
     <row r="10" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+      <c r="A10" s="26">
         <v>2</v>
       </c>
-      <c r="B10" s="13" t="str">
-        <f t="shared" ref="B10:B11" si="0">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A10)*$B$1,0),9)),"0x000000000")</f>
-        <v>0x004800000</v>
-      </c>
-      <c r="C10" s="14">
-        <v>0</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="B10" s="26" t="str">
+        <f t="shared" ref="B10:B41" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D10,"tpi"),25.4/A10,A10))*$B$1,0),8)),"0x00000000")</f>
+        <v>0x04800000</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="14">
-        <v>0</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="26">
+        <v>0</v>
+      </c>
+      <c r="F10" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="25">
         <v>1</v>
       </c>
-      <c r="I10" s="12" t="str">
-        <f>$A$2&amp;B10&amp;$C$2&amp;C10&amp;$D$2&amp;SUBSTITUTE(TEXT(A10,"0,00"),",",".")&amp;$G$2&amp;D10&amp;$E$2&amp;E10&amp;$D$2&amp;F10&amp;$G$2&amp;G10&amp;$E$2&amp;H10&amp;$B$2</f>
-        <v>{ 0x004800000, 0, "2.00", "mm", 0, "1.26", ".050", 1 },</v>
+      <c r="I10" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x04800000, 0, "2.00", "mm", 0, "1.26", ".050", 1 },</v>
       </c>
       <c r="J10" s="4"/>
       <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
+      <c r="A11" s="26">
         <v>2</v>
       </c>
-      <c r="B11" s="13" t="str">
+      <c r="B11" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>0x04800000</v>
+      </c>
+      <c r="C11" s="26">
+        <v>0</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="26">
+        <v>0</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="25">
+        <v>2</v>
+      </c>
+      <c r="I11" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>0x004800000</v>
-      </c>
-      <c r="C11" s="14">
-        <v>0</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="14">
-        <v>0</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="6">
-        <v>2</v>
-      </c>
-      <c r="I11" s="12" t="str">
-        <f>$A$2&amp;B11&amp;$C$2&amp;C11&amp;$D$2&amp;SUBSTITUTE(TEXT(A11,"0,00"),",",".")&amp;$G$2&amp;D11&amp;$E$2&amp;E11&amp;$D$2&amp;F11&amp;$G$2&amp;G11&amp;$E$2&amp;H11&amp;$B$2</f>
-        <v>{ 0x004800000, 0, "2.00", "mm", 0, "1.26", ".050", 2 },</v>
+        <v>{ 0x04800000, 0, "2.00", "mm", 0, "1.26", ".050", 2 },</v>
       </c>
       <c r="J11" s="4"/>
       <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="1:25" ht="13" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
+      <c r="A12" s="26">
         <v>1.5</v>
       </c>
-      <c r="B12" s="13" t="str">
-        <f t="shared" ref="B12:B41" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A12)*$B$1,0),9)),"0x000000000")</f>
-        <v>0x006000000</v>
-      </c>
-      <c r="C12" s="14">
-        <v>0</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="B12" s="26" t="str">
+        <f t="shared" si="1"/>
+        <v>0x06000000</v>
+      </c>
+      <c r="C12" s="26">
+        <v>0</v>
+      </c>
+      <c r="D12" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="14">
-        <v>0</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="E12" s="26">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12" t="str">
-        <f t="shared" ref="I12:I41" si="2">$A$2&amp;B12&amp;$C$2&amp;C12&amp;$D$2&amp;SUBSTITUTE(TEXT(A12,"0,00"),",",".")&amp;$G$2&amp;D12&amp;$E$2&amp;E12&amp;$D$2&amp;F12&amp;$G$2&amp;G12&amp;$E$2&amp;H12&amp;$B$2</f>
-        <v>{ 0x006000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
+      <c r="H12" s="25">
+        <v>0</v>
+      </c>
+      <c r="I12" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x06000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>19</v>
@@ -1274,34 +1295,34 @@
       </c>
     </row>
     <row r="13" spans="1:25" ht="13" x14ac:dyDescent="0.3">
-      <c r="A13" s="13">
+      <c r="A13" s="26">
         <v>1</v>
       </c>
-      <c r="B13" s="13" t="str">
+      <c r="B13" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x009000000</v>
-      </c>
-      <c r="C13" s="14">
-        <v>0</v>
-      </c>
-      <c r="D13" s="13" t="s">
+        <v>0x09000000</v>
+      </c>
+      <c r="C13" s="26">
+        <v>0</v>
+      </c>
+      <c r="D13" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="14">
-        <v>0</v>
-      </c>
-      <c r="F13" s="10" t="s">
+      <c r="E13" s="26">
+        <v>0</v>
+      </c>
+      <c r="F13" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="12" t="str">
-        <f>$A$2&amp;B13&amp;$C$2&amp;C13&amp;$D$2&amp;SUBSTITUTE(TEXT(A13,"0,00"),",",".")&amp;$G$2&amp;D13&amp;$E$2&amp;E13&amp;$D$2&amp;F13&amp;$G$2&amp;G13&amp;$E$2&amp;H13&amp;$B$2</f>
-        <v>{ 0x009000000, 0, "1.00", "mm", 0, ".65", ".026", 0 },</v>
+      <c r="H13" s="25">
+        <v>0</v>
+      </c>
+      <c r="I13" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x09000000, 0, "1.00", "mm", 0, ".65", ".026", 0 },</v>
       </c>
       <c r="J13" s="4"/>
       <c r="P13" s="6" t="s">
@@ -1312,833 +1333,833 @@
       </c>
     </row>
     <row r="14" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="13" t="str">
+      <c r="B14" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000000000</v>
-      </c>
-      <c r="C14" s="14">
+        <v>0x00000000</v>
+      </c>
+      <c r="C14" s="26">
         <v>20</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000000000, 20, "F", "mm", 0, "", "", 0 },</v>
+      <c r="E14" s="26">
+        <v>0</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="25">
+        <v>0</v>
+      </c>
+      <c r="I14" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x00000000, 20, "F", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J14" s="4"/>
       <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+      <c r="A15" s="26">
         <v>0.2</v>
       </c>
-      <c r="B15" s="13" t="str">
+      <c r="B15" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x02D000000</v>
-      </c>
-      <c r="C15" s="14">
-        <v>0</v>
-      </c>
-      <c r="D15" s="13" t="s">
+        <v>0x2D000000</v>
+      </c>
+      <c r="C15" s="26">
+        <v>0</v>
+      </c>
+      <c r="D15" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="26">
         <v>20</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="6">
-        <v>0</v>
-      </c>
-      <c r="I15" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x02D000000, 0, "0.20", "mm", 20, "", "", 0 },</v>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="25">
+        <v>0</v>
+      </c>
+      <c r="I15" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x2D000000, 0, "0.20", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J15" s="4"/>
       <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
+      <c r="A16" s="26">
         <v>0.18</v>
       </c>
-      <c r="B16" s="13" t="str">
+      <c r="B16" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x032000000</v>
-      </c>
-      <c r="C16" s="14">
-        <v>0</v>
-      </c>
-      <c r="D16" s="13" t="s">
+        <v>0x32000000</v>
+      </c>
+      <c r="C16" s="26">
+        <v>0</v>
+      </c>
+      <c r="D16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="26">
         <v>20</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="6">
-        <v>0</v>
-      </c>
-      <c r="I16" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x032000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="25">
+        <v>0</v>
+      </c>
+      <c r="I16" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x32000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J16" s="4"/>
       <c r="Q16" s="7"/>
     </row>
     <row r="17" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
+      <c r="A17" s="26">
         <v>0.15</v>
       </c>
-      <c r="B17" s="13" t="str">
+      <c r="B17" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x03C000000</v>
-      </c>
-      <c r="C17" s="14">
-        <v>0</v>
-      </c>
-      <c r="D17" s="13" t="s">
+        <v>0x3C000000</v>
+      </c>
+      <c r="C17" s="26">
+        <v>0</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="26">
         <v>20</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="6">
-        <v>0</v>
-      </c>
-      <c r="I17" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x03C000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="25">
+        <v>0</v>
+      </c>
+      <c r="I17" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x3C000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J17" s="4"/>
       <c r="Q17" s="7"/>
     </row>
     <row r="18" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
+      <c r="A18" s="26">
         <v>0.12</v>
       </c>
-      <c r="B18" s="13" t="str">
+      <c r="B18" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x04B000000</v>
-      </c>
-      <c r="C18" s="14">
-        <v>0</v>
-      </c>
-      <c r="D18" s="13" t="s">
+        <v>0x4B000000</v>
+      </c>
+      <c r="C18" s="26">
+        <v>0</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="26">
         <v>20</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="6">
-        <v>0</v>
-      </c>
-      <c r="I18" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x04B000000, 0, "0.12", "mm", 20, "", "", 0 },</v>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="25">
+        <v>0</v>
+      </c>
+      <c r="I18" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x4B000000, 0, "0.12", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J18" s="4"/>
       <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
+      <c r="A19" s="26">
         <v>0.09</v>
       </c>
-      <c r="B19" s="15" t="str">
+      <c r="B19" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x064000000</v>
-      </c>
-      <c r="C19" s="14">
-        <v>0</v>
-      </c>
-      <c r="D19" s="13" t="s">
+        <v>0x64000000</v>
+      </c>
+      <c r="C19" s="26">
+        <v>0</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="26">
         <v>20</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="6">
-        <v>0</v>
-      </c>
-      <c r="I19" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x064000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="25">
+        <v>0</v>
+      </c>
+      <c r="I19" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x64000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J19" s="4"/>
       <c r="Q19" s="7"/>
     </row>
     <row r="20" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
+      <c r="A20" s="26">
         <v>0.06</v>
       </c>
-      <c r="B20" s="13" t="str">
+      <c r="B20" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x096000000</v>
-      </c>
-      <c r="C20" s="14">
-        <v>0</v>
-      </c>
-      <c r="D20" s="13" t="s">
+        <v>0x96000000</v>
+      </c>
+      <c r="C20" s="26">
+        <v>0</v>
+      </c>
+      <c r="D20" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="26">
         <v>20</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="6">
-        <v>0</v>
-      </c>
-      <c r="I20" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x096000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="25">
+        <v>0</v>
+      </c>
+      <c r="I20" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x96000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J20" s="4"/>
       <c r="Q20" s="7"/>
     </row>
     <row r="21" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
+      <c r="A21" s="26">
         <v>0.04</v>
       </c>
-      <c r="B21" s="13" t="str">
+      <c r="B21" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x0E1000000</v>
-      </c>
-      <c r="C21" s="14">
-        <v>0</v>
-      </c>
-      <c r="D21" s="13" t="s">
+        <v>0xE1000000</v>
+      </c>
+      <c r="C21" s="26">
+        <v>0</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="26">
         <v>20</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="6">
-        <v>0</v>
-      </c>
-      <c r="I21" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x0E1000000, 0, "0.04", "mm", 20, "", "", 0 },</v>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="25">
+        <v>0</v>
+      </c>
+      <c r="I21" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0xE1000000, 0, "0.04", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J21" s="4"/>
       <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="13" t="str">
+      <c r="B22" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000000000</v>
-      </c>
-      <c r="C22" s="14">
-        <v>0</v>
-      </c>
-      <c r="D22" s="13" t="s">
+        <v>0x00000000</v>
+      </c>
+      <c r="C22" s="26">
+        <v>0</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="26">
         <v>20</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000000000, 0, "..", "up", 20, "", "", 0 },</v>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="25">
+        <v>0</v>
+      </c>
+      <c r="I22" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x00000000, 0, "..", "up", 20, "", "", 0 },</v>
       </c>
       <c r="J22" s="4"/>
       <c r="Q22" s="7"/>
     </row>
     <row r="23" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="13" t="str">
+      <c r="B23" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000000000</v>
-      </c>
-      <c r="C23" s="14">
+        <v>0x00000000</v>
+      </c>
+      <c r="C23" s="26">
         <v>10</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="14">
-        <v>0</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="6">
-        <v>0</v>
-      </c>
-      <c r="I23" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000000000, 10, "T", "mm", 0, "", "", 0 },</v>
+      <c r="E23" s="26">
+        <v>0</v>
+      </c>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="25">
+        <v>0</v>
+      </c>
+      <c r="I23" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x00000000, 10, "T", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J23" s="4"/>
       <c r="Q23" s="7"/>
     </row>
     <row r="24" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
+      <c r="A24" s="26">
         <v>1.25</v>
       </c>
-      <c r="B24" s="13" t="str">
+      <c r="B24" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x007333333</v>
-      </c>
-      <c r="C24" s="14">
-        <v>0</v>
-      </c>
-      <c r="D24" s="13" t="s">
+        <v>0x07333333</v>
+      </c>
+      <c r="C24" s="26">
+        <v>0</v>
+      </c>
+      <c r="D24" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="26">
         <v>10</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="6">
-        <v>0</v>
-      </c>
-      <c r="I24" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x007333333, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
+      <c r="H24" s="25">
+        <v>0</v>
+      </c>
+      <c r="I24" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x07333333, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
       </c>
       <c r="J24" s="4"/>
       <c r="Q24" s="7"/>
     </row>
     <row r="25" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
+      <c r="A25" s="26">
         <v>1.75</v>
       </c>
-      <c r="B25" s="13" t="str">
+      <c r="B25" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x005249249</v>
-      </c>
-      <c r="C25" s="14">
-        <v>0</v>
-      </c>
-      <c r="D25" s="13" t="s">
+        <v>0x05249249</v>
+      </c>
+      <c r="C25" s="26">
+        <v>0</v>
+      </c>
+      <c r="D25" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="26">
         <v>10</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="6">
-        <v>0</v>
-      </c>
-      <c r="I25" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x005249249, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
+      <c r="H25" s="25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x05249249, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
       </c>
       <c r="J25" s="4"/>
       <c r="Q25" s="7"/>
     </row>
     <row r="26" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
+      <c r="A26" s="26">
         <v>2</v>
       </c>
-      <c r="B26" s="13" t="str">
+      <c r="B26" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x004800000</v>
-      </c>
-      <c r="C26" s="14">
-        <v>0</v>
-      </c>
-      <c r="D26" s="13" t="s">
+        <v>0x04800000</v>
+      </c>
+      <c r="C26" s="26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="26">
         <v>10</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H26" s="6">
-        <v>0</v>
-      </c>
-      <c r="I26" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x004800000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
+      <c r="H26" s="25">
+        <v>0</v>
+      </c>
+      <c r="I26" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x04800000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
       </c>
       <c r="J26" s="4"/>
       <c r="Q26" s="7"/>
     </row>
     <row r="27" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
+      <c r="A27" s="26">
         <v>0.5</v>
       </c>
-      <c r="B27" s="13" t="str">
+      <c r="B27" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x012000000</v>
-      </c>
-      <c r="C27" s="14">
-        <v>0</v>
-      </c>
-      <c r="D27" s="13" t="s">
+        <v>0x12000000</v>
+      </c>
+      <c r="C27" s="26">
+        <v>0</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="26">
         <v>10</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="6">
-        <v>0</v>
-      </c>
-      <c r="I27" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x012000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
+      <c r="H27" s="25">
+        <v>0</v>
+      </c>
+      <c r="I27" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x12000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
       </c>
       <c r="J27" s="4"/>
       <c r="Q27" s="7"/>
     </row>
     <row r="28" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
+      <c r="A28" s="26">
         <v>0.75</v>
       </c>
-      <c r="B28" s="13" t="str">
+      <c r="B28" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x00C000000</v>
-      </c>
-      <c r="C28" s="14">
-        <v>0</v>
-      </c>
-      <c r="D28" s="13" t="s">
+        <v>0x0C000000</v>
+      </c>
+      <c r="C28" s="26">
+        <v>0</v>
+      </c>
+      <c r="D28" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="26">
         <v>10</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="6">
-        <v>0</v>
-      </c>
-      <c r="I28" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x00C000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
+      <c r="H28" s="25">
+        <v>0</v>
+      </c>
+      <c r="I28" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x0C000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
       </c>
       <c r="J28" s="4"/>
       <c r="Q28" s="7"/>
     </row>
     <row r="29" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="13" t="str">
+      <c r="B29" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000000000</v>
-      </c>
-      <c r="C29" s="14">
-        <v>0</v>
-      </c>
-      <c r="D29" s="13" t="s">
+        <v>0x00000000</v>
+      </c>
+      <c r="C29" s="26">
+        <v>0</v>
+      </c>
+      <c r="D29" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="26">
         <v>10</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="6">
-        <v>0</v>
-      </c>
-      <c r="I29" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000000000, 0, "..", "up", 10, "", "", 0 },</v>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="25">
+        <v>0</v>
+      </c>
+      <c r="I29" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x00000000, 0, "..", "up", 10, "", "", 0 },</v>
       </c>
       <c r="J29" s="4"/>
       <c r="Q29" s="7"/>
     </row>
     <row r="30" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="13" t="str">
+      <c r="B30" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000000000</v>
-      </c>
-      <c r="C30" s="14">
+        <v>0x00000000</v>
+      </c>
+      <c r="C30" s="26">
         <v>30</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="14">
-        <v>0</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="6">
-        <v>0</v>
-      </c>
-      <c r="I30" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000000000, 30, "T", "tpi", 0, "", "", 0 },</v>
+      <c r="E30" s="26">
+        <v>0</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="25">
+        <v>0</v>
+      </c>
+      <c r="I30" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x00000000, 30, "T", "tpi", 0, "", "", 0 },</v>
       </c>
       <c r="J30" s="4"/>
       <c r="Q30" s="7"/>
     </row>
     <row r="31" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
+      <c r="A31" s="26">
         <v>27</v>
       </c>
-      <c r="B31" s="13" t="str">
+      <c r="B31" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000555555</v>
-      </c>
-      <c r="C31" s="14">
-        <v>0</v>
-      </c>
-      <c r="D31" s="13" t="s">
+        <v>0x09912244</v>
+      </c>
+      <c r="C31" s="26">
+        <v>0</v>
+      </c>
+      <c r="D31" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="26">
         <v>30</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="6">
-        <v>0</v>
-      </c>
-      <c r="I31" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000555555, 0, "27.00", "tpi", 30, "", "", 0 },</v>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="25">
+        <v>0</v>
+      </c>
+      <c r="I31" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x09912244, 0, "27", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J31" s="4"/>
       <c r="Q31" s="7"/>
     </row>
     <row r="32" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
+      <c r="A32" s="26">
         <v>26</v>
       </c>
-      <c r="B32" s="13" t="str">
+      <c r="B32" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000589D89</v>
-      </c>
-      <c r="C32" s="14">
-        <v>0</v>
-      </c>
-      <c r="D32" s="13" t="s">
+        <v>0x09366CD9</v>
+      </c>
+      <c r="C32" s="26">
+        <v>0</v>
+      </c>
+      <c r="D32" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="26">
         <v>30</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="6">
-        <v>0</v>
-      </c>
-      <c r="I32" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000589D89, 0, "26.00", "tpi", 30, "", "", 0 },</v>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="25">
+        <v>0</v>
+      </c>
+      <c r="I32" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x09366CD9, 0, "26", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J32" s="4"/>
       <c r="Q32" s="7"/>
     </row>
     <row r="33" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
+      <c r="A33" s="26">
         <v>24</v>
       </c>
-      <c r="B33" s="13" t="str">
+      <c r="B33" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000600000</v>
-      </c>
-      <c r="C33" s="14">
-        <v>0</v>
-      </c>
-      <c r="D33" s="13" t="s">
+        <v>0x08810204</v>
+      </c>
+      <c r="C33" s="26">
+        <v>0</v>
+      </c>
+      <c r="D33" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="26">
         <v>30</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="6">
-        <v>0</v>
-      </c>
-      <c r="I33" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000600000, 0, "24.00", "tpi", 30, "", "", 0 },</v>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="25">
+        <v>0</v>
+      </c>
+      <c r="I33" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x08810204, 0, "24", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J33" s="4"/>
       <c r="Q33" s="7"/>
     </row>
     <row r="34" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A34" s="14">
+      <c r="A34" s="26">
         <v>22</v>
       </c>
-      <c r="B34" s="13" t="str">
+      <c r="B34" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x00068BA2E</v>
-      </c>
-      <c r="C34" s="14">
-        <v>0</v>
-      </c>
-      <c r="D34" s="13" t="s">
+        <v>0x07CB972E</v>
+      </c>
+      <c r="C34" s="26">
+        <v>0</v>
+      </c>
+      <c r="D34" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="26">
         <v>30</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="6">
-        <v>0</v>
-      </c>
-      <c r="I34" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x00068BA2E, 0, "22.00", "tpi", 30, "", "", 0 },</v>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="25">
+        <v>0</v>
+      </c>
+      <c r="I34" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x07CB972E, 0, "22", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J34" s="4"/>
       <c r="Q34" s="7"/>
     </row>
     <row r="35" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A35" s="14">
+      <c r="A35" s="26">
         <v>20</v>
       </c>
-      <c r="B35" s="13" t="str">
+      <c r="B35" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000733333</v>
-      </c>
-      <c r="C35" s="14">
-        <v>0</v>
-      </c>
-      <c r="D35" s="13" t="s">
+        <v>0x07162C58</v>
+      </c>
+      <c r="C35" s="26">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="26">
         <v>30</v>
       </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="6">
-        <v>0</v>
-      </c>
-      <c r="I35" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x000733333, 0, "20.00", "tpi", 30, "", "", 0 },</v>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="25">
+        <v>0</v>
+      </c>
+      <c r="I35" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>{ 0x07162C58, 0, "20", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J35" s="4"/>
       <c r="Q35" s="7"/>
     </row>
     <row r="36" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="14">
+      <c r="A36" s="26">
         <v>19</v>
       </c>
-      <c r="B36" s="13" t="str">
+      <c r="B36" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x00079435E</v>
-      </c>
-      <c r="C36" s="14">
-        <v>0</v>
-      </c>
-      <c r="D36" s="13" t="s">
+        <v>0x06BB76ED</v>
+      </c>
+      <c r="C36" s="26">
+        <v>0</v>
+      </c>
+      <c r="D36" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="26">
         <v>30</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="6">
-        <v>0</v>
-      </c>
-      <c r="I36" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v>{ 0x00079435E, 0, "19.00", "tpi", 30, "", "", 0 },</v>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="25">
+        <v>0</v>
+      </c>
+      <c r="I36" s="25" t="str">
+        <f t="shared" ref="I36:I41" si="2">$A$2&amp;B36&amp;$C$2&amp;C36&amp;$D$2&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D36&amp;$E$2&amp;E36&amp;$D$2&amp;F36&amp;$G$2&amp;G36&amp;$E$2&amp;H36&amp;$B$2</f>
+        <v>{ 0x06BB76ED, 0, "19", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J36" s="4"/>
       <c r="Q36" s="7"/>
     </row>
     <row r="37" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
+      <c r="A37" s="26">
         <v>18</v>
       </c>
-      <c r="B37" s="13" t="str">
+      <c r="B37" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000800000</v>
-      </c>
-      <c r="C37" s="14">
-        <v>0</v>
-      </c>
-      <c r="D37" s="13" t="s">
+        <v>0x0660C183</v>
+      </c>
+      <c r="C37" s="26">
+        <v>0</v>
+      </c>
+      <c r="D37" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="26">
         <v>30</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="6">
-        <v>0</v>
-      </c>
-      <c r="I37" s="12" t="str">
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="25">
+        <v>0</v>
+      </c>
+      <c r="I37" s="25" t="str">
         <f t="shared" si="2"/>
-        <v>{ 0x000800000, 0, "18.00", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0660C183, 0, "18", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J37" s="4"/>
       <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A38" s="14">
+      <c r="A38" s="26">
         <v>16</v>
       </c>
-      <c r="B38" s="13" t="str">
+      <c r="B38" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000900000</v>
-      </c>
-      <c r="C38" s="14">
-        <v>0</v>
-      </c>
-      <c r="D38" s="13" t="s">
+        <v>0x05AB56AD</v>
+      </c>
+      <c r="C38" s="26">
+        <v>0</v>
+      </c>
+      <c r="D38" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="26">
         <v>30</v>
       </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="6">
-        <v>0</v>
-      </c>
-      <c r="I38" s="12" t="str">
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="25">
+        <v>0</v>
+      </c>
+      <c r="I38" s="25" t="str">
         <f t="shared" si="2"/>
-        <v>{ 0x000900000, 0, "16.00", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x05AB56AD, 0, "16", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J38" s="4"/>
       <c r="Q38" s="7"/>
     </row>
     <row r="39" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A39" s="14">
+      <c r="A39" s="26">
         <v>14</v>
       </c>
-      <c r="B39" s="13" t="str">
+      <c r="B39" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000A49249</v>
-      </c>
-      <c r="C39" s="14">
-        <v>0</v>
-      </c>
-      <c r="D39" s="13" t="s">
+        <v>0x04F5EBD7</v>
+      </c>
+      <c r="C39" s="26">
+        <v>0</v>
+      </c>
+      <c r="D39" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="26">
         <v>30</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="6">
-        <v>0</v>
-      </c>
-      <c r="I39" s="12" t="str">
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="25">
+        <v>0</v>
+      </c>
+      <c r="I39" s="25" t="str">
         <f t="shared" si="2"/>
-        <v>{ 0x000A49249, 0, "14.00", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x04F5EBD7, 0, "14", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J39" s="4"/>
       <c r="Q39" s="7"/>
     </row>
     <row r="40" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A40" s="14">
+      <c r="A40" s="26">
         <v>12</v>
       </c>
-      <c r="B40" s="13" t="str">
+      <c r="B40" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000C00000</v>
-      </c>
-      <c r="C40" s="14">
-        <v>0</v>
-      </c>
-      <c r="D40" s="13" t="s">
+        <v>0x04408102</v>
+      </c>
+      <c r="C40" s="26">
+        <v>0</v>
+      </c>
+      <c r="D40" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="26">
         <v>30</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="6">
-        <v>0</v>
-      </c>
-      <c r="I40" s="12" t="str">
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="25">
+        <v>0</v>
+      </c>
+      <c r="I40" s="25" t="str">
         <f t="shared" si="2"/>
-        <v>{ 0x000C00000, 0, "12.00", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x04408102, 0, "12", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J40" s="4"/>
       <c r="Q40" s="7"/>
     </row>
     <row r="41" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="13" t="str">
+      <c r="B41" s="26" t="str">
         <f t="shared" si="1"/>
-        <v>0x000000000</v>
-      </c>
-      <c r="C41" s="14">
-        <v>0</v>
-      </c>
-      <c r="D41" s="13" t="s">
+        <v>0x00000000</v>
+      </c>
+      <c r="C41" s="26">
+        <v>0</v>
+      </c>
+      <c r="D41" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="26">
         <v>30</v>
       </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="6">
-        <v>0</v>
-      </c>
-      <c r="I41" s="12" t="str">
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="25">
+        <v>0</v>
+      </c>
+      <c r="I41" s="25" t="str">
         <f t="shared" si="2"/>
-        <v>{ 0x000000000, 0, "..", "up", 30, "", "", 0 },</v>
+        <v>{ 0x00000000, 0, "..", "up", 30, "", "", 0 },</v>
       </c>
       <c r="J41" s="4"/>
       <c r="Q41" s="7"/>
@@ -2575,7 +2596,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F10" sqref="F10:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2597,11 +2618,14 @@
       </c>
       <c r="B1" s="6">
         <f>0.65*B3</f>
-        <v>1.3</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="19"/>
+        <v>0.65</v>
+      </c>
+      <c r="C1" s="6">
+        <f>B1/25.4</f>
+        <v>2.5590551181102365E-2</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
       <c r="L1" s="4">
         <v>24</v>
       </c>
@@ -2619,7 +2643,7 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="21"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="L2" s="6"/>
@@ -2630,11 +2654,11 @@
         <v>109</v>
       </c>
       <c r="B3" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="21"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="L3" s="1"/>
@@ -2647,15 +2671,15 @@
       <c r="B4" s="6">
         <v>60</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <f>TAN(RADIANS(B4/2))</f>
         <v>0.57735026918962573</v>
       </c>
       <c r="D4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -2664,7 +2688,7 @@
       <c r="B5" s="6">
         <v>5</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <f>TAN(RADIANS(B4/2-B5))</f>
         <v>0.46630765815499858</v>
       </c>
@@ -2672,27 +2696,27 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="17">
         <f>(B1-C10)*C4</f>
-        <v>0.61352331800588378</v>
+        <v>0.30676165900294189</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="6">
@@ -2707,26 +2731,26 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="5.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="25" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="15" t="s">
         <v>111</v>
       </c>
       <c r="L9" s="14"/>
@@ -2739,13 +2763,13 @@
       <c r="B10" s="6">
         <v>0.3</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <f t="shared" ref="C10:C17" si="0">$B$1*SQRT(B10)/SQRT($B$2-1)</f>
-        <v>0.23734644158557197</v>
-      </c>
-      <c r="D10" s="19">
+        <v>0.11867322079278599</v>
+      </c>
+      <c r="D10" s="18">
         <f>C10/25.4</f>
-        <v>9.344348093920157E-3</v>
+        <v>4.6721740469600785E-3</v>
       </c>
       <c r="E10" s="6">
         <v>0</v>
@@ -2754,14 +2778,14 @@
         <f t="shared" ref="F10:F17" si="1">$B$7/$B$3*E10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="22">
+      <c r="G10" s="19"/>
+      <c r="H10" s="21">
         <f>C10/SIN(RADIANS(60))</f>
-        <v>0.27406406388125953</v>
-      </c>
-      <c r="I10" s="22">
+        <v>0.13703203194062977</v>
+      </c>
+      <c r="I10" s="21">
         <f>H10*C10/2</f>
-        <v>3.2524065164348914E-2</v>
+        <v>8.1310162910872286E-3</v>
       </c>
       <c r="L10" s="14"/>
       <c r="M10" s="13"/>
@@ -2773,30 +2797,30 @@
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <f t="shared" si="0"/>
-        <v>0.43333333333333335</v>
-      </c>
-      <c r="D11" s="19">
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="D11" s="18">
         <f>C11/25.4</f>
-        <v>1.7060367454068245E-2</v>
-      </c>
-      <c r="E11" s="19">
+        <v>8.5301837270341224E-3</v>
+      </c>
+      <c r="E11" s="18">
         <f t="shared" ref="E11:E17" si="2">$B$6-($B$1-C11)*$C$5</f>
-        <v>0.20939001427155168</v>
-      </c>
-      <c r="F11" s="20">
+        <v>0.10469500713577584</v>
+      </c>
+      <c r="F11" s="19">
         <f t="shared" si="1"/>
         <v>188.4510128443965</v>
       </c>
-      <c r="G11" s="20"/>
-      <c r="H11" s="22">
+      <c r="G11" s="19"/>
+      <c r="H11" s="21">
         <f>C11/SIN(RADIANS(60))</f>
-        <v>0.50037023329767572</v>
-      </c>
-      <c r="I11" s="22">
+        <v>0.25018511664883786</v>
+      </c>
+      <c r="I11" s="21">
         <f t="shared" ref="I11:I27" si="3">0.5*(H11*H11-H10*H10)*TAN(RADIANS(60))</f>
-        <v>0.15177897076696162</v>
+        <v>3.7944742691740405E-2</v>
       </c>
       <c r="L11" s="14"/>
       <c r="M11" s="13"/>
@@ -2808,30 +2832,30 @@
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="17">
         <f>$B$1*SQRT(B12)/SQRT($B$2-1)</f>
-        <v>0.61282587702834124</v>
-      </c>
-      <c r="D12" s="19">
+        <v>0.30641293851417062</v>
+      </c>
+      <c r="D12" s="18">
         <f t="shared" ref="D12:D27" si="4">C12/25.4</f>
-        <v>2.4127003032611862E-2</v>
-      </c>
-      <c r="E12" s="19">
+        <v>1.2063501516305931E-2</v>
+      </c>
+      <c r="E12" s="18">
         <f t="shared" si="2"/>
-        <v>0.29308876197825456</v>
-      </c>
-      <c r="F12" s="20">
+        <v>0.14654438098912728</v>
+      </c>
+      <c r="F12" s="19">
         <f t="shared" si="1"/>
         <v>263.77988578042908</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="22">
+      <c r="G12" s="19"/>
+      <c r="H12" s="21">
         <f t="shared" ref="H12:H27" si="5">C12/SIN(RADIANS(60))</f>
-        <v>0.70763037013736263</v>
-      </c>
-      <c r="I12" s="22">
+        <v>0.35381518506868131</v>
+      </c>
+      <c r="I12" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565942</v>
+        <v>5.4206775273914855E-2</v>
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="13"/>
@@ -2843,30 +2867,30 @@
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="17">
         <f t="shared" si="0"/>
-        <v>0.75055534994651341</v>
-      </c>
-      <c r="D13" s="19">
+        <v>0.3752776749732567</v>
+      </c>
+      <c r="D13" s="18">
         <f t="shared" si="4"/>
-        <v>2.9549423226240688E-2</v>
-      </c>
-      <c r="E13" s="19">
+        <v>1.4774711613120344E-2</v>
+      </c>
+      <c r="E13" s="18">
         <f t="shared" si="2"/>
-        <v>0.3573130699536497</v>
-      </c>
-      <c r="F13" s="20">
+        <v>0.17865653497682485</v>
+      </c>
+      <c r="F13" s="19">
         <f t="shared" si="1"/>
         <v>321.58176295828474</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="22">
+      <c r="G13" s="19"/>
+      <c r="H13" s="21">
         <f t="shared" si="5"/>
-        <v>0.86666666666666659</v>
-      </c>
-      <c r="I13" s="22">
+        <v>0.43333333333333329</v>
+      </c>
+      <c r="I13" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565917</v>
+        <v>5.4206775273914792E-2</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2876,30 +2900,30 @@
       <c r="B14" s="6">
         <v>4</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <f t="shared" si="0"/>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="D14" s="19">
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="D14" s="18">
         <f t="shared" si="4"/>
-        <v>3.4120734908136489E-2</v>
-      </c>
-      <c r="E14" s="19">
+        <v>1.7060367454068245E-2</v>
+      </c>
+      <c r="E14" s="18">
         <f t="shared" si="2"/>
-        <v>0.41145666613871773</v>
-      </c>
-      <c r="F14" s="20">
+        <v>0.20572833306935887</v>
+      </c>
+      <c r="F14" s="19">
         <f t="shared" si="1"/>
         <v>370.31099952484595</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="22">
+      <c r="G14" s="19"/>
+      <c r="H14" s="21">
         <f t="shared" si="5"/>
-        <v>1.0007404665953514</v>
-      </c>
-      <c r="I14" s="22">
+        <v>0.50037023329767572</v>
+      </c>
+      <c r="I14" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565967</v>
+        <v>5.4206775273914917E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2909,30 +2933,30 @@
       <c r="B15" s="6">
         <v>5</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="17">
         <f t="shared" si="0"/>
-        <v>0.96896279024990895</v>
-      </c>
-      <c r="D15" s="19">
+        <v>0.48448139512495447</v>
+      </c>
+      <c r="D15" s="18">
         <f t="shared" si="4"/>
-        <v>3.8148141348421614E-2</v>
-      </c>
-      <c r="E15" s="19">
+        <v>1.9074070674210807E-2</v>
+      </c>
+      <c r="E15" s="18">
         <f t="shared" si="2"/>
-        <v>0.45915813196515376</v>
-      </c>
-      <c r="F15" s="20">
+        <v>0.22957906598257688</v>
+      </c>
+      <c r="F15" s="19">
         <f t="shared" si="1"/>
         <v>413.24231876863837</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="22">
+      <c r="G15" s="19"/>
+      <c r="H15" s="21">
         <f t="shared" si="5"/>
-        <v>1.1188618555710317</v>
-      </c>
-      <c r="I15" s="22">
+        <v>0.55943092778551584</v>
+      </c>
+      <c r="I15" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565956</v>
+        <v>5.4206775273914889E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2942,30 +2966,30 @@
       <c r="B16" s="6">
         <v>6</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="17">
         <f t="shared" si="0"/>
-        <v>1.0614455552060438</v>
-      </c>
-      <c r="D16" s="19">
+        <v>0.53072277760302189</v>
+      </c>
+      <c r="D16" s="18">
         <f t="shared" si="4"/>
-        <v>4.1789195086852117E-2</v>
-      </c>
-      <c r="E16" s="19">
+        <v>2.0894597543426058E-2</v>
+      </c>
+      <c r="E16" s="18">
         <f t="shared" si="2"/>
-        <v>0.50228355351154819</v>
-      </c>
-      <c r="F16" s="20">
+        <v>0.25114177675577409</v>
+      </c>
+      <c r="F16" s="19">
         <f t="shared" si="1"/>
         <v>452.05519816039339</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="22">
+      <c r="H16" s="21">
         <f t="shared" si="5"/>
-        <v>1.2256517540566825</v>
-      </c>
-      <c r="I16" s="22">
+        <v>0.61282587702834124</v>
+      </c>
+      <c r="I16" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565936</v>
+        <v>5.4206775273914841E-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2975,29 +2999,29 @@
       <c r="B17" s="6">
         <v>7</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="17">
         <f t="shared" si="0"/>
-        <v>1.146492234794656</v>
-      </c>
-      <c r="D17" s="19">
+        <v>0.573246117397328</v>
+      </c>
+      <c r="D17" s="18">
         <f t="shared" si="4"/>
-        <v>4.513748955884473E-2</v>
-      </c>
-      <c r="E17" s="19">
+        <v>2.2568744779422365E-2</v>
+      </c>
+      <c r="E17" s="18">
         <f t="shared" si="2"/>
-        <v>0.54194147150437244</v>
-      </c>
-      <c r="F17" s="20">
+        <v>0.27097073575218622</v>
+      </c>
+      <c r="F17" s="19">
         <f t="shared" si="1"/>
         <v>487.7473243539352</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="21">
         <f t="shared" si="5"/>
-        <v>1.3238552007650206</v>
-      </c>
-      <c r="I17" s="22">
+        <v>0.66192760038251031</v>
+      </c>
+      <c r="I17" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565936</v>
+        <v>5.4206775273914841E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3007,29 +3031,29 @@
       <c r="B18" s="6">
         <v>8</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="17">
         <f t="shared" ref="C18:C27" si="6">$B$1*SQRT(B18)/SQRT($B$2-1)</f>
-        <v>1.2256517540566825</v>
-      </c>
-      <c r="D18" s="19">
+        <v>0.61282587702834124</v>
+      </c>
+      <c r="D18" s="18">
         <f t="shared" si="4"/>
-        <v>4.8254006065223724E-2</v>
-      </c>
-      <c r="E18" s="19">
+        <v>2.4127003032611862E-2</v>
+      </c>
+      <c r="E18" s="18">
         <f t="shared" ref="E18:E20" si="7">$B$6-($B$1-C18)*$C$5</f>
-        <v>0.57885416155212344</v>
-      </c>
-      <c r="F18" s="20">
+        <v>0.28942708077606172</v>
+      </c>
+      <c r="F18" s="19">
         <f t="shared" ref="F18:F27" si="8">$B$7/$B$3*E18</f>
         <v>520.96874539691112</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="21">
         <f t="shared" si="5"/>
-        <v>1.4152607402747253</v>
-      </c>
-      <c r="I18" s="22">
+        <v>0.70763037013736263</v>
+      </c>
+      <c r="I18" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565936</v>
+        <v>5.4206775273914841E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3039,29 +3063,29 @@
       <c r="B19" s="6">
         <v>9</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="17">
         <f t="shared" si="6"/>
-        <v>1.3</v>
-      </c>
-      <c r="D19" s="19">
+        <v>0.65</v>
+      </c>
+      <c r="D19" s="18">
         <f t="shared" si="4"/>
-        <v>5.1181102362204731E-2</v>
-      </c>
-      <c r="E19" s="19">
+        <v>2.5590551181102365E-2</v>
+      </c>
+      <c r="E19" s="18">
         <f t="shared" si="7"/>
-        <v>0.61352331800588378</v>
-      </c>
-      <c r="F19" s="20">
+        <v>0.30676165900294189</v>
+      </c>
+      <c r="F19" s="19">
         <f t="shared" si="8"/>
         <v>552.17098620529543</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="21">
         <f t="shared" si="5"/>
-        <v>1.501110699893027</v>
-      </c>
-      <c r="I19" s="22">
+        <v>0.75055534994651352</v>
+      </c>
+      <c r="I19" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565917</v>
+        <v>5.4206775273914792E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3071,29 +3095,29 @@
       <c r="B20" s="6">
         <v>10</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="17">
         <f t="shared" si="6"/>
-        <v>1.3703203194062981</v>
-      </c>
-      <c r="D20" s="19">
+        <v>0.68516015970314903</v>
+      </c>
+      <c r="D20" s="18">
         <f t="shared" si="4"/>
-        <v>5.3949618874263708E-2</v>
-      </c>
-      <c r="E20" s="19">
+        <v>2.6974809437131854E-2</v>
+      </c>
+      <c r="E20" s="18">
         <f t="shared" si="7"/>
-        <v>0.64631422146894613</v>
-      </c>
-      <c r="F20" s="20">
+        <v>0.32315711073447306</v>
+      </c>
+      <c r="F20" s="19">
         <f t="shared" si="8"/>
         <v>581.68279932205155</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="21">
         <f t="shared" si="5"/>
-        <v>1.5823096105704804</v>
-      </c>
-      <c r="I20" s="22">
+        <v>0.79115480528524018</v>
+      </c>
+      <c r="I20" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109566072</v>
+        <v>5.4206775273915181E-2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3103,29 +3127,29 @@
       <c r="B21" s="6">
         <v>11</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="17">
         <f t="shared" si="6"/>
-        <v>1.4372040758206734</v>
-      </c>
-      <c r="D21" s="19">
+        <v>0.71860203791033672</v>
+      </c>
+      <c r="D21" s="18">
         <f t="shared" si="4"/>
-        <v>5.6582837630735176E-2</v>
-      </c>
-      <c r="E21" s="19">
+        <v>2.8291418815367588E-2</v>
+      </c>
+      <c r="E21" s="18">
         <f t="shared" ref="E21:E23" si="9">$B$6-($B$1-C21)*$C$5</f>
-        <v>0.6775026292911428</v>
-      </c>
-      <c r="F21" s="20">
+        <v>0.3387513146455714</v>
+      </c>
+      <c r="F21" s="19">
         <f t="shared" si="8"/>
         <v>609.75236636202851</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="21">
         <f t="shared" si="5"/>
-        <v>1.6595403201109864</v>
-      </c>
-      <c r="I21" s="22">
+        <v>0.8297701600554932</v>
+      </c>
+      <c r="I21" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565881</v>
+        <v>5.4206775273914702E-2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3135,29 +3159,29 @@
       <c r="B22" s="6">
         <v>12</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="17">
         <f t="shared" si="6"/>
-        <v>1.5011106998930268</v>
-      </c>
-      <c r="D22" s="19">
+        <v>0.75055534994651341</v>
+      </c>
+      <c r="D22" s="18">
         <f t="shared" si="4"/>
-        <v>5.9098846452481375E-2</v>
-      </c>
-      <c r="E22" s="19">
+        <v>2.9549423226240688E-2</v>
+      </c>
+      <c r="E22" s="18">
         <f t="shared" si="9"/>
-        <v>0.70730277750291382</v>
-      </c>
-      <c r="F22" s="20">
+        <v>0.35365138875145691</v>
+      </c>
+      <c r="F22" s="19">
         <f t="shared" si="8"/>
         <v>636.57249975262243</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="21">
         <f t="shared" si="5"/>
-        <v>1.7333333333333332</v>
-      </c>
-      <c r="I22" s="22">
+        <v>0.86666666666666659</v>
+      </c>
+      <c r="I22" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565803</v>
+        <v>5.4206775273914508E-2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3167,29 +3191,29 @@
       <c r="B23" s="6">
         <v>13</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="17">
         <f t="shared" si="6"/>
-        <v>1.5624055527010621</v>
-      </c>
-      <c r="D23" s="19">
+        <v>0.78120277635053104</v>
+      </c>
+      <c r="D23" s="18">
         <f t="shared" si="4"/>
-        <v>6.1512029633900088E-2</v>
-      </c>
-      <c r="E23" s="19">
+        <v>3.0756014816950044E-2</v>
+      </c>
+      <c r="E23" s="18">
         <f t="shared" si="9"/>
-        <v>0.73588503677278405</v>
-      </c>
-      <c r="F23" s="20">
+        <v>0.36794251838639203</v>
+      </c>
+      <c r="F23" s="19">
         <f t="shared" si="8"/>
         <v>662.29653309550565</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="21">
         <f t="shared" si="5"/>
-        <v>1.8041105328706486</v>
-      </c>
-      <c r="I23" s="22">
+        <v>0.9020552664353243</v>
+      </c>
+      <c r="I23" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109566072</v>
+        <v>5.4206775273915181E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3199,29 +3223,29 @@
       <c r="B24" s="6">
         <v>14</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="17">
         <f t="shared" si="6"/>
-        <v>1.6213848676020415</v>
-      </c>
-      <c r="D24" s="19">
+        <v>0.81069243380102074</v>
+      </c>
+      <c r="D24" s="18">
         <f t="shared" si="4"/>
-        <v>6.3834049905592188E-2</v>
-      </c>
-      <c r="E24" s="19">
+        <v>3.1917024952796094E-2</v>
+      </c>
+      <c r="E24" s="18">
         <f t="shared" ref="E24:E27" si="10">$B$6-($B$1-C24)*$C$5</f>
-        <v>0.76338754298384603</v>
-      </c>
-      <c r="F24" s="20">
+        <v>0.38169377149192302</v>
+      </c>
+      <c r="F24" s="19">
         <f t="shared" si="8"/>
         <v>687.04878868546143</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="21">
         <f t="shared" si="5"/>
-        <v>1.8722139795400488</v>
-      </c>
-      <c r="I24" s="22">
+        <v>0.93610698977002438</v>
+      </c>
+      <c r="I24" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565956</v>
+        <v>5.4206775273914889E-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3231,29 +3255,29 @@
       <c r="B25" s="6">
         <v>15</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="17">
         <f t="shared" si="6"/>
-        <v>1.6782927833565475</v>
-      </c>
-      <c r="D25" s="19">
+        <v>0.83914639167827376</v>
+      </c>
+      <c r="D25" s="18">
         <f t="shared" si="4"/>
-        <v>6.6074519029785339E-2</v>
-      </c>
-      <c r="E25" s="19">
+        <v>3.303725951489267E-2</v>
+      </c>
+      <c r="E25" s="18">
         <f t="shared" si="10"/>
-        <v>0.7899241399098117</v>
-      </c>
-      <c r="F25" s="20">
+        <v>0.39496206995490585</v>
+      </c>
+      <c r="F25" s="19">
         <f t="shared" si="8"/>
         <v>710.93172591883058</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="21">
         <f t="shared" si="5"/>
-        <v>1.9379255804998181</v>
-      </c>
-      <c r="I25" s="22">
+        <v>0.96896279024990906</v>
+      </c>
+      <c r="I25" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565956</v>
+        <v>5.4206775273914889E-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3263,29 +3287,29 @@
       <c r="B26" s="6">
         <v>16</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="17">
         <f t="shared" si="6"/>
-        <v>1.7333333333333334</v>
-      </c>
-      <c r="D26" s="19">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="D26" s="18">
         <f t="shared" si="4"/>
-        <v>6.8241469816272979E-2</v>
-      </c>
-      <c r="E26" s="19">
+        <v>3.4120734908136489E-2</v>
+      </c>
+      <c r="E26" s="18">
         <f t="shared" si="10"/>
-        <v>0.81558996987304977</v>
-      </c>
-      <c r="F26" s="20">
+        <v>0.40779498493652488</v>
+      </c>
+      <c r="F26" s="19">
         <f t="shared" si="8"/>
         <v>734.03097288574475</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="21">
         <f t="shared" si="5"/>
-        <v>2.0014809331907029</v>
-      </c>
-      <c r="I26" s="22">
+        <v>1.0007404665953514</v>
+      </c>
+      <c r="I26" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565881</v>
+        <v>5.4206775273914702E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3295,33 +3319,34 @@
       <c r="B27" s="6">
         <v>17</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="17">
         <f t="shared" si="6"/>
-        <v>1.7866791044343195</v>
-      </c>
-      <c r="D27" s="19">
+        <v>0.89333955221715977</v>
+      </c>
+      <c r="D27" s="18">
         <f t="shared" si="4"/>
-        <v>7.0341697024973213E-2</v>
-      </c>
-      <c r="E27" s="19">
+        <v>3.5170848512486606E-2</v>
+      </c>
+      <c r="E27" s="18">
         <f t="shared" si="10"/>
-        <v>0.84046551146762327</v>
-      </c>
-      <c r="F27" s="20">
+        <v>0.42023275573381164</v>
+      </c>
+      <c r="F27" s="19">
         <f t="shared" si="8"/>
         <v>756.41896032086095</v>
       </c>
-      <c r="H27" s="22">
+      <c r="H27" s="21">
         <f t="shared" si="5"/>
-        <v>2.0630793238012677</v>
-      </c>
-      <c r="I27" s="22">
+        <v>1.0315396619006338</v>
+      </c>
+      <c r="I27" s="21">
         <f t="shared" si="3"/>
-        <v>0.21682710109565842</v>
+        <v>5.4206775273914605E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
modify pulse generation mode for stepper
modify pulse generation mode for stepper(invert is) to use dm556 stepper driver instead drv8825 for z axis. DM556 need high to low pulses, drv8825 need low to high
</commit_message>
<xml_diff>
--- a/feed_tab.xlsx
+++ b/feed_tab.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STM32\project\efeed\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13550" windowHeight="7890" tabRatio="286"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13548" windowHeight="7896" tabRatio="286"/>
   </bookViews>
   <sheets>
     <sheet name="feed" sheetId="1" r:id="rId1"/>
     <sheet name="infeed" sheetId="5" r:id="rId2"/>
     <sheet name="ramp up" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="114">
   <si>
     <t>"</t>
   </si>
@@ -898,7 +893,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -909,24 +904,24 @@
   <dimension ref="A1:Y161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" customWidth="1"/>
-    <col min="9" max="9" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.6328125" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>24</v>
       </c>
@@ -944,7 +939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -973,7 +968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1018,7 +1013,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>45</v>
       </c>
@@ -1051,7 +1046,7 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>1800</v>
       </c>
@@ -1146,7 +1141,7 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
         <v>2</v>
       </c>
@@ -1191,45 +1186,41 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B10" s="26" t="str">
-        <f t="shared" ref="B10:B41" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D10,"tpi"),25.4/A10,A10))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x04800000</v>
+        <f t="shared" ref="B10" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D10,"tpi"),25.4/A10,A10))*$B$1,0),8)),"0x00000000")</f>
+        <v>0x038B162C</v>
       </c>
       <c r="C10" s="26">
         <v>0</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E10" s="26">
         <v>0</v>
       </c>
-      <c r="F10" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>13</v>
-      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x04800000, 0, "2.00", "mm", 0, "1.26", ".050", 1 },</v>
+        <v>{ 0x038B162C, 0, "10", "tpi", 0, "", "", 0 },</v>
       </c>
       <c r="J10" s="4"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
         <v>2</v>
       </c>
       <c r="B11" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B10:B41" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D11,"tpi"),25.4/A11,A11))*$B$1,0),8)),"0x00000000")</f>
         <v>0x04800000</v>
       </c>
       <c r="C11" s="26">
@@ -1257,12 +1248,12 @@
       <c r="J11" s="4"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
         <v>1.5</v>
       </c>
       <c r="B12" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x06000000</v>
       </c>
       <c r="C12" s="26">
@@ -1294,12 +1285,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
         <v>1</v>
       </c>
       <c r="B13" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x09000000</v>
       </c>
       <c r="C13" s="26">
@@ -1332,12 +1323,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x00000000</v>
       </c>
       <c r="C14" s="26">
@@ -1361,12 +1352,12 @@
       <c r="J14" s="4"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="26">
         <v>0.2</v>
       </c>
       <c r="B15" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x2D000000</v>
       </c>
       <c r="C15" s="26">
@@ -1390,12 +1381,12 @@
       <c r="J15" s="4"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="26">
         <v>0.18</v>
       </c>
       <c r="B16" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x32000000</v>
       </c>
       <c r="C16" s="26">
@@ -1419,12 +1410,12 @@
       <c r="J16" s="4"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="26">
         <v>0.15</v>
       </c>
       <c r="B17" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x3C000000</v>
       </c>
       <c r="C17" s="26">
@@ -1448,12 +1439,12 @@
       <c r="J17" s="4"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>0.12</v>
       </c>
       <c r="B18" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x4B000000</v>
       </c>
       <c r="C18" s="26">
@@ -1477,12 +1468,12 @@
       <c r="J18" s="4"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>0.09</v>
       </c>
       <c r="B19" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x64000000</v>
       </c>
       <c r="C19" s="26">
@@ -1506,12 +1497,12 @@
       <c r="J19" s="4"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="26">
         <v>0.06</v>
       </c>
       <c r="B20" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x96000000</v>
       </c>
       <c r="C20" s="26">
@@ -1535,12 +1526,12 @@
       <c r="J20" s="4"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="26">
         <v>0.04</v>
       </c>
       <c r="B21" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0xE1000000</v>
       </c>
       <c r="C21" s="26">
@@ -1564,12 +1555,12 @@
       <c r="J21" s="4"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x00000000</v>
       </c>
       <c r="C22" s="26">
@@ -1593,12 +1584,12 @@
       <c r="J22" s="4"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x00000000</v>
       </c>
       <c r="C23" s="26">
@@ -1622,12 +1613,12 @@
       <c r="J23" s="4"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="26">
         <v>1.25</v>
       </c>
       <c r="B24" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x07333333</v>
       </c>
       <c r="C24" s="26">
@@ -1655,12 +1646,12 @@
       <c r="J24" s="4"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="26">
         <v>1.75</v>
       </c>
       <c r="B25" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x05249249</v>
       </c>
       <c r="C25" s="26">
@@ -1688,12 +1679,12 @@
       <c r="J25" s="4"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A26" s="26">
         <v>2</v>
       </c>
       <c r="B26" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x04800000</v>
       </c>
       <c r="C26" s="26">
@@ -1721,12 +1712,12 @@
       <c r="J26" s="4"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="26">
         <v>0.5</v>
       </c>
       <c r="B27" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x12000000</v>
       </c>
       <c r="C27" s="26">
@@ -1754,12 +1745,12 @@
       <c r="J27" s="4"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="26">
         <v>0.75</v>
       </c>
       <c r="B28" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x0C000000</v>
       </c>
       <c r="C28" s="26">
@@ -1787,12 +1778,12 @@
       <c r="J28" s="4"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x00000000</v>
       </c>
       <c r="C29" s="26">
@@ -1816,12 +1807,12 @@
       <c r="J29" s="4"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x00000000</v>
       </c>
       <c r="C30" s="26">
@@ -1845,12 +1836,12 @@
       <c r="J30" s="4"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="26">
         <v>27</v>
       </c>
       <c r="B31" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x09912244</v>
       </c>
       <c r="C31" s="26">
@@ -1874,12 +1865,12 @@
       <c r="J31" s="4"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="26">
         <v>26</v>
       </c>
       <c r="B32" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x09366CD9</v>
       </c>
       <c r="C32" s="26">
@@ -1903,12 +1894,12 @@
       <c r="J32" s="4"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="26">
         <v>24</v>
       </c>
       <c r="B33" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x08810204</v>
       </c>
       <c r="C33" s="26">
@@ -1932,12 +1923,12 @@
       <c r="J33" s="4"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="26">
         <v>22</v>
       </c>
       <c r="B34" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x07CB972E</v>
       </c>
       <c r="C34" s="26">
@@ -1961,12 +1952,12 @@
       <c r="J34" s="4"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="26">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x07162C58</v>
       </c>
       <c r="C35" s="26">
@@ -1990,12 +1981,12 @@
       <c r="J35" s="4"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="26">
         <v>19</v>
       </c>
       <c r="B36" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x06BB76ED</v>
       </c>
       <c r="C36" s="26">
@@ -2013,18 +2004,18 @@
         <v>0</v>
       </c>
       <c r="I36" s="25" t="str">
-        <f t="shared" ref="I36:I41" si="2">$A$2&amp;B36&amp;$C$2&amp;C36&amp;$D$2&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D36&amp;$E$2&amp;E36&amp;$D$2&amp;F36&amp;$G$2&amp;G36&amp;$E$2&amp;H36&amp;$B$2</f>
+        <f t="shared" ref="I36:I41" si="3">$A$2&amp;B36&amp;$C$2&amp;C36&amp;$D$2&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D36&amp;$E$2&amp;E36&amp;$D$2&amp;F36&amp;$G$2&amp;G36&amp;$E$2&amp;H36&amp;$B$2</f>
         <v>{ 0x06BB76ED, 0, "19", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J36" s="4"/>
       <c r="Q36" s="7"/>
     </row>
-    <row r="37" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="26">
         <v>18</v>
       </c>
       <c r="B37" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x0660C183</v>
       </c>
       <c r="C37" s="26">
@@ -2042,18 +2033,18 @@
         <v>0</v>
       </c>
       <c r="I37" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>{ 0x0660C183, 0, "18", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J37" s="4"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="26">
         <v>16</v>
       </c>
       <c r="B38" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x05AB56AD</v>
       </c>
       <c r="C38" s="26">
@@ -2071,18 +2062,18 @@
         <v>0</v>
       </c>
       <c r="I38" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>{ 0x05AB56AD, 0, "16", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J38" s="4"/>
       <c r="Q38" s="7"/>
     </row>
-    <row r="39" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="26">
         <v>14</v>
       </c>
       <c r="B39" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x04F5EBD7</v>
       </c>
       <c r="C39" s="26">
@@ -2100,18 +2091,18 @@
         <v>0</v>
       </c>
       <c r="I39" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>{ 0x04F5EBD7, 0, "14", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J39" s="4"/>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="26">
         <v>12</v>
       </c>
       <c r="B40" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x04408102</v>
       </c>
       <c r="C40" s="26">
@@ -2129,18 +2120,18 @@
         <v>0</v>
       </c>
       <c r="I40" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>{ 0x04408102, 0, "12", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J40" s="4"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B41" s="26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0x00000000</v>
       </c>
       <c r="C41" s="26">
@@ -2158,13 +2149,13 @@
         <v>0</v>
       </c>
       <c r="I41" s="25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>{ 0x00000000, 0, "..", "up", 30, "", "", 0 },</v>
       </c>
       <c r="J41" s="4"/>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="C42" s="4"/>
       <c r="E42" s="4"/>
@@ -2174,7 +2165,7 @@
       <c r="J42" s="4"/>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="6"/>
       <c r="C43" s="4"/>
@@ -2238,123 +2229,123 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="E64"/>
     </row>
-    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="E68"/>
     </row>
-    <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="E69"/>
     </row>
-    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="E70"/>
     </row>
-    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="E71"/>
     </row>
-    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="E72"/>
     </row>
-    <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="E73"/>
     </row>
-    <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="E74"/>
     </row>
-    <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="E75"/>
     </row>
-    <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="E76"/>
     </row>
-    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="E77"/>
     </row>
-    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="E78"/>
     </row>
-    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="E79"/>
     </row>
-    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="E80"/>
     </row>
-    <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="E81"/>
     </row>
-    <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="E82"/>
     </row>
-    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="E84"/>
     </row>
-    <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="E86"/>
     </row>
-    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="E88"/>
     </row>
@@ -2599,20 +2590,20 @@
       <selection activeCell="F10" sqref="F10:F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>107</v>
       </c>
@@ -2649,7 +2640,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>109</v>
       </c>
@@ -2699,7 +2690,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>104</v>
       </c>
@@ -2731,7 +2722,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>105</v>
       </c>
@@ -2756,7 +2747,7 @@
       <c r="L9" s="14"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -2790,7 +2781,7 @@
       <c r="L10" s="14"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -2825,7 +2816,7 @@
       <c r="L11" s="14"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>3</v>
       </c>
@@ -3358,12 +3349,12 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>30</v>
       </c>
@@ -3371,7 +3362,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>21.888000000000002</v>
       </c>
@@ -3379,7 +3370,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>17.024000000000001</v>
       </c>
@@ -3387,7 +3378,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>14.40492308</v>
       </c>
@@ -3395,7 +3386,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>12.710226240000001</v>
       </c>
@@ -3403,7 +3394,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>11.499728510000001</v>
       </c>
@@ -3411,7 +3402,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>10.57975023</v>
       </c>
@@ -3419,7 +3410,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>9.8501122799999994</v>
       </c>

</xml_diff>

<commit_message>
refactor code add timer2 as async
</commit_message>
<xml_diff>
--- a/feed_tab.xlsx
+++ b/feed_tab.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STM32\project\efeed\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13548" windowHeight="7896" tabRatio="286"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13550" windowHeight="7900" tabRatio="286"/>
   </bookViews>
   <sheets>
     <sheet name="feed" sheetId="1" r:id="rId1"/>
     <sheet name="infeed" sheetId="5" r:id="rId2"/>
     <sheet name="ramp up" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -893,7 +898,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -904,24 +909,24 @@
   <dimension ref="A1:Y161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
-    <col min="9" max="9" width="42.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" customWidth="1"/>
+    <col min="9" max="9" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>24</v>
       </c>
@@ -939,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -968,13 +973,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="K3">
         <f>$A$6*2/($B$6/$C$6*A9)</f>
-        <v>4.5</v>
+        <v>150</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>5</v>
@@ -1000,11 +1005,11 @@
       <c r="H4" s="6"/>
       <c r="J4">
         <f>A6*2*C6/A9/B6*B1</f>
-        <v>75497472</v>
+        <v>2516582400</v>
       </c>
       <c r="K4">
         <f>ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0)</f>
-        <v>75497472</v>
+        <v>2516582400</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>7</v>
@@ -1013,7 +1018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>45</v>
       </c>
@@ -1046,7 +1051,7 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>1800</v>
       </c>
@@ -1054,7 +1059,7 @@
         <v>400</v>
       </c>
       <c r="C6" s="16">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D6" s="16">
         <v>400</v>
@@ -1067,7 +1072,7 @@
       <c r="H6" s="6"/>
       <c r="J6" s="13" t="str">
         <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0),9)),"0x000000000")</f>
-        <v>0x004800000</v>
+        <v>0x096000000</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>11</v>
@@ -1141,13 +1146,13 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
-        <v>2</v>
+        <v>0.09</v>
       </c>
       <c r="B9" s="26" t="str">
         <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D9,"tpi"),25.4/A9,A9))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x04800000</v>
+        <v>0x96000000</v>
       </c>
       <c r="C9" s="26">
         <v>0</v>
@@ -1169,7 +1174,7 @@
       </c>
       <c r="I9" s="25" t="str">
         <f t="shared" ref="I9:I35" si="0">$A$2&amp;B9&amp;$C$2&amp;C9&amp;$D$2&amp;SUBSTITUTE(TEXT(A9,IF(EXACT(D9,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D9&amp;$E$2&amp;E9&amp;$D$2&amp;F9&amp;$G$2&amp;G9&amp;$E$2&amp;H9&amp;$B$2</f>
-        <v>{ 0x04800000, 0, "2.00", "mm", 0, "1.26", ".050", 0 },</v>
+        <v>{ 0x96000000, 0, "0.09", "mm", 0, "1.26", ".050", 0 },</v>
       </c>
       <c r="J9" s="4"/>
       <c r="P9" s="6" t="s">
@@ -1186,19 +1191,19 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
-        <v>10</v>
+        <v>0.15</v>
       </c>
       <c r="B10" s="26" t="str">
         <f t="shared" ref="B10" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D10,"tpi"),25.4/A10,A10))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x038B162C</v>
+        <v>0x5A000000</v>
       </c>
       <c r="C10" s="26">
         <v>0</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E10" s="26">
         <v>0</v>
@@ -1210,18 +1215,18 @@
       </c>
       <c r="I10" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x038B162C, 0, "10", "tpi", 0, "", "", 0 },</v>
+        <v>{ 0x5A000000, 0, "0.15", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J10" s="4"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B11" s="26" t="str">
-        <f t="shared" ref="B10:B41" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D11,"tpi"),25.4/A11,A11))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x04800000</v>
+        <f t="shared" ref="B11:B41" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D11,"tpi"),25.4/A11,A11))*$B$1,0),8)),"0x00000000")</f>
+        <v>0x09000000</v>
       </c>
       <c r="C11" s="26">
         <v>0</v>
@@ -1243,18 +1248,18 @@
       </c>
       <c r="I11" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x04800000, 0, "2.00", "mm", 0, "1.26", ".050", 2 },</v>
+        <v>{ 0x09000000, 0, "1.50", "mm", 0, "1.26", ".050", 2 },</v>
       </c>
       <c r="J11" s="4"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B12" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x06000000</v>
+        <v>0x0D800000</v>
       </c>
       <c r="C12" s="26">
         <v>0</v>
@@ -1276,7 +1281,7 @@
       </c>
       <c r="I12" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x06000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
+        <v>{ 0x0D800000, 0, "1.00", "mm", 0, ".95", ".037", 0 },</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>19</v>
@@ -1285,19 +1290,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B13" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x09000000</v>
+        <v>0x0550A142</v>
       </c>
       <c r="C13" s="26">
         <v>0</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E13" s="26">
         <v>0</v>
@@ -1313,7 +1318,7 @@
       </c>
       <c r="I13" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x09000000, 0, "1.00", "mm", 0, ".65", ".026", 0 },</v>
+        <v>{ 0x0550A142, 0, "10", "tpi", 0, ".65", ".026", 0 },</v>
       </c>
       <c r="J13" s="4"/>
       <c r="P13" s="6" t="s">
@@ -1323,7 +1328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>26</v>
       </c>
@@ -1352,13 +1357,13 @@
       <c r="J14" s="4"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="26">
         <v>0.2</v>
       </c>
       <c r="B15" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x2D000000</v>
+        <v>0x43800000</v>
       </c>
       <c r="C15" s="26">
         <v>0</v>
@@ -1376,18 +1381,18 @@
       </c>
       <c r="I15" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x2D000000, 0, "0.20", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x43800000, 0, "0.20", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J15" s="4"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="26">
         <v>0.18</v>
       </c>
       <c r="B16" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x32000000</v>
+        <v>0x4B000000</v>
       </c>
       <c r="C16" s="26">
         <v>0</v>
@@ -1405,18 +1410,18 @@
       </c>
       <c r="I16" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x32000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x4B000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J16" s="4"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="26">
         <v>0.15</v>
       </c>
       <c r="B17" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x3C000000</v>
+        <v>0x5A000000</v>
       </c>
       <c r="C17" s="26">
         <v>0</v>
@@ -1434,18 +1439,18 @@
       </c>
       <c r="I17" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x3C000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x5A000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J17" s="4"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>0.12</v>
       </c>
       <c r="B18" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x4B000000</v>
+        <v>0x70800000</v>
       </c>
       <c r="C18" s="26">
         <v>0</v>
@@ -1463,18 +1468,18 @@
       </c>
       <c r="I18" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x4B000000, 0, "0.12", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x70800000, 0, "0.12", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J18" s="4"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>0.09</v>
       </c>
       <c r="B19" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x64000000</v>
+        <v>0x96000000</v>
       </c>
       <c r="C19" s="26">
         <v>0</v>
@@ -1492,18 +1497,18 @@
       </c>
       <c r="I19" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x64000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x96000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J19" s="4"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="26">
         <v>0.06</v>
       </c>
       <c r="B20" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x96000000</v>
+        <v>0xE1000000</v>
       </c>
       <c r="C20" s="26">
         <v>0</v>
@@ -1521,18 +1526,18 @@
       </c>
       <c r="I20" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x96000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
+        <v>{ 0xE1000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J20" s="4"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="26">
         <v>0.04</v>
       </c>
       <c r="B21" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0xE1000000</v>
+        <v>0x00000000</v>
       </c>
       <c r="C21" s="26">
         <v>0</v>
@@ -1550,12 +1555,12 @@
       </c>
       <c r="I21" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0xE1000000, 0, "0.04", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x00000000, 0, "0.04", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J21" s="4"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>24</v>
       </c>
@@ -1584,7 +1589,7 @@
       <c r="J22" s="4"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>37</v>
       </c>
@@ -1613,13 +1618,13 @@
       <c r="J23" s="4"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="26">
         <v>1.25</v>
       </c>
       <c r="B24" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x07333333</v>
+        <v>0x0ACCCCCC</v>
       </c>
       <c r="C24" s="26">
         <v>0</v>
@@ -1641,18 +1646,18 @@
       </c>
       <c r="I24" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x07333333, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
+        <v>{ 0x0ACCCCCC, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
       </c>
       <c r="J24" s="4"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="26">
         <v>1.75</v>
       </c>
       <c r="B25" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x05249249</v>
+        <v>0x07B6DB6D</v>
       </c>
       <c r="C25" s="26">
         <v>0</v>
@@ -1674,18 +1679,18 @@
       </c>
       <c r="I25" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x05249249, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
+        <v>{ 0x07B6DB6D, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
       </c>
       <c r="J25" s="4"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="26">
         <v>2</v>
       </c>
       <c r="B26" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x04800000</v>
+        <v>0x06C00000</v>
       </c>
       <c r="C26" s="26">
         <v>0</v>
@@ -1707,18 +1712,18 @@
       </c>
       <c r="I26" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x04800000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
+        <v>{ 0x06C00000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
       </c>
       <c r="J26" s="4"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="26">
         <v>0.5</v>
       </c>
       <c r="B27" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x12000000</v>
+        <v>0x1B000000</v>
       </c>
       <c r="C27" s="26">
         <v>0</v>
@@ -1740,18 +1745,18 @@
       </c>
       <c r="I27" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x12000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
+        <v>{ 0x1B000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
       </c>
       <c r="J27" s="4"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="26">
         <v>0.75</v>
       </c>
       <c r="B28" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0C000000</v>
+        <v>0x12000000</v>
       </c>
       <c r="C28" s="26">
         <v>0</v>
@@ -1773,12 +1778,12 @@
       </c>
       <c r="I28" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0C000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
+        <v>{ 0x12000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
       </c>
       <c r="J28" s="4"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
         <v>24</v>
       </c>
@@ -1807,7 +1812,7 @@
       <c r="J29" s="4"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>37</v>
       </c>
@@ -1836,13 +1841,13 @@
       <c r="J30" s="4"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="26">
         <v>27</v>
       </c>
       <c r="B31" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x09912244</v>
+        <v>0x0E59B366</v>
       </c>
       <c r="C31" s="26">
         <v>0</v>
@@ -1860,18 +1865,18 @@
       </c>
       <c r="I31" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x09912244, 0, "27", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0E59B366, 0, "27", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J31" s="4"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="26">
         <v>26</v>
       </c>
       <c r="B32" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x09366CD9</v>
+        <v>0x0DD1A346</v>
       </c>
       <c r="C32" s="26">
         <v>0</v>
@@ -1889,18 +1894,18 @@
       </c>
       <c r="I32" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x09366CD9, 0, "26", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0DD1A346, 0, "26", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J32" s="4"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="26">
         <v>24</v>
       </c>
       <c r="B33" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x08810204</v>
+        <v>0x0CC18306</v>
       </c>
       <c r="C33" s="26">
         <v>0</v>
@@ -1918,18 +1923,18 @@
       </c>
       <c r="I33" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x08810204, 0, "24", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0CC18306, 0, "24", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J33" s="4"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="26">
         <v>22</v>
       </c>
       <c r="B34" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x07CB972E</v>
+        <v>0x0BB162C5</v>
       </c>
       <c r="C34" s="26">
         <v>0</v>
@@ -1947,18 +1952,18 @@
       </c>
       <c r="I34" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x07CB972E, 0, "22", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0BB162C5, 0, "22", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J34" s="4"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="26">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x07162C58</v>
+        <v>0x0AA14285</v>
       </c>
       <c r="C35" s="26">
         <v>0</v>
@@ -1976,18 +1981,18 @@
       </c>
       <c r="I35" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x07162C58, 0, "20", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0AA14285, 0, "20", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J35" s="4"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="26">
         <v>19</v>
       </c>
       <c r="B36" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x06BB76ED</v>
+        <v>0x0A193264</v>
       </c>
       <c r="C36" s="26">
         <v>0</v>
@@ -2005,18 +2010,18 @@
       </c>
       <c r="I36" s="25" t="str">
         <f t="shared" ref="I36:I41" si="3">$A$2&amp;B36&amp;$C$2&amp;C36&amp;$D$2&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D36&amp;$E$2&amp;E36&amp;$D$2&amp;F36&amp;$G$2&amp;G36&amp;$E$2&amp;H36&amp;$B$2</f>
-        <v>{ 0x06BB76ED, 0, "19", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0A193264, 0, "19", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J36" s="4"/>
       <c r="Q36" s="7"/>
     </row>
-    <row r="37" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="26">
         <v>18</v>
       </c>
       <c r="B37" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0660C183</v>
+        <v>0x09912244</v>
       </c>
       <c r="C37" s="26">
         <v>0</v>
@@ -2034,18 +2039,18 @@
       </c>
       <c r="I37" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>{ 0x0660C183, 0, "18", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x09912244, 0, "18", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J37" s="4"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A38" s="26">
         <v>16</v>
       </c>
       <c r="B38" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x05AB56AD</v>
+        <v>0x08810204</v>
       </c>
       <c r="C38" s="26">
         <v>0</v>
@@ -2063,18 +2068,18 @@
       </c>
       <c r="I38" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>{ 0x05AB56AD, 0, "16", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x08810204, 0, "16", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J38" s="4"/>
       <c r="Q38" s="7"/>
     </row>
-    <row r="39" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A39" s="26">
         <v>14</v>
       </c>
       <c r="B39" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x04F5EBD7</v>
+        <v>0x0770E1C3</v>
       </c>
       <c r="C39" s="26">
         <v>0</v>
@@ -2092,18 +2097,18 @@
       </c>
       <c r="I39" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>{ 0x04F5EBD7, 0, "14", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0770E1C3, 0, "14", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J39" s="4"/>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A40" s="26">
         <v>12</v>
       </c>
       <c r="B40" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x04408102</v>
+        <v>0x0660C183</v>
       </c>
       <c r="C40" s="26">
         <v>0</v>
@@ -2121,12 +2126,12 @@
       </c>
       <c r="I40" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>{ 0x04408102, 0, "12", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0660C183, 0, "12", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J40" s="4"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
         <v>24</v>
       </c>
@@ -2155,7 +2160,7 @@
       <c r="J41" s="4"/>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="C42" s="4"/>
       <c r="E42" s="4"/>
@@ -2165,7 +2170,7 @@
       <c r="J42" s="4"/>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="13" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="6"/>
       <c r="C43" s="4"/>
@@ -2229,123 +2234,123 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="E64"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="E68"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="E69"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="E70"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="E71"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="E72"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="E73"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="E74"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="E75"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="E76"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="E77"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="E78"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="E79"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="E80"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="E81"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="E82"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="E84"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="E86"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="E88"/>
     </row>
@@ -2590,20 +2595,20 @@
       <selection activeCell="F10" sqref="F10:F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.77734375" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>107</v>
       </c>
@@ -2640,7 +2645,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>109</v>
       </c>
@@ -2690,7 +2695,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>104</v>
       </c>
@@ -2722,7 +2727,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="25" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>105</v>
       </c>
@@ -2747,7 +2752,7 @@
       <c r="L9" s="14"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -2781,7 +2786,7 @@
       <c r="L10" s="14"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -2816,7 +2821,7 @@
       <c r="L11" s="14"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>3</v>
       </c>
@@ -3349,12 +3354,12 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>30</v>
       </c>
@@ -3362,7 +3367,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>21.888000000000002</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>17.024000000000001</v>
       </c>
@@ -3378,7 +3383,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>14.40492308</v>
       </c>
@@ -3386,7 +3391,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>12.710226240000001</v>
       </c>
@@ -3394,7 +3399,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>11.499728510000001</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>10.57975023</v>
       </c>
@@ -3410,7 +3415,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>9.8501122799999994</v>
       </c>
@@ -3418,7 +3423,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>9.2531357780000008</v>
       </c>
@@ -3426,7 +3431,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8.7529662760000004</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8.3259923120000003</v>
       </c>
@@ -3442,7 +3447,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>7.9559482089999998</v>
       </c>
@@ -3450,7 +3455,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7.6312156289999997</v>
       </c>
@@ -3458,7 +3463,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>7.3432452279999998</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>7.085587501</v>
       </c>
@@ -3474,7 +3479,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>6.8532731560000002</v>
       </c>
@@ -3482,7 +3487,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>6.6424032129999997</v>
       </c>
@@ -3490,7 +3495,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>6.4498697869999999</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>6.2731610250000003</v>
       </c>
@@ -3506,7 +3511,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>6.1102217779999997</v>
       </c>
@@ -3514,7 +3519,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>5.9593521039999997</v>
       </c>
@@ -3522,7 +3527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>5.8191320549999999</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>5.688365042</v>
       </c>
@@ -3538,7 +3543,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>5.5660346110000001</v>
       </c>
@@ -3546,7 +3551,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>5.4512710110000002</v>
       </c>
@@ -3554,7 +3559,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>5.3433250499999998</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>5.2415474299999998</v>
       </c>
@@ -3570,7 +3575,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>5.1453722480000001</v>
       </c>
@@ -3578,7 +3583,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>5.0543037130000004</v>
       </c>
@@ -3586,7 +3591,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>4.9679053590000004</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>4.8857912209999999</v>
       </c>
@@ -3602,7 +3607,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>4.807618561</v>
       </c>
@@ -3610,7 +3615,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>4.7330818389999996</v>
       </c>
@@ -3618,7 +3623,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>4.6619076760000002</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>4.5938506300000004</v>
       </c>

</xml_diff>

<commit_message>
invert motor Z levels for new stepper driver(556), add disable motor on reset, recalculate setup for 1,5 mm pich leadscrew, add 0.09mm/rev feed on top of the menu, fix few bugfixes
invert motor Z levels for new stepper driver(556), add disable motor on reset, recalculate setup for 1,5 mm pich leadscrew, add 0.09mm/rev feed on top of the menu, fix few bugfixes
</commit_message>
<xml_diff>
--- a/feed_tab.xlsx
+++ b/feed_tab.xlsx
@@ -893,7 +893,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -903,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -974,7 +974,7 @@
       <c r="H3" s="2"/>
       <c r="K3">
         <f>$A$6*2/($B$6/$C$6*A9)</f>
-        <v>4.5</v>
+        <v>225</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>5</v>
@@ -1000,11 +1000,11 @@
       <c r="H4" s="6"/>
       <c r="J4">
         <f>A6*2*C6/A9/B6*B1</f>
-        <v>75497472</v>
+        <v>3774873600</v>
       </c>
       <c r="K4">
         <f>ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0)</f>
-        <v>75497472</v>
+        <v>3774873600</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>7</v>
@@ -1054,7 +1054,7 @@
         <v>400</v>
       </c>
       <c r="C6" s="16">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D6" s="16">
         <v>400</v>
@@ -1067,7 +1067,7 @@
       <c r="H6" s="6"/>
       <c r="J6" s="13" t="str">
         <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0),9)),"0x000000000")</f>
-        <v>0x004800000</v>
+        <v>0x0E1000000</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>11</v>
@@ -1143,11 +1143,11 @@
     </row>
     <row r="9" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
-        <v>2</v>
+        <v>0.06</v>
       </c>
       <c r="B9" s="26" t="str">
         <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D9,"tpi"),25.4/A9,A9))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x04800000</v>
+        <v>0xE1000000</v>
       </c>
       <c r="C9" s="26">
         <v>0</v>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="I9" s="25" t="str">
         <f t="shared" ref="I9:I35" si="0">$A$2&amp;B9&amp;$C$2&amp;C9&amp;$D$2&amp;SUBSTITUTE(TEXT(A9,IF(EXACT(D9,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D9&amp;$E$2&amp;E9&amp;$D$2&amp;F9&amp;$G$2&amp;G9&amp;$E$2&amp;H9&amp;$B$2</f>
-        <v>{ 0x04800000, 0, "2.00", "mm", 0, "1.26", ".050", 0 },</v>
+        <v>{ 0xE1000000, 0, "0.06", "mm", 0, "1.26", ".050", 0 },</v>
       </c>
       <c r="J9" s="4"/>
       <c r="P9" s="6" t="s">
@@ -1188,17 +1188,17 @@
     </row>
     <row r="10" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
-        <v>10</v>
+        <v>0.09</v>
       </c>
       <c r="B10" s="26" t="str">
         <f t="shared" ref="B10" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D10,"tpi"),25.4/A10,A10))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x038B162C</v>
+        <v>0x96000000</v>
       </c>
       <c r="C10" s="26">
         <v>0</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="E10" s="26">
         <v>0</v>
@@ -1210,24 +1210,24 @@
       </c>
       <c r="I10" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x038B162C, 0, "10", "tpi", 0, "", "", 0 },</v>
+        <v>{ 0x96000000, 0, "0.09", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J10" s="4"/>
       <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B11" s="26" t="str">
-        <f t="shared" ref="B10:B41" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D11,"tpi"),25.4/A11,A11))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x04800000</v>
+        <f t="shared" ref="B11" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D11,"tpi"),25.4/A11,A11))*$B$1,0),8)),"0x00000000")</f>
+        <v>0x0550A142</v>
       </c>
       <c r="C11" s="26">
         <v>0</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E11" s="26">
         <v>0</v>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="I11" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x04800000, 0, "2.00", "mm", 0, "1.26", ".050", 2 },</v>
+        <v>{ 0x0550A142, 0, "10", "tpi", 0, "1.26", ".050", 2 },</v>
       </c>
       <c r="J11" s="4"/>
       <c r="Q11" s="7"/>
@@ -1253,8 +1253,8 @@
         <v>1.5</v>
       </c>
       <c r="B12" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x06000000</v>
+        <f t="shared" ref="B11:B41" si="3">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D12,"tpi"),25.4/A12,A12))*$B$1,0),8)),"0x00000000")</f>
+        <v>0x09000000</v>
       </c>
       <c r="C12" s="26">
         <v>0</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="I12" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x06000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
+        <v>{ 0x09000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>19</v>
@@ -1290,8 +1290,8 @@
         <v>1</v>
       </c>
       <c r="B13" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x09000000</v>
+        <f t="shared" si="3"/>
+        <v>0x0D800000</v>
       </c>
       <c r="C13" s="26">
         <v>0</v>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="I13" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x09000000, 0, "1.00", "mm", 0, ".65", ".026", 0 },</v>
+        <v>{ 0x0D800000, 0, "1.00", "mm", 0, ".65", ".026", 0 },</v>
       </c>
       <c r="J13" s="4"/>
       <c r="P13" s="6" t="s">
@@ -1328,7 +1328,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0x00000000</v>
       </c>
       <c r="C14" s="26">
@@ -1357,8 +1357,8 @@
         <v>0.2</v>
       </c>
       <c r="B15" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x2D000000</v>
+        <f t="shared" si="3"/>
+        <v>0x43800000</v>
       </c>
       <c r="C15" s="26">
         <v>0</v>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="I15" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x2D000000, 0, "0.20", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x43800000, 0, "0.20", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J15" s="4"/>
       <c r="Q15" s="7"/>
@@ -1386,8 +1386,8 @@
         <v>0.18</v>
       </c>
       <c r="B16" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x32000000</v>
+        <f t="shared" si="3"/>
+        <v>0x4B000000</v>
       </c>
       <c r="C16" s="26">
         <v>0</v>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="I16" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x32000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x4B000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J16" s="4"/>
       <c r="Q16" s="7"/>
@@ -1415,8 +1415,8 @@
         <v>0.15</v>
       </c>
       <c r="B17" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x3C000000</v>
+        <f t="shared" si="3"/>
+        <v>0x5A000000</v>
       </c>
       <c r="C17" s="26">
         <v>0</v>
@@ -1434,7 +1434,7 @@
       </c>
       <c r="I17" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x3C000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x5A000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J17" s="4"/>
       <c r="Q17" s="7"/>
@@ -1444,8 +1444,8 @@
         <v>0.12</v>
       </c>
       <c r="B18" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x4B000000</v>
+        <f t="shared" si="3"/>
+        <v>0x70800000</v>
       </c>
       <c r="C18" s="26">
         <v>0</v>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="I18" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x4B000000, 0, "0.12", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x70800000, 0, "0.12", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J18" s="4"/>
       <c r="Q18" s="7"/>
@@ -1473,8 +1473,8 @@
         <v>0.09</v>
       </c>
       <c r="B19" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x64000000</v>
+        <f t="shared" si="3"/>
+        <v>0x96000000</v>
       </c>
       <c r="C19" s="26">
         <v>0</v>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="I19" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x64000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x96000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J19" s="4"/>
       <c r="Q19" s="7"/>
@@ -1502,8 +1502,8 @@
         <v>0.06</v>
       </c>
       <c r="B20" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x96000000</v>
+        <f t="shared" si="3"/>
+        <v>0xE1000000</v>
       </c>
       <c r="C20" s="26">
         <v>0</v>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="I20" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x96000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
+        <v>{ 0xE1000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J20" s="4"/>
       <c r="Q20" s="7"/>
@@ -1531,8 +1531,8 @@
         <v>0.04</v>
       </c>
       <c r="B21" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0xE1000000</v>
+        <f t="shared" si="3"/>
+        <v>0x00000000</v>
       </c>
       <c r="C21" s="26">
         <v>0</v>
@@ -1550,7 +1550,7 @@
       </c>
       <c r="I21" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0xE1000000, 0, "0.04", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x00000000, 0, "0.04", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J21" s="4"/>
       <c r="Q21" s="7"/>
@@ -1560,7 +1560,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0x00000000</v>
       </c>
       <c r="C22" s="26">
@@ -1589,7 +1589,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0x00000000</v>
       </c>
       <c r="C23" s="26">
@@ -1618,8 +1618,8 @@
         <v>1.25</v>
       </c>
       <c r="B24" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x07333333</v>
+        <f t="shared" si="3"/>
+        <v>0x0ACCCCCC</v>
       </c>
       <c r="C24" s="26">
         <v>0</v>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="I24" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x07333333, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
+        <v>{ 0x0ACCCCCC, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
       </c>
       <c r="J24" s="4"/>
       <c r="Q24" s="7"/>
@@ -1651,8 +1651,8 @@
         <v>1.75</v>
       </c>
       <c r="B25" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x05249249</v>
+        <f t="shared" si="3"/>
+        <v>0x07B6DB6D</v>
       </c>
       <c r="C25" s="26">
         <v>0</v>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="I25" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x05249249, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
+        <v>{ 0x07B6DB6D, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
       </c>
       <c r="J25" s="4"/>
       <c r="Q25" s="7"/>
@@ -1684,8 +1684,8 @@
         <v>2</v>
       </c>
       <c r="B26" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x04800000</v>
+        <f t="shared" si="3"/>
+        <v>0x06C00000</v>
       </c>
       <c r="C26" s="26">
         <v>0</v>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="I26" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x04800000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
+        <v>{ 0x06C00000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
       </c>
       <c r="J26" s="4"/>
       <c r="Q26" s="7"/>
@@ -1717,8 +1717,8 @@
         <v>0.5</v>
       </c>
       <c r="B27" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x12000000</v>
+        <f t="shared" si="3"/>
+        <v>0x1B000000</v>
       </c>
       <c r="C27" s="26">
         <v>0</v>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="I27" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x12000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
+        <v>{ 0x1B000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
       </c>
       <c r="J27" s="4"/>
       <c r="Q27" s="7"/>
@@ -1750,8 +1750,8 @@
         <v>0.75</v>
       </c>
       <c r="B28" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x0C000000</v>
+        <f t="shared" si="3"/>
+        <v>0x12000000</v>
       </c>
       <c r="C28" s="26">
         <v>0</v>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="I28" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0C000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
+        <v>{ 0x12000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
       </c>
       <c r="J28" s="4"/>
       <c r="Q28" s="7"/>
@@ -1783,7 +1783,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0x00000000</v>
       </c>
       <c r="C29" s="26">
@@ -1812,7 +1812,7 @@
         <v>37</v>
       </c>
       <c r="B30" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0x00000000</v>
       </c>
       <c r="C30" s="26">
@@ -1841,8 +1841,8 @@
         <v>27</v>
       </c>
       <c r="B31" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x09912244</v>
+        <f t="shared" si="3"/>
+        <v>0x0E59B366</v>
       </c>
       <c r="C31" s="26">
         <v>0</v>
@@ -1860,7 +1860,7 @@
       </c>
       <c r="I31" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x09912244, 0, "27", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0E59B366, 0, "27", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J31" s="4"/>
       <c r="Q31" s="7"/>
@@ -1870,8 +1870,8 @@
         <v>26</v>
       </c>
       <c r="B32" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x09366CD9</v>
+        <f t="shared" si="3"/>
+        <v>0x0DD1A346</v>
       </c>
       <c r="C32" s="26">
         <v>0</v>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="I32" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x09366CD9, 0, "26", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0DD1A346, 0, "26", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J32" s="4"/>
       <c r="Q32" s="7"/>
@@ -1899,8 +1899,8 @@
         <v>24</v>
       </c>
       <c r="B33" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x08810204</v>
+        <f t="shared" si="3"/>
+        <v>0x0CC18306</v>
       </c>
       <c r="C33" s="26">
         <v>0</v>
@@ -1918,7 +1918,7 @@
       </c>
       <c r="I33" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x08810204, 0, "24", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0CC18306, 0, "24", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J33" s="4"/>
       <c r="Q33" s="7"/>
@@ -1928,8 +1928,8 @@
         <v>22</v>
       </c>
       <c r="B34" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x07CB972E</v>
+        <f t="shared" si="3"/>
+        <v>0x0BB162C5</v>
       </c>
       <c r="C34" s="26">
         <v>0</v>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="I34" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x07CB972E, 0, "22", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0BB162C5, 0, "22", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J34" s="4"/>
       <c r="Q34" s="7"/>
@@ -1957,8 +1957,8 @@
         <v>20</v>
       </c>
       <c r="B35" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x07162C58</v>
+        <f t="shared" si="3"/>
+        <v>0x0AA14285</v>
       </c>
       <c r="C35" s="26">
         <v>0</v>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="I35" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x07162C58, 0, "20", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0AA14285, 0, "20", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J35" s="4"/>
       <c r="Q35" s="7"/>
@@ -1986,8 +1986,8 @@
         <v>19</v>
       </c>
       <c r="B36" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x06BB76ED</v>
+        <f t="shared" si="3"/>
+        <v>0x0A193264</v>
       </c>
       <c r="C36" s="26">
         <v>0</v>
@@ -2004,8 +2004,8 @@
         <v>0</v>
       </c>
       <c r="I36" s="25" t="str">
-        <f t="shared" ref="I36:I41" si="3">$A$2&amp;B36&amp;$C$2&amp;C36&amp;$D$2&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D36&amp;$E$2&amp;E36&amp;$D$2&amp;F36&amp;$G$2&amp;G36&amp;$E$2&amp;H36&amp;$B$2</f>
-        <v>{ 0x06BB76ED, 0, "19", "tpi", 30, "", "", 0 },</v>
+        <f t="shared" ref="I36:I41" si="4">$A$2&amp;B36&amp;$C$2&amp;C36&amp;$D$2&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D36&amp;$E$2&amp;E36&amp;$D$2&amp;F36&amp;$G$2&amp;G36&amp;$E$2&amp;H36&amp;$B$2</f>
+        <v>{ 0x0A193264, 0, "19", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J36" s="4"/>
       <c r="Q36" s="7"/>
@@ -2015,8 +2015,8 @@
         <v>18</v>
       </c>
       <c r="B37" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x0660C183</v>
+        <f t="shared" si="3"/>
+        <v>0x09912244</v>
       </c>
       <c r="C37" s="26">
         <v>0</v>
@@ -2033,8 +2033,8 @@
         <v>0</v>
       </c>
       <c r="I37" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>{ 0x0660C183, 0, "18", "tpi", 30, "", "", 0 },</v>
+        <f t="shared" si="4"/>
+        <v>{ 0x09912244, 0, "18", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J37" s="4"/>
       <c r="Q37" s="7"/>
@@ -2044,8 +2044,8 @@
         <v>16</v>
       </c>
       <c r="B38" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x05AB56AD</v>
+        <f t="shared" si="3"/>
+        <v>0x08810204</v>
       </c>
       <c r="C38" s="26">
         <v>0</v>
@@ -2062,8 +2062,8 @@
         <v>0</v>
       </c>
       <c r="I38" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>{ 0x05AB56AD, 0, "16", "tpi", 30, "", "", 0 },</v>
+        <f t="shared" si="4"/>
+        <v>{ 0x08810204, 0, "16", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J38" s="4"/>
       <c r="Q38" s="7"/>
@@ -2073,8 +2073,8 @@
         <v>14</v>
       </c>
       <c r="B39" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x04F5EBD7</v>
+        <f t="shared" si="3"/>
+        <v>0x0770E1C3</v>
       </c>
       <c r="C39" s="26">
         <v>0</v>
@@ -2091,8 +2091,8 @@
         <v>0</v>
       </c>
       <c r="I39" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>{ 0x04F5EBD7, 0, "14", "tpi", 30, "", "", 0 },</v>
+        <f t="shared" si="4"/>
+        <v>{ 0x0770E1C3, 0, "14", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J39" s="4"/>
       <c r="Q39" s="7"/>
@@ -2102,8 +2102,8 @@
         <v>12</v>
       </c>
       <c r="B40" s="26" t="str">
-        <f t="shared" si="2"/>
-        <v>0x04408102</v>
+        <f t="shared" si="3"/>
+        <v>0x0660C183</v>
       </c>
       <c r="C40" s="26">
         <v>0</v>
@@ -2120,8 +2120,8 @@
         <v>0</v>
       </c>
       <c r="I40" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>{ 0x04408102, 0, "12", "tpi", 30, "", "", 0 },</v>
+        <f t="shared" si="4"/>
+        <v>{ 0x0660C183, 0, "12", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J40" s="4"/>
       <c r="Q40" s="7"/>
@@ -2131,7 +2131,7 @@
         <v>24</v>
       </c>
       <c r="B41" s="26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0x00000000</v>
       </c>
       <c r="C41" s="26">
@@ -2149,7 +2149,7 @@
         <v>0</v>
       </c>
       <c r="I41" s="25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>{ 0x00000000, 0, "..", "up", 30, "", "", 0 },</v>
       </c>
       <c r="J41" s="4"/>

</xml_diff>

<commit_message>
change leadscrew to 2mm
change leadscrew to 2mm, fix button BB range
</commit_message>
<xml_diff>
--- a/feed_tab.xlsx
+++ b/feed_tab.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STM32\project\efeed\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13548" windowHeight="7896" tabRatio="286"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13550" windowHeight="7900" tabRatio="286"/>
   </bookViews>
   <sheets>
     <sheet name="feed" sheetId="1" r:id="rId1"/>
     <sheet name="infeed" sheetId="5" r:id="rId2"/>
     <sheet name="ramp up" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -893,7 +898,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -903,25 +908,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.81640625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
-    <col min="9" max="9" width="42.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" customWidth="1"/>
+    <col min="9" max="9" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>24</v>
       </c>
@@ -939,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -968,13 +973,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="K3">
         <f>$A$6*2/($B$6/$C$6*A9)</f>
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>5</v>
@@ -1000,11 +1005,11 @@
       <c r="H4" s="6"/>
       <c r="J4">
         <f>A6*2*C6/A9/B6*B1</f>
-        <v>3774873600</v>
+        <v>5033164800</v>
       </c>
       <c r="K4">
         <f>ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0)</f>
-        <v>3774873600</v>
+        <v>5033164800</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>7</v>
@@ -1013,7 +1018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>45</v>
       </c>
@@ -1046,7 +1051,7 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>1800</v>
       </c>
@@ -1054,7 +1059,7 @@
         <v>400</v>
       </c>
       <c r="C6" s="16">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D6" s="16">
         <v>400</v>
@@ -1067,7 +1072,7 @@
       <c r="H6" s="6"/>
       <c r="J6" s="13" t="str">
         <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0),9)),"0x000000000")</f>
-        <v>0x0E1000000</v>
+        <v>0x12C000000</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>11</v>
@@ -1141,13 +1146,13 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
     </row>
-    <row r="9" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
         <v>0.06</v>
       </c>
       <c r="B9" s="26" t="str">
         <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D9,"tpi"),25.4/A9,A9))*$B$1,0),8)),"0x00000000")</f>
-        <v>0xE1000000</v>
+        <v>0x00000000</v>
       </c>
       <c r="C9" s="26">
         <v>0</v>
@@ -1169,7 +1174,7 @@
       </c>
       <c r="I9" s="25" t="str">
         <f t="shared" ref="I9:I35" si="0">$A$2&amp;B9&amp;$C$2&amp;C9&amp;$D$2&amp;SUBSTITUTE(TEXT(A9,IF(EXACT(D9,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D9&amp;$E$2&amp;E9&amp;$D$2&amp;F9&amp;$G$2&amp;G9&amp;$E$2&amp;H9&amp;$B$2</f>
-        <v>{ 0xE1000000, 0, "0.06", "mm", 0, "1.26", ".050", 0 },</v>
+        <v>{ 0x00000000, 0, "0.06", "mm", 0, "1.26", ".050", 0 },</v>
       </c>
       <c r="J9" s="4"/>
       <c r="P9" s="6" t="s">
@@ -1186,13 +1191,13 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
         <v>0.09</v>
       </c>
       <c r="B10" s="26" t="str">
         <f t="shared" ref="B10" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D10,"tpi"),25.4/A10,A10))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x96000000</v>
+        <v>0xC8000000</v>
       </c>
       <c r="C10" s="26">
         <v>0</v>
@@ -1210,18 +1215,18 @@
       </c>
       <c r="I10" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x96000000, 0, "0.09", "mm", 0, "", "", 0 },</v>
+        <v>{ 0xC8000000, 0, "0.09", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J10" s="4"/>
       <c r="Q10" s="7"/>
     </row>
-    <row r="11" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
         <v>10</v>
       </c>
       <c r="B11" s="26" t="str">
         <f t="shared" ref="B11" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D11,"tpi"),25.4/A11,A11))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x0550A142</v>
+        <v>0x07162C58</v>
       </c>
       <c r="C11" s="26">
         <v>0</v>
@@ -1243,18 +1248,18 @@
       </c>
       <c r="I11" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0550A142, 0, "10", "tpi", 0, "1.26", ".050", 2 },</v>
+        <v>{ 0x07162C58, 0, "10", "tpi", 0, "1.26", ".050", 2 },</v>
       </c>
       <c r="J11" s="4"/>
       <c r="Q11" s="7"/>
     </row>
-    <row r="12" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="26">
         <v>1.5</v>
       </c>
       <c r="B12" s="26" t="str">
-        <f t="shared" ref="B11:B41" si="3">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D12,"tpi"),25.4/A12,A12))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x09000000</v>
+        <f t="shared" ref="B12:B41" si="3">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D12,"tpi"),25.4/A12,A12))*$B$1,0),8)),"0x00000000")</f>
+        <v>0x0C000000</v>
       </c>
       <c r="C12" s="26">
         <v>0</v>
@@ -1276,7 +1281,7 @@
       </c>
       <c r="I12" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x09000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
+        <v>{ 0x0C000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>19</v>
@@ -1285,13 +1290,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="26">
         <v>1</v>
       </c>
       <c r="B13" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0D800000</v>
+        <v>0x12000000</v>
       </c>
       <c r="C13" s="26">
         <v>0</v>
@@ -1313,7 +1318,7 @@
       </c>
       <c r="I13" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0D800000, 0, "1.00", "mm", 0, ".65", ".026", 0 },</v>
+        <v>{ 0x12000000, 0, "1.00", "mm", 0, ".65", ".026", 0 },</v>
       </c>
       <c r="J13" s="4"/>
       <c r="P13" s="6" t="s">
@@ -1323,7 +1328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>26</v>
       </c>
@@ -1352,13 +1357,13 @@
       <c r="J14" s="4"/>
       <c r="Q14" s="7"/>
     </row>
-    <row r="15" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="26">
         <v>0.2</v>
       </c>
       <c r="B15" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x43800000</v>
+        <v>0x5A000000</v>
       </c>
       <c r="C15" s="26">
         <v>0</v>
@@ -1376,18 +1381,18 @@
       </c>
       <c r="I15" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x43800000, 0, "0.20", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x5A000000, 0, "0.20", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J15" s="4"/>
       <c r="Q15" s="7"/>
     </row>
-    <row r="16" spans="1:25" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="26">
         <v>0.18</v>
       </c>
       <c r="B16" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x4B000000</v>
+        <v>0x64000000</v>
       </c>
       <c r="C16" s="26">
         <v>0</v>
@@ -1405,18 +1410,18 @@
       </c>
       <c r="I16" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x4B000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x64000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J16" s="4"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="26">
         <v>0.15</v>
       </c>
       <c r="B17" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x5A000000</v>
+        <v>0x78000000</v>
       </c>
       <c r="C17" s="26">
         <v>0</v>
@@ -1434,18 +1439,18 @@
       </c>
       <c r="I17" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x5A000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x78000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J17" s="4"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>0.12</v>
       </c>
       <c r="B18" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x70800000</v>
+        <v>0x96000000</v>
       </c>
       <c r="C18" s="26">
         <v>0</v>
@@ -1463,18 +1468,18 @@
       </c>
       <c r="I18" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x70800000, 0, "0.12", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x96000000, 0, "0.12", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J18" s="4"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>0.09</v>
       </c>
       <c r="B19" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x96000000</v>
+        <v>0xC8000000</v>
       </c>
       <c r="C19" s="26">
         <v>0</v>
@@ -1492,14 +1497,14 @@
       </c>
       <c r="I19" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x96000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
+        <v>{ 0xC8000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J19" s="4"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A20" s="26">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="B20" s="26" t="str">
         <f t="shared" si="3"/>
@@ -1521,12 +1526,12 @@
       </c>
       <c r="I20" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0xE1000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
+        <v>{ 0xE1000000, 0, "0.08", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J20" s="4"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="26">
         <v>0.04</v>
       </c>
@@ -1555,7 +1560,7 @@
       <c r="J21" s="4"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>24</v>
       </c>
@@ -1584,7 +1589,7 @@
       <c r="J22" s="4"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>37</v>
       </c>
@@ -1613,13 +1618,13 @@
       <c r="J23" s="4"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="26">
         <v>1.25</v>
       </c>
       <c r="B24" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0ACCCCCC</v>
+        <v>0x0E666666</v>
       </c>
       <c r="C24" s="26">
         <v>0</v>
@@ -1641,18 +1646,18 @@
       </c>
       <c r="I24" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0ACCCCCC, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
+        <v>{ 0x0E666666, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
       </c>
       <c r="J24" s="4"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="26">
         <v>1.75</v>
       </c>
       <c r="B25" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x07B6DB6D</v>
+        <v>0x0A492492</v>
       </c>
       <c r="C25" s="26">
         <v>0</v>
@@ -1674,18 +1679,18 @@
       </c>
       <c r="I25" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x07B6DB6D, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
+        <v>{ 0x0A492492, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
       </c>
       <c r="J25" s="4"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="26">
         <v>2</v>
       </c>
       <c r="B26" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x06C00000</v>
+        <v>0x09000000</v>
       </c>
       <c r="C26" s="26">
         <v>0</v>
@@ -1707,18 +1712,18 @@
       </c>
       <c r="I26" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x06C00000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
+        <v>{ 0x09000000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
       </c>
       <c r="J26" s="4"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="26">
         <v>0.5</v>
       </c>
       <c r="B27" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x1B000000</v>
+        <v>0x24000000</v>
       </c>
       <c r="C27" s="26">
         <v>0</v>
@@ -1740,18 +1745,18 @@
       </c>
       <c r="I27" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x1B000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
+        <v>{ 0x24000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
       </c>
       <c r="J27" s="4"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="26">
         <v>0.75</v>
       </c>
       <c r="B28" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x12000000</v>
+        <v>0x18000000</v>
       </c>
       <c r="C28" s="26">
         <v>0</v>
@@ -1773,12 +1778,12 @@
       </c>
       <c r="I28" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x12000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
+        <v>{ 0x18000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
       </c>
       <c r="J28" s="4"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
         <v>24</v>
       </c>
@@ -1807,7 +1812,7 @@
       <c r="J29" s="4"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>37</v>
       </c>
@@ -1836,13 +1841,13 @@
       <c r="J30" s="4"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A31" s="26">
         <v>27</v>
       </c>
       <c r="B31" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0E59B366</v>
+        <v>0x13224489</v>
       </c>
       <c r="C31" s="26">
         <v>0</v>
@@ -1860,18 +1865,18 @@
       </c>
       <c r="I31" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0E59B366, 0, "27", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x13224489, 0, "27", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J31" s="4"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A32" s="26">
         <v>26</v>
       </c>
       <c r="B32" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0DD1A346</v>
+        <v>0x126CD9B3</v>
       </c>
       <c r="C32" s="26">
         <v>0</v>
@@ -1889,18 +1894,18 @@
       </c>
       <c r="I32" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0DD1A346, 0, "26", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x126CD9B3, 0, "26", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J32" s="4"/>
       <c r="Q32" s="7"/>
     </row>
-    <row r="33" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A33" s="26">
         <v>24</v>
       </c>
       <c r="B33" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0CC18306</v>
+        <v>0x11020408</v>
       </c>
       <c r="C33" s="26">
         <v>0</v>
@@ -1918,18 +1923,18 @@
       </c>
       <c r="I33" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0CC18306, 0, "24", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x11020408, 0, "24", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J33" s="4"/>
       <c r="Q33" s="7"/>
     </row>
-    <row r="34" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A34" s="26">
         <v>22</v>
       </c>
       <c r="B34" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0BB162C5</v>
+        <v>0x0F972E5C</v>
       </c>
       <c r="C34" s="26">
         <v>0</v>
@@ -1947,18 +1952,18 @@
       </c>
       <c r="I34" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0BB162C5, 0, "22", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0F972E5C, 0, "22", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J34" s="4"/>
       <c r="Q34" s="7"/>
     </row>
-    <row r="35" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A35" s="26">
         <v>20</v>
       </c>
       <c r="B35" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0AA14285</v>
+        <v>0x0E2C58B1</v>
       </c>
       <c r="C35" s="26">
         <v>0</v>
@@ -1976,18 +1981,18 @@
       </c>
       <c r="I35" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0AA14285, 0, "20", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0E2C58B1, 0, "20", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J35" s="4"/>
       <c r="Q35" s="7"/>
     </row>
-    <row r="36" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="26">
         <v>19</v>
       </c>
       <c r="B36" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0A193264</v>
+        <v>0x0D76EDDB</v>
       </c>
       <c r="C36" s="26">
         <v>0</v>
@@ -2005,18 +2010,18 @@
       </c>
       <c r="I36" s="25" t="str">
         <f t="shared" ref="I36:I41" si="4">$A$2&amp;B36&amp;$C$2&amp;C36&amp;$D$2&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D36&amp;$E$2&amp;E36&amp;$D$2&amp;F36&amp;$G$2&amp;G36&amp;$E$2&amp;H36&amp;$B$2</f>
-        <v>{ 0x0A193264, 0, "19", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0D76EDDB, 0, "19", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J36" s="4"/>
       <c r="Q36" s="7"/>
     </row>
-    <row r="37" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A37" s="26">
         <v>18</v>
       </c>
       <c r="B37" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x09912244</v>
+        <v>0x0CC18306</v>
       </c>
       <c r="C37" s="26">
         <v>0</v>
@@ -2034,18 +2039,18 @@
       </c>
       <c r="I37" s="25" t="str">
         <f t="shared" si="4"/>
-        <v>{ 0x09912244, 0, "18", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0CC18306, 0, "18", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J37" s="4"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A38" s="26">
         <v>16</v>
       </c>
       <c r="B38" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x08810204</v>
+        <v>0x0B56AD5A</v>
       </c>
       <c r="C38" s="26">
         <v>0</v>
@@ -2063,18 +2068,18 @@
       </c>
       <c r="I38" s="25" t="str">
         <f t="shared" si="4"/>
-        <v>{ 0x08810204, 0, "16", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0B56AD5A, 0, "16", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J38" s="4"/>
       <c r="Q38" s="7"/>
     </row>
-    <row r="39" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A39" s="26">
         <v>14</v>
       </c>
       <c r="B39" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0770E1C3</v>
+        <v>0x09EBD7AF</v>
       </c>
       <c r="C39" s="26">
         <v>0</v>
@@ -2092,18 +2097,18 @@
       </c>
       <c r="I39" s="25" t="str">
         <f t="shared" si="4"/>
-        <v>{ 0x0770E1C3, 0, "14", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x09EBD7AF, 0, "14", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J39" s="4"/>
       <c r="Q39" s="7"/>
     </row>
-    <row r="40" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A40" s="26">
         <v>12</v>
       </c>
       <c r="B40" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>0x0660C183</v>
+        <v>0x08810204</v>
       </c>
       <c r="C40" s="26">
         <v>0</v>
@@ -2121,12 +2126,12 @@
       </c>
       <c r="I40" s="25" t="str">
         <f t="shared" si="4"/>
-        <v>{ 0x0660C183, 0, "12", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x08810204, 0, "12", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J40" s="4"/>
       <c r="Q40" s="7"/>
     </row>
-    <row r="41" spans="1:17" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
         <v>24</v>
       </c>
@@ -2155,7 +2160,7 @@
       <c r="J41" s="4"/>
       <c r="Q41" s="7"/>
     </row>
-    <row r="42" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" s="6" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="C42" s="4"/>
       <c r="E42" s="4"/>
@@ -2165,7 +2170,7 @@
       <c r="J42" s="4"/>
       <c r="Q42" s="7"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="13" x14ac:dyDescent="0.3">
       <c r="A43" s="9"/>
       <c r="B43" s="6"/>
       <c r="C43" s="4"/>
@@ -2229,123 +2234,123 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="E64"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="E68"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="E69"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="E70"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="E71"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="E72"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="E73"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="E74"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="E75"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="E76"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="E77"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="E78"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="E79"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A80" s="4"/>
       <c r="E80"/>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="E81"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="E82"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="E84"/>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A85" s="4"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="E86"/>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A88" s="4"/>
       <c r="E88"/>
     </row>
@@ -2590,20 +2595,20 @@
       <selection activeCell="F10" sqref="F10:F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.77734375" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>107</v>
       </c>
@@ -2640,7 +2645,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>109</v>
       </c>
@@ -2690,7 +2695,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>104</v>
       </c>
@@ -2722,7 +2727,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="25" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>105</v>
       </c>
@@ -2747,7 +2752,7 @@
       <c r="L9" s="14"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -2781,7 +2786,7 @@
       <c r="L10" s="14"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -2816,7 +2821,7 @@
       <c r="L11" s="14"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>3</v>
       </c>
@@ -3349,12 +3354,12 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>30</v>
       </c>
@@ -3362,7 +3367,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>21.888000000000002</v>
       </c>
@@ -3370,7 +3375,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>17.024000000000001</v>
       </c>
@@ -3378,7 +3383,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>14.40492308</v>
       </c>
@@ -3386,7 +3391,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>12.710226240000001</v>
       </c>
@@ -3394,7 +3399,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>11.499728510000001</v>
       </c>
@@ -3402,7 +3407,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>10.57975023</v>
       </c>
@@ -3410,7 +3415,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>9.8501122799999994</v>
       </c>
@@ -3418,7 +3423,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>9.2531357780000008</v>
       </c>
@@ -3426,7 +3431,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8.7529662760000004</v>
       </c>
@@ -3434,7 +3439,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8.3259923120000003</v>
       </c>
@@ -3442,7 +3447,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>7.9559482089999998</v>
       </c>
@@ -3450,7 +3455,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7.6312156289999997</v>
       </c>
@@ -3458,7 +3463,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>7.3432452279999998</v>
       </c>
@@ -3466,7 +3471,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>7.085587501</v>
       </c>
@@ -3474,7 +3479,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>6.8532731560000002</v>
       </c>
@@ -3482,7 +3487,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>6.6424032129999997</v>
       </c>
@@ -3490,7 +3495,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>6.4498697869999999</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>6.2731610250000003</v>
       </c>
@@ -3506,7 +3511,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>6.1102217779999997</v>
       </c>
@@ -3514,7 +3519,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>5.9593521039999997</v>
       </c>
@@ -3522,7 +3527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>5.8191320549999999</v>
       </c>
@@ -3530,7 +3535,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>5.688365042</v>
       </c>
@@ -3538,7 +3543,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>5.5660346110000001</v>
       </c>
@@ -3546,7 +3551,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>5.4512710110000002</v>
       </c>
@@ -3554,7 +3559,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>5.3433250499999998</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>5.2415474299999998</v>
       </c>
@@ -3570,7 +3575,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>5.1453722480000001</v>
       </c>
@@ -3578,7 +3583,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>5.0543037130000004</v>
       </c>
@@ -3586,7 +3591,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>4.9679053590000004</v>
       </c>
@@ -3594,7 +3599,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>4.8857912209999999</v>
       </c>
@@ -3602,7 +3607,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>4.807618561</v>
       </c>
@@ -3610,7 +3615,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>4.7330818389999996</v>
       </c>
@@ -3618,7 +3623,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>4.6619076760000002</v>
       </c>
@@ -3626,7 +3631,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>4.5938506300000004</v>
       </c>

</xml_diff>

<commit_message>
stm32 cube 1.8.0, LL i2c screen work, leadscrew 2mm
</commit_message>
<xml_diff>
--- a/feed_tab.xlsx
+++ b/feed_tab.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
   <si>
     <t>"</t>
   </si>
@@ -909,7 +909,7 @@
   <dimension ref="A1:Y161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -979,7 +979,7 @@
       <c r="H3" s="2"/>
       <c r="K3">
         <f>$A$6*2/($B$6/$C$6*A9)</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>5</v>
@@ -1005,11 +1005,11 @@
       <c r="H4" s="6"/>
       <c r="J4">
         <f>A6*2*C6/A9/B6*B1</f>
-        <v>2516582400</v>
+        <v>3355443200</v>
       </c>
       <c r="K4">
         <f>ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0)</f>
-        <v>2516582400</v>
+        <v>3355443200</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>7</v>
@@ -1059,7 +1059,7 @@
         <v>400</v>
       </c>
       <c r="C6" s="16">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D6" s="16">
         <v>400</v>
@@ -1072,7 +1072,7 @@
       <c r="H6" s="6"/>
       <c r="J6" s="13" t="str">
         <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*A9)*$B$1,0),9)),"0x000000000")</f>
-        <v>0x096000000</v>
+        <v>0x0C8000000</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>11</v>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="B9" s="26" t="str">
         <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D9,"tpi"),25.4/A9,A9))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x96000000</v>
+        <v>0xC8000000</v>
       </c>
       <c r="C9" s="26">
         <v>0</v>
@@ -1163,18 +1163,14 @@
       <c r="E9" s="26">
         <v>0</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>13</v>
-      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="25">
         <v>0</v>
       </c>
       <c r="I9" s="25" t="str">
         <f t="shared" ref="I9:I35" si="0">$A$2&amp;B9&amp;$C$2&amp;C9&amp;$D$2&amp;SUBSTITUTE(TEXT(A9,IF(EXACT(D9,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D9&amp;$E$2&amp;E9&amp;$D$2&amp;F9&amp;$G$2&amp;G9&amp;$E$2&amp;H9&amp;$B$2</f>
-        <v>{ 0x96000000, 0, "0.09", "mm", 0, "1.26", ".050", 0 },</v>
+        <v>{ 0xC8000000, 0, "0.09", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J9" s="4"/>
       <c r="P9" s="6" t="s">
@@ -1197,7 +1193,7 @@
       </c>
       <c r="B10" s="26" t="str">
         <f t="shared" ref="B10" si="1">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D10,"tpi"),25.4/A10,A10))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x5A000000</v>
+        <v>0x78000000</v>
       </c>
       <c r="C10" s="26">
         <v>0</v>
@@ -1215,7 +1211,7 @@
       </c>
       <c r="I10" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x5A000000, 0, "0.15", "mm", 0, "", "", 0 },</v>
+        <v>{ 0x78000000, 0, "0.15", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J10" s="4"/>
       <c r="Q10" s="7"/>
@@ -1226,7 +1222,7 @@
       </c>
       <c r="B11" s="26" t="str">
         <f t="shared" ref="B11:B41" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$6*2/($B$6/$C$6*IF(EXACT(D11,"tpi"),25.4/A11,A11))*$B$1,0),8)),"0x00000000")</f>
-        <v>0x09000000</v>
+        <v>0x0C000000</v>
       </c>
       <c r="C11" s="26">
         <v>0</v>
@@ -1248,7 +1244,7 @@
       </c>
       <c r="I11" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x09000000, 0, "1.50", "mm", 0, "1.26", ".050", 2 },</v>
+        <v>{ 0x0C000000, 0, "1.50", "mm", 0, "1.26", ".050", 2 },</v>
       </c>
       <c r="J11" s="4"/>
       <c r="Q11" s="7"/>
@@ -1259,7 +1255,7 @@
       </c>
       <c r="B12" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0D800000</v>
+        <v>0x12000000</v>
       </c>
       <c r="C12" s="26">
         <v>0</v>
@@ -1281,7 +1277,7 @@
       </c>
       <c r="I12" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0D800000, 0, "1.00", "mm", 0, ".95", ".037", 0 },</v>
+        <v>{ 0x12000000, 0, "1.00", "mm", 0, ".95", ".037", 0 },</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>19</v>
@@ -1296,7 +1292,7 @@
       </c>
       <c r="B13" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0550A142</v>
+        <v>0x07162C58</v>
       </c>
       <c r="C13" s="26">
         <v>0</v>
@@ -1318,7 +1314,7 @@
       </c>
       <c r="I13" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0550A142, 0, "10", "tpi", 0, ".65", ".026", 0 },</v>
+        <v>{ 0x07162C58, 0, "10", "tpi", 0, ".65", ".026", 0 },</v>
       </c>
       <c r="J13" s="4"/>
       <c r="P13" s="6" t="s">
@@ -1363,7 +1359,7 @@
       </c>
       <c r="B15" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x43800000</v>
+        <v>0x5A000000</v>
       </c>
       <c r="C15" s="26">
         <v>0</v>
@@ -1381,7 +1377,7 @@
       </c>
       <c r="I15" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x43800000, 0, "0.20", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x5A000000, 0, "0.20", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J15" s="4"/>
       <c r="Q15" s="7"/>
@@ -1392,7 +1388,7 @@
       </c>
       <c r="B16" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x4B000000</v>
+        <v>0x64000000</v>
       </c>
       <c r="C16" s="26">
         <v>0</v>
@@ -1410,7 +1406,7 @@
       </c>
       <c r="I16" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x4B000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x64000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J16" s="4"/>
       <c r="Q16" s="7"/>
@@ -1421,7 +1417,7 @@
       </c>
       <c r="B17" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x5A000000</v>
+        <v>0x78000000</v>
       </c>
       <c r="C17" s="26">
         <v>0</v>
@@ -1439,7 +1435,7 @@
       </c>
       <c r="I17" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x5A000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x78000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J17" s="4"/>
       <c r="Q17" s="7"/>
@@ -1450,7 +1446,7 @@
       </c>
       <c r="B18" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x70800000</v>
+        <v>0x96000000</v>
       </c>
       <c r="C18" s="26">
         <v>0</v>
@@ -1468,7 +1464,7 @@
       </c>
       <c r="I18" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x70800000, 0, "0.12", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x96000000, 0, "0.12", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J18" s="4"/>
       <c r="Q18" s="7"/>
@@ -1479,7 +1475,7 @@
       </c>
       <c r="B19" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x96000000</v>
+        <v>0xC8000000</v>
       </c>
       <c r="C19" s="26">
         <v>0</v>
@@ -1497,7 +1493,7 @@
       </c>
       <c r="I19" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x96000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
+        <v>{ 0xC8000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J19" s="4"/>
       <c r="Q19" s="7"/>
@@ -1508,7 +1504,7 @@
       </c>
       <c r="B20" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0xE1000000</v>
+        <v>0x00000000</v>
       </c>
       <c r="C20" s="26">
         <v>0</v>
@@ -1526,7 +1522,7 @@
       </c>
       <c r="I20" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0xE1000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
+        <v>{ 0x00000000, 0, "0.06", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J20" s="4"/>
       <c r="Q20" s="7"/>
@@ -1624,7 +1620,7 @@
       </c>
       <c r="B24" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0ACCCCCC</v>
+        <v>0x0E666666</v>
       </c>
       <c r="C24" s="26">
         <v>0</v>
@@ -1646,7 +1642,7 @@
       </c>
       <c r="I24" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0ACCCCCC, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
+        <v>{ 0x0E666666, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
       </c>
       <c r="J24" s="4"/>
       <c r="Q24" s="7"/>
@@ -1657,7 +1653,7 @@
       </c>
       <c r="B25" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x07B6DB6D</v>
+        <v>0x0A492492</v>
       </c>
       <c r="C25" s="26">
         <v>0</v>
@@ -1679,7 +1675,7 @@
       </c>
       <c r="I25" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x07B6DB6D, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
+        <v>{ 0x0A492492, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
       </c>
       <c r="J25" s="4"/>
       <c r="Q25" s="7"/>
@@ -1690,7 +1686,7 @@
       </c>
       <c r="B26" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x06C00000</v>
+        <v>0x09000000</v>
       </c>
       <c r="C26" s="26">
         <v>0</v>
@@ -1712,7 +1708,7 @@
       </c>
       <c r="I26" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x06C00000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
+        <v>{ 0x09000000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
       </c>
       <c r="J26" s="4"/>
       <c r="Q26" s="7"/>
@@ -1723,7 +1719,7 @@
       </c>
       <c r="B27" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x1B000000</v>
+        <v>0x24000000</v>
       </c>
       <c r="C27" s="26">
         <v>0</v>
@@ -1745,7 +1741,7 @@
       </c>
       <c r="I27" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x1B000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
+        <v>{ 0x24000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
       </c>
       <c r="J27" s="4"/>
       <c r="Q27" s="7"/>
@@ -1756,7 +1752,7 @@
       </c>
       <c r="B28" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x12000000</v>
+        <v>0x18000000</v>
       </c>
       <c r="C28" s="26">
         <v>0</v>
@@ -1778,7 +1774,7 @@
       </c>
       <c r="I28" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x12000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
+        <v>{ 0x18000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
       </c>
       <c r="J28" s="4"/>
       <c r="Q28" s="7"/>
@@ -1847,7 +1843,7 @@
       </c>
       <c r="B31" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0E59B366</v>
+        <v>0x13224489</v>
       </c>
       <c r="C31" s="26">
         <v>0</v>
@@ -1865,7 +1861,7 @@
       </c>
       <c r="I31" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0E59B366, 0, "27", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x13224489, 0, "27", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J31" s="4"/>
       <c r="Q31" s="7"/>
@@ -1876,7 +1872,7 @@
       </c>
       <c r="B32" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0DD1A346</v>
+        <v>0x126CD9B3</v>
       </c>
       <c r="C32" s="26">
         <v>0</v>
@@ -1894,7 +1890,7 @@
       </c>
       <c r="I32" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0DD1A346, 0, "26", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x126CD9B3, 0, "26", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J32" s="4"/>
       <c r="Q32" s="7"/>
@@ -1905,7 +1901,7 @@
       </c>
       <c r="B33" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0CC18306</v>
+        <v>0x11020408</v>
       </c>
       <c r="C33" s="26">
         <v>0</v>
@@ -1923,7 +1919,7 @@
       </c>
       <c r="I33" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0CC18306, 0, "24", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x11020408, 0, "24", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J33" s="4"/>
       <c r="Q33" s="7"/>
@@ -1934,7 +1930,7 @@
       </c>
       <c r="B34" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0BB162C5</v>
+        <v>0x0F972E5C</v>
       </c>
       <c r="C34" s="26">
         <v>0</v>
@@ -1952,7 +1948,7 @@
       </c>
       <c r="I34" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0BB162C5, 0, "22", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0F972E5C, 0, "22", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J34" s="4"/>
       <c r="Q34" s="7"/>
@@ -1963,7 +1959,7 @@
       </c>
       <c r="B35" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0AA14285</v>
+        <v>0x0E2C58B1</v>
       </c>
       <c r="C35" s="26">
         <v>0</v>
@@ -1981,7 +1977,7 @@
       </c>
       <c r="I35" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>{ 0x0AA14285, 0, "20", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0E2C58B1, 0, "20", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J35" s="4"/>
       <c r="Q35" s="7"/>
@@ -1992,7 +1988,7 @@
       </c>
       <c r="B36" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0A193264</v>
+        <v>0x0D76EDDB</v>
       </c>
       <c r="C36" s="26">
         <v>0</v>
@@ -2010,7 +2006,7 @@
       </c>
       <c r="I36" s="25" t="str">
         <f t="shared" ref="I36:I41" si="3">$A$2&amp;B36&amp;$C$2&amp;C36&amp;$D$2&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$G$2&amp;D36&amp;$E$2&amp;E36&amp;$D$2&amp;F36&amp;$G$2&amp;G36&amp;$E$2&amp;H36&amp;$B$2</f>
-        <v>{ 0x0A193264, 0, "19", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0D76EDDB, 0, "19", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J36" s="4"/>
       <c r="Q36" s="7"/>
@@ -2021,7 +2017,7 @@
       </c>
       <c r="B37" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x09912244</v>
+        <v>0x0CC18306</v>
       </c>
       <c r="C37" s="26">
         <v>0</v>
@@ -2039,7 +2035,7 @@
       </c>
       <c r="I37" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>{ 0x09912244, 0, "18", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0CC18306, 0, "18", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J37" s="4"/>
       <c r="Q37" s="7"/>
@@ -2050,7 +2046,7 @@
       </c>
       <c r="B38" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x08810204</v>
+        <v>0x0B56AD5A</v>
       </c>
       <c r="C38" s="26">
         <v>0</v>
@@ -2068,7 +2064,7 @@
       </c>
       <c r="I38" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>{ 0x08810204, 0, "16", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x0B56AD5A, 0, "16", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J38" s="4"/>
       <c r="Q38" s="7"/>
@@ -2079,7 +2075,7 @@
       </c>
       <c r="B39" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0770E1C3</v>
+        <v>0x09EBD7AF</v>
       </c>
       <c r="C39" s="26">
         <v>0</v>
@@ -2097,7 +2093,7 @@
       </c>
       <c r="I39" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>{ 0x0770E1C3, 0, "14", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x09EBD7AF, 0, "14", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J39" s="4"/>
       <c r="Q39" s="7"/>
@@ -2108,7 +2104,7 @@
       </c>
       <c r="B40" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>0x0660C183</v>
+        <v>0x08810204</v>
       </c>
       <c r="C40" s="26">
         <v>0</v>
@@ -2126,7 +2122,7 @@
       </c>
       <c r="I40" s="25" t="str">
         <f t="shared" si="3"/>
-        <v>{ 0x0660C183, 0, "12", "tpi", 30, "", "", 0 },</v>
+        <v>{ 0x08810204, 0, "12", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J40" s="4"/>
       <c r="Q40" s="7"/>
@@ -3423,7 +3419,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>9.2531357780000008</v>
       </c>
@@ -3431,7 +3427,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8.7529662760000004</v>
       </c>
@@ -3439,7 +3435,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8.3259923120000003</v>
       </c>
@@ -3447,7 +3443,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>7.9559482089999998</v>
       </c>
@@ -3455,7 +3451,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7.6312156289999997</v>
       </c>
@@ -3463,7 +3459,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>7.3432452279999998</v>
       </c>
@@ -3471,7 +3467,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>7.085587501</v>
       </c>
@@ -3479,7 +3475,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>6.8532731560000002</v>
       </c>
@@ -3487,7 +3483,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>6.6424032129999997</v>
       </c>
@@ -3495,7 +3491,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>6.4498697869999999</v>
       </c>
@@ -3503,7 +3499,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>6.2731610250000003</v>
       </c>
@@ -3511,7 +3507,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>6.1102217779999997</v>
       </c>
@@ -3519,7 +3515,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>5.9593521039999997</v>
       </c>
@@ -3527,7 +3523,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>5.8191320549999999</v>
       </c>
@@ -3535,7 +3531,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>5.688365042</v>
       </c>
@@ -3543,7 +3539,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>5.5660346110000001</v>
       </c>
@@ -3551,7 +3547,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>5.4512710110000002</v>
       </c>
@@ -3559,7 +3555,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>5.3433250499999998</v>
       </c>
@@ -3567,7 +3563,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>5.2415474299999998</v>
       </c>
@@ -3575,7 +3571,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>5.1453722480000001</v>
       </c>
@@ -3583,7 +3579,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>5.0543037130000004</v>
       </c>
@@ -3591,7 +3587,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>4.9679053590000004</v>
       </c>
@@ -3599,7 +3595,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>4.8857912209999999</v>
       </c>
@@ -3607,7 +3603,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>4.807618561</v>
       </c>
@@ -3615,7 +3611,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>4.7330818389999996</v>
       </c>
@@ -3623,7 +3619,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>4.6619076760000002</v>
       </c>
@@ -3631,7 +3627,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>4.5938506300000004</v>
       </c>

</xml_diff>

<commit_message>
refactoring of init_gp using, bugfixes of coordinate system, incremental mode
</commit_message>
<xml_diff>
--- a/feed_tab.xlsx
+++ b/feed_tab.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\STM32\project\efeed\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13550" windowHeight="7890" tabRatio="286"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13548" windowHeight="7896" tabRatio="286" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="feed" sheetId="1" r:id="rId1"/>
     <sheet name="infeed" sheetId="5" r:id="rId2"/>
     <sheet name="ramp up" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -336,9 +331,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -489,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -552,7 +548,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -561,9 +557,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -921,7 +918,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -931,25 +928,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" customWidth="1"/>
-    <col min="9" max="9" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.6328125" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2">
         <v>24</v>
       </c>
@@ -981,8 +978,8 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:25" s="4" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:25" s="4" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="30"/>
@@ -990,7 +987,7 @@
       <c r="F2" s="2"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:25" s="4" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" s="4" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>32</v>
       </c>
@@ -1004,7 +1001,7 @@
       <c r="F3" s="2"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:25" s="4" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" s="4" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>1800</v>
       </c>
@@ -1017,7 +1014,7 @@
       <c r="F4" s="2"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:25" s="4" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" s="4" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
         <v>35</v>
       </c>
@@ -1026,7 +1023,7 @@
       <c r="F5" s="2"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>33</v>
       </c>
@@ -1039,7 +1036,7 @@
       <c r="F6" s="2"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:25" s="4" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" s="4" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>400</v>
       </c>
@@ -1052,7 +1049,7 @@
       <c r="F7" s="2"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:25" s="4" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" s="4" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
         <v>34</v>
       </c>
@@ -1061,11 +1058,11 @@
       <c r="F8" s="2"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:25" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" s="4" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="29" t="s">
         <v>101</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1074,7 +1071,7 @@
       <c r="F9" s="2"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:25" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>400</v>
       </c>
@@ -1088,7 +1085,7 @@
       <c r="F10" s="2"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:25" ht="26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>29</v>
       </c>
@@ -1119,12 +1116,12 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
         <v>2</v>
       </c>
       <c r="B12" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D12,"tpi"),25.4/A12,A12))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" ref="B12:B31" si="0">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D12,"tpi"),25.4/A12,A12))*$B$1,0),8)),"0x00000000")</f>
         <v>0x09000000</v>
       </c>
       <c r="C12" s="24">
@@ -1146,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="23" t="str">
-        <f>$D$1&amp;B12&amp;$F$1&amp;C12&amp;$G$1&amp;SUBSTITUTE(TEXT(A12,IF(EXACT(D12,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D12&amp;$H$1&amp;E12&amp;$G$1&amp;F12&amp;$C$1&amp;G12&amp;$H$1&amp;H12&amp;$E$1</f>
+        <f t="shared" ref="I12:I45" si="1">$D$1&amp;B12&amp;$F$1&amp;C12&amp;$G$1&amp;SUBSTITUTE(TEXT(A12,IF(EXACT(D12,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D12&amp;$H$1&amp;E12&amp;$G$1&amp;F12&amp;$C$1&amp;G12&amp;$H$1&amp;H12&amp;$E$1</f>
         <v>{ 0x09000000, 0, "2.00", "mm", 0, "1.26", ".050", 0 },</v>
       </c>
       <c r="J12" s="2"/>
@@ -1160,12 +1157,12 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" spans="1:25" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="24">
         <v>2</v>
       </c>
       <c r="B13" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D13,"tpi"),25.4/A13,A13))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x09000000</v>
       </c>
       <c r="C13" s="24">
@@ -1187,18 +1184,18 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="str">
-        <f>$D$1&amp;B13&amp;$F$1&amp;C13&amp;$G$1&amp;SUBSTITUTE(TEXT(A13,IF(EXACT(D13,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D13&amp;$H$1&amp;E13&amp;$G$1&amp;F13&amp;$C$1&amp;G13&amp;$H$1&amp;H13&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x09000000, 0, "2.00", "mm", 0, "1.26", ".050", 1 },</v>
       </c>
       <c r="J13" s="2"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:25" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
         <v>2</v>
       </c>
       <c r="B14" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D14,"tpi"),25.4/A14,A14))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x09000000</v>
       </c>
       <c r="C14" s="24">
@@ -1220,18 +1217,18 @@
         <v>2</v>
       </c>
       <c r="I14" s="23" t="str">
-        <f>$D$1&amp;B14&amp;$F$1&amp;C14&amp;$G$1&amp;SUBSTITUTE(TEXT(A14,IF(EXACT(D14,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D14&amp;$H$1&amp;E14&amp;$G$1&amp;F14&amp;$C$1&amp;G14&amp;$H$1&amp;H14&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x09000000, 0, "2.00", "mm", 0, "1.26", ".050", 2 },</v>
       </c>
       <c r="J14" s="2"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="24">
         <v>1.5</v>
       </c>
       <c r="B15" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D15,"tpi"),25.4/A15,A15))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x0C000000</v>
       </c>
       <c r="C15" s="24">
@@ -1253,18 +1250,18 @@
         <v>0</v>
       </c>
       <c r="I15" s="23" t="str">
-        <f>$D$1&amp;B15&amp;$F$1&amp;C15&amp;$G$1&amp;SUBSTITUTE(TEXT(A15,IF(EXACT(D15,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D15&amp;$H$1&amp;E15&amp;$G$1&amp;F15&amp;$C$1&amp;G15&amp;$H$1&amp;H15&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x0C000000, 0, "1.50", "mm", 0, ".95", ".037", 0 },</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="24">
         <v>1</v>
       </c>
       <c r="B16" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D16,"tpi"),25.4/A16,A16))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x12000000</v>
       </c>
       <c r="C16" s="24">
@@ -1286,19 +1283,19 @@
         <v>0</v>
       </c>
       <c r="I16" s="23" t="str">
-        <f>$D$1&amp;B16&amp;$F$1&amp;C16&amp;$G$1&amp;SUBSTITUTE(TEXT(A16,IF(EXACT(D16,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D16&amp;$H$1&amp;E16&amp;$G$1&amp;F16&amp;$C$1&amp;G16&amp;$H$1&amp;H16&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x12000000, 0, "1.00", "mm", 0, ".65", ".026", 0 },</v>
       </c>
       <c r="J16" s="2"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D17,"tpi"),25.4/A17,A17))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x00000000</v>
       </c>
       <c r="C17" s="24">
@@ -1316,18 +1313,18 @@
         <v>0</v>
       </c>
       <c r="I17" s="23" t="str">
-        <f>$D$1&amp;B17&amp;$F$1&amp;C17&amp;$G$1&amp;SUBSTITUTE(TEXT(A17,IF(EXACT(D17,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D17&amp;$H$1&amp;E17&amp;$G$1&amp;F17&amp;$C$1&amp;G17&amp;$H$1&amp;H17&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x00000000, 20, "F", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J17" s="2"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="24">
         <v>0.2</v>
       </c>
       <c r="B18" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D18,"tpi"),25.4/A18,A18))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x5A000000</v>
       </c>
       <c r="C18" s="24">
@@ -1345,18 +1342,18 @@
         <v>0</v>
       </c>
       <c r="I18" s="23" t="str">
-        <f>$D$1&amp;B18&amp;$F$1&amp;C18&amp;$G$1&amp;SUBSTITUTE(TEXT(A18,IF(EXACT(D18,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D18&amp;$H$1&amp;E18&amp;$G$1&amp;F18&amp;$C$1&amp;G18&amp;$H$1&amp;H18&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x5A000000, 0, "0.20", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J18" s="2"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="24">
         <v>0.18</v>
       </c>
       <c r="B19" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D19,"tpi"),25.4/A19,A19))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x64000000</v>
       </c>
       <c r="C19" s="24">
@@ -1374,18 +1371,18 @@
         <v>0</v>
       </c>
       <c r="I19" s="23" t="str">
-        <f>$D$1&amp;B19&amp;$F$1&amp;C19&amp;$G$1&amp;SUBSTITUTE(TEXT(A19,IF(EXACT(D19,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D19&amp;$H$1&amp;E19&amp;$G$1&amp;F19&amp;$C$1&amp;G19&amp;$H$1&amp;H19&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x64000000, 0, "0.18", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J19" s="2"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="24">
         <v>0.15</v>
       </c>
       <c r="B20" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D20,"tpi"),25.4/A20,A20))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x78000000</v>
       </c>
       <c r="C20" s="24">
@@ -1403,18 +1400,18 @@
         <v>0</v>
       </c>
       <c r="I20" s="23" t="str">
-        <f>$D$1&amp;B20&amp;$F$1&amp;C20&amp;$G$1&amp;SUBSTITUTE(TEXT(A20,IF(EXACT(D20,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D20&amp;$H$1&amp;E20&amp;$G$1&amp;F20&amp;$C$1&amp;G20&amp;$H$1&amp;H20&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x78000000, 0, "0.15", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J20" s="2"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="24">
         <v>0.12</v>
       </c>
       <c r="B21" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D21,"tpi"),25.4/A21,A21))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x96000000</v>
       </c>
       <c r="C21" s="24">
@@ -1432,18 +1429,18 @@
         <v>0</v>
       </c>
       <c r="I21" s="23" t="str">
-        <f>$D$1&amp;B21&amp;$F$1&amp;C21&amp;$G$1&amp;SUBSTITUTE(TEXT(A21,IF(EXACT(D21,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D21&amp;$H$1&amp;E21&amp;$G$1&amp;F21&amp;$C$1&amp;G21&amp;$H$1&amp;H21&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x96000000, 0, "0.12", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J21" s="2"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="24">
         <v>0.09</v>
       </c>
       <c r="B22" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D22,"tpi"),25.4/A22,A22))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0xC8000000</v>
       </c>
       <c r="C22" s="24">
@@ -1461,18 +1458,18 @@
         <v>0</v>
       </c>
       <c r="I22" s="23" t="str">
-        <f>$D$1&amp;B22&amp;$F$1&amp;C22&amp;$G$1&amp;SUBSTITUTE(TEXT(A22,IF(EXACT(D22,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D22&amp;$H$1&amp;E22&amp;$G$1&amp;F22&amp;$C$1&amp;G22&amp;$H$1&amp;H22&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0xC8000000, 0, "0.09", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J22" s="2"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="24">
         <v>0.08</v>
       </c>
       <c r="B23" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D23,"tpi"),25.4/A23,A23))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0xE1000000</v>
       </c>
       <c r="C23" s="24">
@@ -1490,18 +1487,18 @@
         <v>0</v>
       </c>
       <c r="I23" s="23" t="str">
-        <f>$D$1&amp;B23&amp;$F$1&amp;C23&amp;$G$1&amp;SUBSTITUTE(TEXT(A23,IF(EXACT(D23,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D23&amp;$H$1&amp;E23&amp;$G$1&amp;F23&amp;$C$1&amp;G23&amp;$H$1&amp;H23&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0xE1000000, 0, "0.08", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J23" s="2"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="24">
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="B24" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D24,"tpi"),25.4/A24,A24))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0xFA000000</v>
       </c>
       <c r="C24" s="24">
@@ -1519,18 +1516,18 @@
         <v>0</v>
       </c>
       <c r="I24" s="23" t="str">
-        <f>$D$1&amp;B24&amp;$F$1&amp;C24&amp;$G$1&amp;SUBSTITUTE(TEXT(A24,IF(EXACT(D24,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D24&amp;$H$1&amp;E24&amp;$G$1&amp;F24&amp;$C$1&amp;G24&amp;$H$1&amp;H24&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0xFA000000, 0, "0.07", "mm", 20, "", "", 0 },</v>
       </c>
       <c r="J24" s="2"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>11</v>
       </c>
       <c r="B25" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D25,"tpi"),25.4/A25,A25))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x00000000</v>
       </c>
       <c r="C25" s="24">
@@ -1548,18 +1545,18 @@
         <v>0</v>
       </c>
       <c r="I25" s="23" t="str">
-        <f>$D$1&amp;B25&amp;$F$1&amp;C25&amp;$G$1&amp;SUBSTITUTE(TEXT(A25,IF(EXACT(D25,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D25&amp;$H$1&amp;E25&amp;$G$1&amp;F25&amp;$C$1&amp;G25&amp;$H$1&amp;H25&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x00000000, 0, "..", "up", 20, "", "", 0 },</v>
       </c>
       <c r="J25" s="2"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D26,"tpi"),25.4/A26,A26))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x00000000</v>
       </c>
       <c r="C26" s="24">
@@ -1577,18 +1574,18 @@
         <v>0</v>
       </c>
       <c r="I26" s="23" t="str">
-        <f>$D$1&amp;B26&amp;$F$1&amp;C26&amp;$G$1&amp;SUBSTITUTE(TEXT(A26,IF(EXACT(D26,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D26&amp;$H$1&amp;E26&amp;$G$1&amp;F26&amp;$C$1&amp;G26&amp;$H$1&amp;H26&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x00000000, 10, "T", "mm", 0, "", "", 0 },</v>
       </c>
       <c r="J26" s="2"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="24">
         <v>1.25</v>
       </c>
       <c r="B27" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D27,"tpi"),25.4/A27,A27))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x0E666666</v>
       </c>
       <c r="C27" s="24">
@@ -1610,18 +1607,18 @@
         <v>0</v>
       </c>
       <c r="I27" s="23" t="str">
-        <f>$D$1&amp;B27&amp;$F$1&amp;C27&amp;$G$1&amp;SUBSTITUTE(TEXT(A27,IF(EXACT(D27,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D27&amp;$H$1&amp;E27&amp;$G$1&amp;F27&amp;$C$1&amp;G27&amp;$H$1&amp;H27&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x0E666666, 0, "1.25", "mm", 10, ".79", ".031", 0 },</v>
       </c>
       <c r="J27" s="2"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="24">
         <v>1.75</v>
       </c>
       <c r="B28" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D28,"tpi"),25.4/A28,A28))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x0A492492</v>
       </c>
       <c r="C28" s="24">
@@ -1643,18 +1640,18 @@
         <v>0</v>
       </c>
       <c r="I28" s="23" t="str">
-        <f>$D$1&amp;B28&amp;$F$1&amp;C28&amp;$G$1&amp;SUBSTITUTE(TEXT(A28,IF(EXACT(D28,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D28&amp;$H$1&amp;E28&amp;$G$1&amp;F28&amp;$C$1&amp;G28&amp;$H$1&amp;H28&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x0A492492, 0, "1.75", "mm", 10, "1.11", ".044", 0 },</v>
       </c>
       <c r="J28" s="2"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="24">
         <v>2</v>
       </c>
       <c r="B29" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D29,"tpi"),25.4/A29,A29))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x09000000</v>
       </c>
       <c r="C29" s="24">
@@ -1676,18 +1673,18 @@
         <v>0</v>
       </c>
       <c r="I29" s="23" t="str">
-        <f>$D$1&amp;B29&amp;$F$1&amp;C29&amp;$G$1&amp;SUBSTITUTE(TEXT(A29,IF(EXACT(D29,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D29&amp;$H$1&amp;E29&amp;$G$1&amp;F29&amp;$C$1&amp;G29&amp;$H$1&amp;H29&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x09000000, 0, "2.00", "mm", 10, "1.26", ".050", 0 },</v>
       </c>
       <c r="J29" s="2"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="24">
         <v>0.5</v>
       </c>
       <c r="B30" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D30,"tpi"),25.4/A30,A30))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x24000000</v>
       </c>
       <c r="C30" s="24">
@@ -1709,18 +1706,18 @@
         <v>0</v>
       </c>
       <c r="I30" s="23" t="str">
-        <f>$D$1&amp;B30&amp;$F$1&amp;C30&amp;$G$1&amp;SUBSTITUTE(TEXT(A30,IF(EXACT(D30,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D30&amp;$H$1&amp;E30&amp;$G$1&amp;F30&amp;$C$1&amp;G30&amp;$H$1&amp;H30&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x24000000, 0, "0.50", "mm", 10, ".34", ".013", 0 },</v>
       </c>
       <c r="J30" s="2"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="24">
         <v>0.75</v>
       </c>
       <c r="B31" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D31,"tpi"),25.4/A31,A31))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="0"/>
         <v>0x18000000</v>
       </c>
       <c r="C31" s="24">
@@ -1742,13 +1739,13 @@
         <v>0</v>
       </c>
       <c r="I31" s="23" t="str">
-        <f>$D$1&amp;B31&amp;$F$1&amp;C31&amp;$G$1&amp;SUBSTITUTE(TEXT(A31,IF(EXACT(D31,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D31&amp;$H$1&amp;E31&amp;$G$1&amp;F31&amp;$C$1&amp;G31&amp;$H$1&amp;H31&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x18000000, 0, "0.75", "mm", 10, ".50", ".020", 0 },</v>
       </c>
       <c r="J31" s="2"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>11</v>
       </c>
@@ -1771,13 +1768,13 @@
         <v>0</v>
       </c>
       <c r="I32" s="23" t="str">
-        <f>$D$1&amp;B32&amp;$F$1&amp;C32&amp;$G$1&amp;SUBSTITUTE(TEXT(A32,IF(EXACT(D32,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D32&amp;$H$1&amp;E32&amp;$G$1&amp;F32&amp;$C$1&amp;G32&amp;$H$1&amp;H32&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x00000000, 0, "..", "up", 10, "", "", 0 },</v>
       </c>
       <c r="J32" s="2"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>24</v>
       </c>
@@ -1800,18 +1797,18 @@
         <v>0</v>
       </c>
       <c r="I33" s="23" t="str">
-        <f>$D$1&amp;B33&amp;$F$1&amp;C33&amp;$G$1&amp;SUBSTITUTE(TEXT(A33,IF(EXACT(D33,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D33&amp;$H$1&amp;E33&amp;$G$1&amp;F33&amp;$C$1&amp;G33&amp;$H$1&amp;H33&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x00000000, 30, "T", "tpi", 0, "", "", 0 },</v>
       </c>
       <c r="J33" s="2"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="24">
         <v>27</v>
       </c>
       <c r="B34" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D34,"tpi"),25.4/A34,A34))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" ref="B34:B44" si="2">IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D34,"tpi"),25.4/A34,A34))*$B$1,0),8)),"0x00000000")</f>
         <v>0x13224489</v>
       </c>
       <c r="C34" s="24">
@@ -1829,18 +1826,18 @@
         <v>0</v>
       </c>
       <c r="I34" s="23" t="str">
-        <f>$D$1&amp;B34&amp;$F$1&amp;C34&amp;$G$1&amp;SUBSTITUTE(TEXT(A34,IF(EXACT(D34,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D34&amp;$H$1&amp;E34&amp;$G$1&amp;F34&amp;$C$1&amp;G34&amp;$H$1&amp;H34&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x13224489, 0, "27", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J34" s="2"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="24">
         <v>26</v>
       </c>
       <c r="B35" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D35,"tpi"),25.4/A35,A35))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x126CD9B3</v>
       </c>
       <c r="C35" s="24">
@@ -1858,18 +1855,18 @@
         <v>0</v>
       </c>
       <c r="I35" s="23" t="str">
-        <f>$D$1&amp;B35&amp;$F$1&amp;C35&amp;$G$1&amp;SUBSTITUTE(TEXT(A35,IF(EXACT(D35,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D35&amp;$H$1&amp;E35&amp;$G$1&amp;F35&amp;$C$1&amp;G35&amp;$H$1&amp;H35&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x126CD9B3, 0, "26", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J35" s="2"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="24">
         <v>24</v>
       </c>
       <c r="B36" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D36,"tpi"),25.4/A36,A36))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x11020408</v>
       </c>
       <c r="C36" s="24">
@@ -1887,18 +1884,18 @@
         <v>0</v>
       </c>
       <c r="I36" s="23" t="str">
-        <f>$D$1&amp;B36&amp;$F$1&amp;C36&amp;$G$1&amp;SUBSTITUTE(TEXT(A36,IF(EXACT(D36,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D36&amp;$H$1&amp;E36&amp;$G$1&amp;F36&amp;$C$1&amp;G36&amp;$H$1&amp;H36&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x11020408, 0, "24", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J36" s="2"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="24">
         <v>22</v>
       </c>
       <c r="B37" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D37,"tpi"),25.4/A37,A37))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x0F972E5C</v>
       </c>
       <c r="C37" s="24">
@@ -1916,18 +1913,18 @@
         <v>0</v>
       </c>
       <c r="I37" s="23" t="str">
-        <f>$D$1&amp;B37&amp;$F$1&amp;C37&amp;$G$1&amp;SUBSTITUTE(TEXT(A37,IF(EXACT(D37,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D37&amp;$H$1&amp;E37&amp;$G$1&amp;F37&amp;$C$1&amp;G37&amp;$H$1&amp;H37&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x0F972E5C, 0, "22", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J37" s="2"/>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="24">
         <v>20</v>
       </c>
       <c r="B38" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D38,"tpi"),25.4/A38,A38))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x0E2C58B1</v>
       </c>
       <c r="C38" s="24">
@@ -1945,18 +1942,18 @@
         <v>0</v>
       </c>
       <c r="I38" s="23" t="str">
-        <f>$D$1&amp;B38&amp;$F$1&amp;C38&amp;$G$1&amp;SUBSTITUTE(TEXT(A38,IF(EXACT(D38,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D38&amp;$H$1&amp;E38&amp;$G$1&amp;F38&amp;$C$1&amp;G38&amp;$H$1&amp;H38&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x0E2C58B1, 0, "20", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J38" s="2"/>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="24">
         <v>19</v>
       </c>
       <c r="B39" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D39,"tpi"),25.4/A39,A39))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x0D76EDDB</v>
       </c>
       <c r="C39" s="24">
@@ -1974,18 +1971,18 @@
         <v>0</v>
       </c>
       <c r="I39" s="23" t="str">
-        <f>$D$1&amp;B39&amp;$F$1&amp;C39&amp;$G$1&amp;SUBSTITUTE(TEXT(A39,IF(EXACT(D39,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D39&amp;$H$1&amp;E39&amp;$G$1&amp;F39&amp;$C$1&amp;G39&amp;$H$1&amp;H39&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x0D76EDDB, 0, "19", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J39" s="2"/>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="24">
         <v>18</v>
       </c>
       <c r="B40" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D40,"tpi"),25.4/A40,A40))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x0CC18306</v>
       </c>
       <c r="C40" s="24">
@@ -2003,18 +2000,18 @@
         <v>0</v>
       </c>
       <c r="I40" s="23" t="str">
-        <f>$D$1&amp;B40&amp;$F$1&amp;C40&amp;$G$1&amp;SUBSTITUTE(TEXT(A40,IF(EXACT(D40,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D40&amp;$H$1&amp;E40&amp;$G$1&amp;F40&amp;$C$1&amp;G40&amp;$H$1&amp;H40&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x0CC18306, 0, "18", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J40" s="2"/>
       <c r="Q40" s="5"/>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="24">
         <v>16</v>
       </c>
       <c r="B41" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D41,"tpi"),25.4/A41,A41))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x0B56AD5A</v>
       </c>
       <c r="C41" s="24">
@@ -2032,18 +2029,18 @@
         <v>0</v>
       </c>
       <c r="I41" s="23" t="str">
-        <f>$D$1&amp;B41&amp;$F$1&amp;C41&amp;$G$1&amp;SUBSTITUTE(TEXT(A41,IF(EXACT(D41,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D41&amp;$H$1&amp;E41&amp;$G$1&amp;F41&amp;$C$1&amp;G41&amp;$H$1&amp;H41&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x0B56AD5A, 0, "16", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J41" s="2"/>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A42" s="24">
         <v>14</v>
       </c>
       <c r="B42" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D42,"tpi"),25.4/A42,A42))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x09EBD7AF</v>
       </c>
       <c r="C42" s="24">
@@ -2061,18 +2058,18 @@
         <v>0</v>
       </c>
       <c r="I42" s="23" t="str">
-        <f>$D$1&amp;B42&amp;$F$1&amp;C42&amp;$G$1&amp;SUBSTITUTE(TEXT(A42,IF(EXACT(D42,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D42&amp;$H$1&amp;E42&amp;$G$1&amp;F42&amp;$C$1&amp;G42&amp;$H$1&amp;H42&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x09EBD7AF, 0, "14", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J42" s="2"/>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A43" s="24">
         <v>12</v>
       </c>
       <c r="B43" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D43,"tpi"),25.4/A43,A43))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x08810204</v>
       </c>
       <c r="C43" s="24">
@@ -2090,18 +2087,18 @@
         <v>0</v>
       </c>
       <c r="I43" s="23" t="str">
-        <f>$D$1&amp;B43&amp;$F$1&amp;C43&amp;$G$1&amp;SUBSTITUTE(TEXT(A43,IF(EXACT(D43,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D43&amp;$H$1&amp;E43&amp;$G$1&amp;F43&amp;$C$1&amp;G43&amp;$H$1&amp;H43&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x08810204, 0, "12", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J43" s="2"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A44" s="24">
         <v>10</v>
       </c>
       <c r="B44" s="24" t="str">
-        <f>IFERROR(CONCATENATE("0x",DEC2HEX(ROUNDDOWN($A$4*$B$4/($A$7/$B$7*IF(EXACT(D44,"tpi"),25.4/A44,A44))*$B$1,0),8)),"0x00000000")</f>
+        <f t="shared" si="2"/>
         <v>0x07162C58</v>
       </c>
       <c r="C44" s="24">
@@ -2119,13 +2116,13 @@
         <v>0</v>
       </c>
       <c r="I44" s="23" t="str">
-        <f>$D$1&amp;B44&amp;$F$1&amp;C44&amp;$G$1&amp;SUBSTITUTE(TEXT(A44,IF(EXACT(D44,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D44&amp;$H$1&amp;E44&amp;$G$1&amp;F44&amp;$C$1&amp;G44&amp;$H$1&amp;H44&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x07162C58, 0, "10", "tpi", 30, "", "", 0 },</v>
       </c>
       <c r="J44" s="2"/>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>11</v>
       </c>
@@ -2148,13 +2145,13 @@
         <v>0</v>
       </c>
       <c r="I45" s="23" t="str">
-        <f>$D$1&amp;B45&amp;$F$1&amp;C45&amp;$G$1&amp;SUBSTITUTE(TEXT(A45,IF(EXACT(D45,"tpi"),"0","0,00")),",",".")&amp;$C$1&amp;D45&amp;$H$1&amp;E45&amp;$G$1&amp;F45&amp;$C$1&amp;G45&amp;$H$1&amp;H45&amp;$E$1</f>
+        <f t="shared" si="1"/>
         <v>{ 0x00000000, 0, "..", "up", 30, "", "", 0 },</v>
       </c>
       <c r="J45" s="2"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" s="4" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="C46" s="2"/>
       <c r="E46" s="2"/>
@@ -2164,7 +2161,7 @@
       <c r="J46" s="2"/>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="4"/>
       <c r="C47" s="2"/>
@@ -2228,123 +2225,123 @@
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="E64"/>
     </row>
-    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="E68"/>
     </row>
-    <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="E69"/>
     </row>
-    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="E70"/>
     </row>
-    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="E71"/>
     </row>
-    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="E72"/>
     </row>
-    <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="E73"/>
     </row>
-    <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="E74"/>
     </row>
-    <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="E75"/>
     </row>
-    <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="E76"/>
     </row>
-    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="E77"/>
     </row>
-    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="E78"/>
     </row>
-    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="E79"/>
     </row>
-    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="E80"/>
     </row>
-    <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="E81"/>
     </row>
-    <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="E82"/>
     </row>
-    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="E84"/>
     </row>
-    <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="E86"/>
     </row>
-    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="E88"/>
     </row>
-    <row r="89" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="E89"/>
     </row>
-    <row r="90" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="E90"/>
     </row>
-    <row r="91" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="E91"/>
     </row>
-    <row r="92" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="E92"/>
     </row>
@@ -2590,34 +2587,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.90625" customWidth="1"/>
-    <col min="7" max="7" width="12.6328125" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="4">
         <f>0.65*B3</f>
-        <v>0.65</v>
+        <v>0.97500000000000009</v>
       </c>
       <c r="C1" s="4">
         <f>B1/25.4</f>
-        <v>2.5590551181102365E-2</v>
+        <v>3.8385826771653551E-2</v>
       </c>
       <c r="F1" s="15"/>
       <c r="G1" s="16"/>
@@ -2634,7 +2631,7 @@
         <v>94</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2644,12 +2641,12 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B3" s="4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -2666,7 +2663,7 @@
       <c r="B4" s="4">
         <v>60</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="33">
         <f>TAN(RADIANS(B4/2))</f>
         <v>0.57735026918962573</v>
       </c>
@@ -2683,7 +2680,7 @@
       <c r="B5" s="4">
         <v>5</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="33">
         <f>TAN(RADIANS(B4/2-B5))</f>
         <v>0.46630765815499858</v>
       </c>
@@ -2694,13 +2691,13 @@
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
     </row>
-    <row r="6" spans="1:13" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B6" s="15">
         <f>(B1-C10)*C4</f>
-        <v>0.30676165900294189</v>
+        <v>0.42503069012850836</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2726,7 +2723,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" ht="25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>91</v>
       </c>
@@ -2751,7 +2748,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -2760,11 +2757,11 @@
       </c>
       <c r="C10" s="15">
         <f t="shared" ref="C10:C17" si="0">$B$1*SQRT(B10)/SQRT($B$2-1)</f>
-        <v>0.11867322079278599</v>
+        <v>0.23882524992135984</v>
       </c>
       <c r="D10" s="16">
         <f>C10/25.4</f>
-        <v>4.6721740469600785E-3</v>
+        <v>9.4025688945417272E-3</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
@@ -2773,19 +2770,26 @@
         <f t="shared" ref="F10:F17" si="1">$B$7/$B$3*E10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="17"/>
+      <c r="G10" s="15">
+        <f>C10</f>
+        <v>0.23882524992135984</v>
+      </c>
       <c r="H10" s="19">
         <f>C10/SIN(RADIANS(60))</f>
-        <v>0.13703203194062977</v>
+        <v>0.2757716446627535</v>
       </c>
       <c r="I10" s="19">
         <f>H10*C10/2</f>
-        <v>8.1310162910872286E-3</v>
+        <v>3.2930615978903274E-2</v>
+      </c>
+      <c r="J10">
+        <f>C10*C10/(SQRT(3))</f>
+        <v>3.2930615978903274E-2</v>
       </c>
       <c r="L10" s="12"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -2794,33 +2798,40 @@
       </c>
       <c r="C11" s="15">
         <f t="shared" si="0"/>
-        <v>0.21666666666666667</v>
+        <v>0.43603325561245904</v>
       </c>
       <c r="D11" s="16">
         <f>C11/25.4</f>
-        <v>8.5301837270341224E-3</v>
+        <v>1.7166663606789728E-2</v>
       </c>
       <c r="E11" s="16">
         <f t="shared" ref="E11:E17" si="2">$B$6-($B$1-C11)*$C$5</f>
-        <v>0.10469500713577584</v>
+        <v>0.17370636972973041</v>
       </c>
       <c r="F11" s="17">
-        <f t="shared" si="1"/>
-        <v>188.4510128443965</v>
-      </c>
-      <c r="G11" s="17"/>
+        <f>$B$7/$B$3*E11</f>
+        <v>208.44764367567649</v>
+      </c>
+      <c r="G11" s="15">
+        <f>C11-C10</f>
+        <v>0.1972080056910992</v>
+      </c>
       <c r="H11" s="19">
         <f>C11/SIN(RADIANS(60))</f>
-        <v>0.25018511664883786</v>
+        <v>0.50348783500696426</v>
       </c>
       <c r="I11" s="19">
         <f t="shared" ref="I11:I27" si="3">0.5*(H11*H11-H10*H10)*TAN(RADIANS(60))</f>
-        <v>3.7944742691740405E-2</v>
+        <v>0.15367620790154865</v>
+      </c>
+      <c r="J11" s="4">
+        <f>(C11*C11-C10*C10)/(SQRT(3))</f>
+        <v>7.6838103950774353E-2</v>
       </c>
       <c r="L11" s="12"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -2829,28 +2840,35 @@
       </c>
       <c r="C12" s="15">
         <f>$B$1*SQRT(B12)/SQRT($B$2-1)</f>
-        <v>0.30641293851417062</v>
+        <v>0.61664414373283405</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" ref="D12:D27" si="4">C12/25.4</f>
-        <v>1.2063501516305931E-2</v>
+        <v>2.4277328493418664E-2</v>
       </c>
       <c r="E12" s="16">
         <f t="shared" si="2"/>
-        <v>0.14654438098912728</v>
+        <v>0.25792661000643691</v>
       </c>
       <c r="F12" s="17">
         <f t="shared" si="1"/>
-        <v>263.77988578042908</v>
-      </c>
-      <c r="G12" s="17"/>
+        <v>309.51193200772428</v>
+      </c>
+      <c r="G12" s="15">
+        <f t="shared" ref="G12:G26" si="5">C12-C11</f>
+        <v>0.18061088812037501</v>
+      </c>
       <c r="H12" s="19">
-        <f t="shared" ref="H12:H27" si="5">C12/SIN(RADIANS(60))</f>
-        <v>0.35381518506868131</v>
+        <f t="shared" ref="H12:H27" si="6">C12/SIN(RADIANS(60))</f>
+        <v>0.71203932475671605</v>
       </c>
       <c r="I12" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914855E-2</v>
+        <v>0.21953743985935517</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" ref="J12:J27" si="7">(C12*C12-C11*C11)/(SQRT(3))</f>
+        <v>0.10976871992967763</v>
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="11"/>
@@ -2864,28 +2882,35 @@
       </c>
       <c r="C13" s="15">
         <f t="shared" si="0"/>
-        <v>0.3752776749732567</v>
+        <v>0.75523175251044627</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="4"/>
-        <v>1.4774711613120344E-2</v>
+        <v>2.97335335634034E-2</v>
       </c>
       <c r="E13" s="16">
         <f t="shared" si="2"/>
-        <v>0.17865653497682485</v>
+        <v>0.32255107330482635</v>
       </c>
       <c r="F13" s="17">
         <f t="shared" si="1"/>
-        <v>321.58176295828474</v>
-      </c>
-      <c r="G13" s="17"/>
+        <v>387.06128796579162</v>
+      </c>
+      <c r="G13" s="15">
+        <f t="shared" si="5"/>
+        <v>0.13858760877761223</v>
+      </c>
       <c r="H13" s="19">
-        <f t="shared" si="5"/>
-        <v>0.43333333333333329</v>
+        <f t="shared" si="6"/>
+        <v>0.87206651122491796</v>
       </c>
       <c r="I13" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914792E-2</v>
+        <v>0.21953743985935498</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967753</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2897,28 +2922,35 @@
       </c>
       <c r="C14" s="15">
         <f t="shared" si="0"/>
-        <v>0.43333333333333335</v>
+        <v>0.87206651122491807</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="4"/>
-        <v>1.7060367454068245E-2</v>
+        <v>3.4333327213579456E-2</v>
       </c>
       <c r="E14" s="16">
         <f t="shared" si="2"/>
-        <v>0.20572833306935887</v>
+        <v>0.37703201603207603</v>
       </c>
       <c r="F14" s="17">
         <f t="shared" si="1"/>
-        <v>370.31099952484595</v>
-      </c>
-      <c r="G14" s="17"/>
+        <v>452.43841923849124</v>
+      </c>
+      <c r="G14" s="15">
+        <f t="shared" si="5"/>
+        <v>0.1168347587144718</v>
+      </c>
       <c r="H14" s="19">
-        <f t="shared" si="5"/>
-        <v>0.50037023329767572</v>
+        <f t="shared" si="6"/>
+        <v>1.0069756700139285</v>
       </c>
       <c r="I14" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914917E-2</v>
+        <v>0.21953743985935537</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967772</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2930,28 +2962,35 @@
       </c>
       <c r="C15" s="15">
         <f t="shared" si="0"/>
-        <v>0.48448139512495447</v>
+        <v>0.97500000000000009</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="4"/>
-        <v>1.9074070674210807E-2</v>
+        <v>3.8385826771653551E-2</v>
       </c>
       <c r="E15" s="16">
         <f t="shared" si="2"/>
-        <v>0.22957906598257688</v>
+        <v>0.42503069012850836</v>
       </c>
       <c r="F15" s="17">
         <f t="shared" si="1"/>
-        <v>413.24231876863837</v>
-      </c>
-      <c r="G15" s="17"/>
+        <v>510.03682815421001</v>
+      </c>
+      <c r="G15" s="15">
+        <f t="shared" si="5"/>
+        <v>0.10293348877508202</v>
+      </c>
       <c r="H15" s="19">
-        <f t="shared" si="5"/>
-        <v>0.55943092778551584</v>
+        <f t="shared" si="6"/>
+        <v>1.1258330249197703</v>
       </c>
       <c r="I15" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914889E-2</v>
+        <v>0.21953743985935517</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="7"/>
+        <v>0.1097687199296776</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2963,31 +3002,38 @@
       </c>
       <c r="C16" s="15">
         <f t="shared" si="0"/>
-        <v>0.53072277760302189</v>
+        <v>1.0680589871350739</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" si="4"/>
-        <v>2.0894597543426058E-2</v>
+        <v>4.2049566422640704E-2</v>
       </c>
       <c r="E16" s="16">
         <f t="shared" si="2"/>
-        <v>0.25114177675577409</v>
+        <v>0.46842480848974077</v>
       </c>
       <c r="F16" s="17">
         <f t="shared" si="1"/>
-        <v>452.05519816039339</v>
-      </c>
-      <c r="G16" s="4"/>
+        <v>562.10977018768892</v>
+      </c>
+      <c r="G16" s="15">
+        <f t="shared" si="5"/>
+        <v>9.3058987135073767E-2</v>
+      </c>
       <c r="H16" s="19">
-        <f t="shared" si="5"/>
-        <v>0.61282587702834124</v>
+        <f t="shared" si="6"/>
+        <v>1.2332882874656679</v>
       </c>
       <c r="I16" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914841E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935478</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967747</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>8</v>
       </c>
@@ -2996,30 +3042,38 @@
       </c>
       <c r="C17" s="15">
         <f t="shared" si="0"/>
-        <v>0.573246117397328</v>
+        <v>1.1536355577044253</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="4"/>
-        <v>2.2568744779422365E-2</v>
+        <v>4.5418722744268711E-2</v>
       </c>
       <c r="E17" s="16">
         <f t="shared" si="2"/>
-        <v>0.27097073575218622</v>
+        <v>0.50832981870487104</v>
       </c>
       <c r="F17" s="17">
         <f t="shared" si="1"/>
-        <v>487.7473243539352</v>
+        <v>609.99578244584529</v>
+      </c>
+      <c r="G17" s="15">
+        <f t="shared" si="5"/>
+        <v>8.5576570569351418E-2</v>
       </c>
       <c r="H17" s="19">
-        <f t="shared" si="5"/>
-        <v>0.66192760038251031</v>
+        <f t="shared" si="6"/>
+        <v>1.3321035995747481</v>
       </c>
       <c r="I17" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914841E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935595</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967779</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>9</v>
       </c>
@@ -3027,31 +3081,39 @@
         <v>8</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" ref="C18:C27" si="6">$B$1*SQRT(B18)/SQRT($B$2-1)</f>
-        <v>0.61282587702834124</v>
+        <f t="shared" ref="C18:C27" si="8">$B$1*SQRT(B18)/SQRT($B$2-1)</f>
+        <v>1.2332882874656681</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="4"/>
-        <v>2.4127003032611862E-2</v>
+        <v>4.8554656986837329E-2</v>
       </c>
       <c r="E18" s="16">
-        <f t="shared" ref="E18:E20" si="7">$B$6-($B$1-C18)*$C$5</f>
-        <v>0.28942708077606172</v>
+        <f t="shared" ref="E18:E20" si="9">$B$6-($B$1-C18)*$C$5</f>
+        <v>0.54547249658548913</v>
       </c>
       <c r="F18" s="17">
-        <f t="shared" ref="F18:F27" si="8">$B$7/$B$3*E18</f>
-        <v>520.96874539691112</v>
+        <f t="shared" ref="F18:F27" si="10">$B$7/$B$3*E18</f>
+        <v>654.566995902587</v>
+      </c>
+      <c r="G18" s="15">
+        <f t="shared" si="5"/>
+        <v>7.9652729761242824E-2</v>
       </c>
       <c r="H18" s="19">
-        <f t="shared" si="5"/>
-        <v>0.70763037013736263</v>
+        <f t="shared" si="6"/>
+        <v>1.4240786495134321</v>
       </c>
       <c r="I18" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914841E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935478</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967767</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>10</v>
       </c>
@@ -3059,31 +3121,39 @@
         <v>9</v>
       </c>
       <c r="C19" s="15">
-        <f t="shared" si="6"/>
-        <v>0.65</v>
+        <f t="shared" si="8"/>
+        <v>1.3080997668373771</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="4"/>
-        <v>2.5590551181102365E-2</v>
+        <v>5.1499990820369178E-2</v>
       </c>
       <c r="E19" s="16">
-        <f t="shared" si="7"/>
-        <v>0.30676165900294189</v>
+        <f t="shared" si="9"/>
+        <v>0.58035766233442165</v>
       </c>
       <c r="F19" s="17">
-        <f t="shared" si="8"/>
-        <v>552.17098620529543</v>
+        <f t="shared" si="10"/>
+        <v>696.42919480130604</v>
+      </c>
+      <c r="G19" s="15">
+        <f t="shared" si="5"/>
+        <v>7.4811479371708955E-2</v>
       </c>
       <c r="H19" s="19">
-        <f t="shared" si="5"/>
-        <v>0.75055534994651352</v>
+        <f t="shared" si="6"/>
+        <v>1.5104635050208928</v>
       </c>
       <c r="I19" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914792E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935537</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967753</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>11</v>
       </c>
@@ -3091,31 +3161,39 @@
         <v>10</v>
       </c>
       <c r="C20" s="15">
-        <f t="shared" si="6"/>
-        <v>0.68516015970314903</v>
+        <f t="shared" si="8"/>
+        <v>1.3788582233137678</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="4"/>
-        <v>2.6974809437131854E-2</v>
+        <v>5.4285756823376691E-2</v>
       </c>
       <c r="E20" s="16">
-        <f t="shared" si="7"/>
-        <v>0.32315711073447306</v>
+        <f t="shared" si="9"/>
+        <v>0.61335287246858983</v>
       </c>
       <c r="F20" s="17">
-        <f t="shared" si="8"/>
-        <v>581.68279932205155</v>
+        <f t="shared" si="10"/>
+        <v>736.02344696230784</v>
+      </c>
+      <c r="G20" s="15">
+        <f t="shared" si="5"/>
+        <v>7.0758456476390785E-2</v>
       </c>
       <c r="H20" s="19">
-        <f t="shared" si="5"/>
-        <v>0.79115480528524018</v>
+        <f t="shared" si="6"/>
+        <v>1.5921683328090661</v>
       </c>
       <c r="I20" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273915181E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935537</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967779</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>12</v>
       </c>
@@ -3123,31 +3201,39 @@
         <v>11</v>
       </c>
       <c r="C21" s="15">
-        <f t="shared" si="6"/>
-        <v>0.71860203791033672</v>
+        <f t="shared" si="8"/>
+        <v>1.4461587049836544</v>
       </c>
       <c r="D21" s="16">
         <f t="shared" si="4"/>
-        <v>2.8291418815367588E-2</v>
+        <v>5.6935382085970647E-2</v>
       </c>
       <c r="E21" s="16">
-        <f t="shared" ref="E21:E23" si="9">$B$6-($B$1-C21)*$C$5</f>
-        <v>0.3387513146455714</v>
+        <f t="shared" ref="E21:E23" si="11">$B$6-($B$1-C21)*$C$5</f>
+        <v>0.64473560246877804</v>
       </c>
       <c r="F21" s="17">
-        <f t="shared" si="8"/>
-        <v>609.75236636202851</v>
+        <f t="shared" si="10"/>
+        <v>773.6827229625336</v>
+      </c>
+      <c r="G21" s="15">
+        <f t="shared" si="5"/>
+        <v>6.7300481669886558E-2</v>
       </c>
       <c r="H21" s="19">
-        <f t="shared" si="5"/>
-        <v>0.8297701600554932</v>
+        <f t="shared" si="6"/>
+        <v>1.669880235226467</v>
       </c>
       <c r="I21" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914702E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935498</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967741</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>13</v>
       </c>
@@ -3155,31 +3241,39 @@
         <v>12</v>
       </c>
       <c r="C22" s="15">
-        <f t="shared" si="6"/>
-        <v>0.75055534994651341</v>
+        <f t="shared" si="8"/>
+        <v>1.5104635050208925</v>
       </c>
       <c r="D22" s="16">
         <f t="shared" si="4"/>
-        <v>2.9549423226240688E-2</v>
+        <v>5.94670671268068E-2</v>
       </c>
       <c r="E22" s="16">
-        <f t="shared" si="9"/>
-        <v>0.35365138875145691</v>
+        <f t="shared" si="11"/>
+        <v>0.67472142318226802</v>
       </c>
       <c r="F22" s="17">
-        <f t="shared" si="8"/>
-        <v>636.57249975262243</v>
+        <f t="shared" si="10"/>
+        <v>809.66570781872167</v>
+      </c>
+      <c r="G22" s="15">
+        <f t="shared" si="5"/>
+        <v>6.4304800037238152E-2</v>
       </c>
       <c r="H22" s="19">
-        <f t="shared" si="5"/>
-        <v>0.86666666666666659</v>
+        <f t="shared" si="6"/>
+        <v>1.7441330224498359</v>
       </c>
       <c r="I22" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914508E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935423</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967741</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>14</v>
       </c>
@@ -3187,31 +3281,39 @@
         <v>13</v>
       </c>
       <c r="C23" s="15">
-        <f t="shared" si="6"/>
-        <v>0.78120277635053104</v>
+        <f t="shared" si="8"/>
+        <v>1.5721402609182171</v>
       </c>
       <c r="D23" s="16">
         <f t="shared" si="4"/>
-        <v>3.0756014816950044E-2</v>
+        <v>6.1895285862921937E-2</v>
       </c>
       <c r="E23" s="16">
-        <f t="shared" si="9"/>
-        <v>0.36794251838639203</v>
+        <f t="shared" si="11"/>
+        <v>0.70348176678734697</v>
       </c>
       <c r="F23" s="17">
-        <f t="shared" si="8"/>
-        <v>662.29653309550565</v>
+        <f t="shared" si="10"/>
+        <v>844.17812014481638</v>
+      </c>
+      <c r="G23" s="15">
+        <f t="shared" si="5"/>
+        <v>6.1676755897324576E-2</v>
       </c>
       <c r="H23" s="19">
-        <f t="shared" si="5"/>
-        <v>0.9020552664353243</v>
+        <f t="shared" si="6"/>
+        <v>1.8153512056899623</v>
       </c>
       <c r="I23" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273915181E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935537</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>15</v>
       </c>
@@ -3219,31 +3321,39 @@
         <v>14</v>
       </c>
       <c r="C24" s="15">
-        <f t="shared" si="6"/>
-        <v>0.81069243380102074</v>
+        <f t="shared" si="8"/>
+        <v>1.6314870517414475</v>
       </c>
       <c r="D24" s="16">
         <f t="shared" si="4"/>
-        <v>3.1917024952796094E-2</v>
+        <v>6.4231773690608174E-2</v>
       </c>
       <c r="E24" s="16">
-        <f t="shared" ref="E24:E27" si="10">$B$6-($B$1-C24)*$C$5</f>
-        <v>0.38169377149192302</v>
+        <f t="shared" ref="E24:E27" si="12">$B$6-($B$1-C24)*$C$5</f>
+        <v>0.73115562983514204</v>
       </c>
       <c r="F24" s="17">
-        <f t="shared" si="8"/>
-        <v>687.04878868546143</v>
+        <f t="shared" si="10"/>
+        <v>877.38675580217046</v>
+      </c>
+      <c r="G24" s="15">
+        <f t="shared" si="5"/>
+        <v>5.9346790823230355E-2</v>
       </c>
       <c r="H24" s="19">
-        <f t="shared" si="5"/>
-        <v>0.93610698977002438</v>
+        <f t="shared" si="6"/>
+        <v>1.8838789770046274</v>
       </c>
       <c r="I24" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914889E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935614</v>
+      </c>
+      <c r="J24" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967792</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>16</v>
       </c>
@@ -3251,31 +3361,39 @@
         <v>15</v>
       </c>
       <c r="C25" s="15">
-        <f t="shared" si="6"/>
-        <v>0.83914639167827376</v>
+        <f t="shared" si="8"/>
+        <v>1.6887495373796555</v>
       </c>
       <c r="D25" s="16">
         <f t="shared" si="4"/>
-        <v>3.303725951489267E-2</v>
+        <v>6.648620225904156E-2</v>
       </c>
       <c r="E25" s="16">
+        <f t="shared" si="12"/>
+        <v>0.75785756541322913</v>
+      </c>
+      <c r="F25" s="17">
         <f t="shared" si="10"/>
-        <v>0.39496206995490585</v>
-      </c>
-      <c r="F25" s="17">
-        <f t="shared" si="8"/>
-        <v>710.93172591883058</v>
+        <v>909.42907849587493</v>
+      </c>
+      <c r="G25" s="15">
+        <f t="shared" si="5"/>
+        <v>5.7262485638208016E-2</v>
       </c>
       <c r="H25" s="19">
-        <f t="shared" si="5"/>
-        <v>0.96896279024990906</v>
+        <f t="shared" si="6"/>
+        <v>1.9500000000000002</v>
       </c>
       <c r="I25" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914889E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935459</v>
+      </c>
+      <c r="J25" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967767</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>17</v>
       </c>
@@ -3283,31 +3401,39 @@
         <v>16</v>
       </c>
       <c r="C26" s="15">
-        <f t="shared" si="6"/>
-        <v>0.8666666666666667</v>
+        <f t="shared" si="8"/>
+        <v>1.7441330224498361</v>
       </c>
       <c r="D26" s="16">
         <f t="shared" si="4"/>
-        <v>3.4120734908136489E-2</v>
+        <v>6.8666654427158913E-2</v>
       </c>
       <c r="E26" s="16">
+        <f t="shared" si="12"/>
+        <v>0.78368330863676738</v>
+      </c>
+      <c r="F26" s="17">
         <f t="shared" si="10"/>
-        <v>0.40779498493652488</v>
-      </c>
-      <c r="F26" s="17">
-        <f t="shared" si="8"/>
-        <v>734.03097288574475</v>
+        <v>940.4199703641209</v>
+      </c>
+      <c r="G26" s="15">
+        <f t="shared" si="5"/>
+        <v>5.5383485070180649E-2</v>
       </c>
       <c r="H26" s="19">
-        <f t="shared" si="5"/>
-        <v>1.0007404665953514</v>
+        <f t="shared" si="6"/>
+        <v>2.013951340027857</v>
       </c>
       <c r="I26" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914702E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.21953743985935537</v>
+      </c>
+      <c r="J26" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967767</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>18</v>
       </c>
@@ -3315,28 +3441,32 @@
         <v>17</v>
       </c>
       <c r="C27" s="15">
-        <f t="shared" si="6"/>
-        <v>0.89333955221715977</v>
+        <f t="shared" si="8"/>
+        <v>1.7978111691721133</v>
       </c>
       <c r="D27" s="16">
         <f t="shared" si="4"/>
-        <v>3.5170848512486606E-2</v>
+        <v>7.0779967290240678E-2</v>
       </c>
       <c r="E27" s="16">
+        <f t="shared" si="12"/>
+        <v>0.80871383952893283</v>
+      </c>
+      <c r="F27" s="17">
         <f t="shared" si="10"/>
-        <v>0.42023275573381164</v>
-      </c>
-      <c r="F27" s="17">
-        <f t="shared" si="8"/>
-        <v>756.41896032086095</v>
+        <v>970.45660743471944</v>
       </c>
       <c r="H27" s="19">
-        <f t="shared" si="5"/>
-        <v>1.0315396619006338</v>
+        <f t="shared" si="6"/>
+        <v>2.075933524947271</v>
       </c>
       <c r="I27" s="19">
         <f t="shared" si="3"/>
-        <v>5.4206775273914605E-2</v>
+        <v>0.21953743985935575</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="7"/>
+        <v>0.10976871992967767</v>
       </c>
     </row>
   </sheetData>
@@ -3353,12 +3483,12 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>30</v>
       </c>
@@ -3366,7 +3496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>21.888000000000002</v>
       </c>
@@ -3374,7 +3504,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>17.024000000000001</v>
       </c>
@@ -3382,7 +3512,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>14.40492308</v>
       </c>
@@ -3390,7 +3520,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>12.710226240000001</v>
       </c>
@@ -3398,7 +3528,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>11.499728510000001</v>
       </c>
@@ -3406,7 +3536,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>10.57975023</v>
       </c>
@@ -3414,7 +3544,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>9.8501122799999994</v>
       </c>

</xml_diff>